<commit_message>
This is the first commit on 4/30/19
</commit_message>
<xml_diff>
--- a/TestDataAndResults/Run1/SophieAutomation.xlsx
+++ b/TestDataAndResults/Run1/SophieAutomation.xlsx
@@ -3,19 +3,20 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr documentId="13_ncr:1_{0BCA9586-7F92-4F67-89EE-7CD50C2B894D}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43"/>
+  <xr:revisionPtr documentId="13_ncr:1_{1C1D9540-4568-420E-91B6-3A27BB8435DB}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43"/>
   <bookViews>
-    <workbookView activeTab="2" firstSheet="2" windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
+    <workbookView activeTab="4" firstSheet="4" windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" r:id="rId1" sheetId="8"/>
     <sheet name="DriverSheet" r:id="rId2" sheetId="1"/>
     <sheet name="VerifyCSVForExistingVersion" r:id="rId3" sheetId="4"/>
     <sheet name="VerifyCSVForNewVersion" r:id="rId4" sheetId="10"/>
-    <sheet name="VerifyEventAPI" r:id="rId5" sheetId="6"/>
-    <sheet name="Cases_RealTimeSpine" r:id="rId6" sheetId="9"/>
-    <sheet name="BatchDecisionOutputValidations" r:id="rId7" sheetId="5"/>
-    <sheet name="CheckLists" r:id="rId8" sheetId="7"/>
+    <sheet name="VerifyDeleteOffer" r:id="rId5" sheetId="11"/>
+    <sheet name="VerifyEventAPI" r:id="rId6" sheetId="6"/>
+    <sheet name="Cases_RealTimeSpine" r:id="rId7" sheetId="9"/>
+    <sheet name="BatchDecisionOutputValidations" r:id="rId8" sheetId="5"/>
+    <sheet name="CheckLists" r:id="rId9" sheetId="7"/>
   </sheets>
   <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1211" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1405" uniqueCount="287">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -840,6 +841,54 @@
   </si>
   <si>
     <t>Switch To Parent</t>
+  </si>
+  <si>
+    <t>TS1_Regr_014</t>
+  </si>
+  <si>
+    <t>Delete_offer</t>
+  </si>
+  <si>
+    <t>Delete the offer</t>
+  </si>
+  <si>
+    <t>rbdeloffer</t>
+  </si>
+  <si>
+    <t>hiddenClick</t>
+  </si>
+  <si>
+    <t>ED_Offer_RenamedLabel_2</t>
+  </si>
+  <si>
+    <t>select radio button</t>
+  </si>
+  <si>
+    <t>radBtndeloffer</t>
+  </si>
+  <si>
+    <t>click on next button</t>
+  </si>
+  <si>
+    <t>btnNxt</t>
+  </si>
+  <si>
+    <t>TS_37</t>
+  </si>
+  <si>
+    <t>TS_39</t>
+  </si>
+  <si>
+    <t>VerifyDeleteOffer</t>
+  </si>
+  <si>
+    <t>TS1_Regr_14</t>
+  </si>
+  <si>
+    <t>Scenario to validate the deleted offer is not present in the CSV</t>
+  </si>
+  <si>
+    <t>Not Available</t>
   </si>
   <si>
     <t>Pass</t>
@@ -888,7 +937,7 @@
       <name val="Calibiri"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -910,6 +959,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1021,7 +1082,7 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="38">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
     <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
@@ -1083,6 +1144,11 @@
     <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="7" fillId="3" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
+    <xf applyFill="1" borderId="0" fillId="5" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="6" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="1" fillId="0" fontId="3" numFmtId="0" quotePrefix="1" xfId="1"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="0" fontId="2" numFmtId="0" quotePrefix="1" xfId="0"/>
+    <xf applyFill="1" applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
@@ -1449,10 +1515,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1554,18 +1620,33 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="E8" s="3"/>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B9" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C9" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D9" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="E8" s="3"/>
+      <c r="E9" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1580,7 +1661,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32EA4E71-0B53-4881-A15A-C454293CD34C}">
   <dimension ref="A1:I44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+    <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
@@ -1677,7 +1758,7 @@
       </c>
       <c r="G5" s="9"/>
       <c r="H5" s="3" t="s">
-        <v>269</v>
+        <v>285</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -1701,7 +1782,7 @@
       </c>
       <c r="G6" s="9"/>
       <c r="H6" s="3" t="s">
-        <v>269</v>
+        <v>285</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -1725,7 +1806,7 @@
       </c>
       <c r="G7" s="9"/>
       <c r="H7" s="3" t="s">
-        <v>269</v>
+        <v>285</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -1747,7 +1828,7 @@
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
       <c r="H8" s="3" t="s">
-        <v>269</v>
+        <v>285</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -1771,7 +1852,7 @@
       </c>
       <c r="G9" s="9"/>
       <c r="H9" s="3" t="s">
-        <v>269</v>
+        <v>285</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -1793,7 +1874,7 @@
       <c r="F10" s="9"/>
       <c r="G10" s="9"/>
       <c r="H10" s="3" t="s">
-        <v>269</v>
+        <v>285</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -1817,7 +1898,7 @@
       </c>
       <c r="G11" s="9"/>
       <c r="H11" s="3" t="s">
-        <v>269</v>
+        <v>285</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -1839,7 +1920,7 @@
       <c r="F12" s="9"/>
       <c r="G12" s="9"/>
       <c r="H12" s="3" t="s">
-        <v>269</v>
+        <v>285</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -1863,7 +1944,7 @@
       </c>
       <c r="G13" s="9"/>
       <c r="H13" s="3" t="s">
-        <v>269</v>
+        <v>285</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -1885,7 +1966,7 @@
       <c r="F14" s="9"/>
       <c r="G14" s="9"/>
       <c r="H14" s="3" t="s">
-        <v>269</v>
+        <v>285</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -1909,7 +1990,7 @@
       </c>
       <c r="G15" s="9"/>
       <c r="H15" s="3" t="s">
-        <v>269</v>
+        <v>285</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -1933,7 +2014,7 @@
       </c>
       <c r="G16" s="9"/>
       <c r="H16" s="3" t="s">
-        <v>269</v>
+        <v>285</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -1957,7 +2038,7 @@
       </c>
       <c r="G17" s="9"/>
       <c r="H17" s="3" t="s">
-        <v>269</v>
+        <v>286</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -1981,7 +2062,7 @@
       </c>
       <c r="G18" s="7"/>
       <c r="H18" s="3" t="s">
-        <v>269</v>
+        <v>285</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -2003,7 +2084,7 @@
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
       <c r="H19" s="3" t="s">
-        <v>269</v>
+        <v>285</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -2027,7 +2108,7 @@
       </c>
       <c r="G20" s="3"/>
       <c r="H20" s="3" t="s">
-        <v>269</v>
+        <v>286</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -2051,7 +2132,7 @@
       </c>
       <c r="G21" s="3"/>
       <c r="H21" s="3" t="s">
-        <v>269</v>
+        <v>286</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -2073,7 +2154,7 @@
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
       <c r="H22" s="3" t="s">
-        <v>269</v>
+        <v>286</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -2097,7 +2178,7 @@
       </c>
       <c r="G23" s="7"/>
       <c r="H23" s="3" t="s">
-        <v>269</v>
+        <v>285</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -2118,9 +2199,7 @@
       </c>
       <c r="F24" s="7"/>
       <c r="G24" s="7"/>
-      <c r="H24" s="3" t="s">
-        <v>269</v>
-      </c>
+      <c r="H24" s="3"/>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="19" t="s">
@@ -2140,9 +2219,7 @@
       </c>
       <c r="F25" s="7"/>
       <c r="G25" s="7"/>
-      <c r="H25" s="3" t="s">
-        <v>269</v>
-      </c>
+      <c r="H25" s="3"/>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="19" t="s">
@@ -2162,9 +2239,7 @@
       </c>
       <c r="F26" s="7"/>
       <c r="G26" s="7"/>
-      <c r="H26" s="3" t="s">
-        <v>269</v>
-      </c>
+      <c r="H26" s="3"/>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="19" t="s">
@@ -2184,9 +2259,7 @@
       </c>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
-      <c r="H27" s="3" t="s">
-        <v>269</v>
-      </c>
+      <c r="H27" s="3"/>
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="19" t="s">
@@ -2208,9 +2281,7 @@
         <v>3000</v>
       </c>
       <c r="G28" s="7"/>
-      <c r="H28" s="3" t="s">
-        <v>269</v>
-      </c>
+      <c r="H28" s="3"/>
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="19" t="s">
@@ -2230,9 +2301,7 @@
       </c>
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
-      <c r="H29" s="3" t="s">
-        <v>269</v>
-      </c>
+      <c r="H29" s="3"/>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="19" t="s">
@@ -2254,9 +2323,7 @@
         <v>3000</v>
       </c>
       <c r="G30" s="7"/>
-      <c r="H30" s="3" t="s">
-        <v>269</v>
-      </c>
+      <c r="H30" s="3"/>
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="19" t="s">
@@ -2276,9 +2343,7 @@
       </c>
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
-      <c r="H31" s="3" t="s">
-        <v>269</v>
-      </c>
+      <c r="H31" s="3"/>
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="19" t="s">
@@ -2300,9 +2365,7 @@
         <v>3000</v>
       </c>
       <c r="G32" s="7"/>
-      <c r="H32" s="3" t="s">
-        <v>269</v>
-      </c>
+      <c r="H32" s="3"/>
     </row>
     <row r="33" spans="1:8">
       <c r="A33" s="19" t="s">
@@ -2322,9 +2385,7 @@
       </c>
       <c r="F33" s="3"/>
       <c r="G33" s="3"/>
-      <c r="H33" s="3" t="s">
-        <v>269</v>
-      </c>
+      <c r="H33" s="3"/>
     </row>
     <row r="34" spans="1:8">
       <c r="A34" s="19" t="s">
@@ -2344,9 +2405,7 @@
       </c>
       <c r="F34" s="3"/>
       <c r="G34" s="3"/>
-      <c r="H34" s="3" t="s">
-        <v>269</v>
-      </c>
+      <c r="H34" s="3"/>
     </row>
     <row r="35" spans="1:8">
       <c r="A35" s="19" t="s">
@@ -2368,9 +2427,7 @@
         <v>20000</v>
       </c>
       <c r="G35" s="7"/>
-      <c r="H35" s="3" t="s">
-        <v>269</v>
-      </c>
+      <c r="H35" s="3"/>
     </row>
     <row r="36" spans="1:8">
       <c r="A36" s="19" t="s">
@@ -2390,9 +2447,7 @@
       </c>
       <c r="F36" s="3"/>
       <c r="G36" s="3"/>
-      <c r="H36" s="3" t="s">
-        <v>269</v>
-      </c>
+      <c r="H36" s="3"/>
     </row>
     <row r="37" spans="1:8">
       <c r="A37" s="19" t="s">
@@ -2412,9 +2467,7 @@
       </c>
       <c r="F37" s="3"/>
       <c r="G37" s="3"/>
-      <c r="H37" s="3" t="s">
-        <v>270</v>
-      </c>
+      <c r="H37" s="3"/>
     </row>
     <row r="38" spans="1:8">
       <c r="A38" s="19" t="s">
@@ -2436,9 +2489,7 @@
         <v>10000</v>
       </c>
       <c r="G38" s="3"/>
-      <c r="H38" s="3" t="s">
-        <v>269</v>
-      </c>
+      <c r="H38" s="3"/>
     </row>
     <row r="39" spans="1:8">
       <c r="A39" s="19" t="s">
@@ -2458,9 +2509,7 @@
       </c>
       <c r="F39" s="3"/>
       <c r="G39" s="3"/>
-      <c r="H39" s="3" t="s">
-        <v>270</v>
-      </c>
+      <c r="H39" s="3"/>
     </row>
     <row r="40" spans="1:8">
       <c r="A40" s="19" t="s">
@@ -2482,9 +2531,7 @@
         <v>10000</v>
       </c>
       <c r="G40" s="3"/>
-      <c r="H40" s="3" t="s">
-        <v>269</v>
-      </c>
+      <c r="H40" s="3"/>
     </row>
     <row r="41" spans="1:8">
       <c r="A41" s="19" t="s">
@@ -2504,9 +2551,7 @@
       </c>
       <c r="F41" s="3"/>
       <c r="G41" s="3"/>
-      <c r="H41" s="3" t="s">
-        <v>270</v>
-      </c>
+      <c r="H41" s="3"/>
     </row>
     <row r="42" spans="1:8">
       <c r="A42" s="19" t="s">
@@ -2526,9 +2571,7 @@
       </c>
       <c r="F42" s="3"/>
       <c r="G42" s="3"/>
-      <c r="H42" s="3" t="s">
-        <v>269</v>
-      </c>
+      <c r="H42" s="3"/>
     </row>
     <row r="43" spans="1:8">
       <c r="A43" s="19" t="s">
@@ -2550,9 +2593,7 @@
         <v>30000</v>
       </c>
       <c r="G43" s="3"/>
-      <c r="H43" s="3" t="s">
-        <v>269</v>
-      </c>
+      <c r="H43" s="3"/>
     </row>
     <row r="44" spans="1:8">
       <c r="A44" s="19" t="s">
@@ -2572,9 +2613,7 @@
       </c>
       <c r="F44" s="3"/>
       <c r="G44" s="3"/>
-      <c r="H44" s="3" t="s">
-        <v>269</v>
-      </c>
+      <c r="H44" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2592,7 +2631,7 @@
   <dimension ref="A1:I55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E53" sqref="E53"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2686,7 +2725,7 @@
       </c>
       <c r="G5" s="9"/>
       <c r="H5" s="9" t="s">
-        <v>269</v>
+        <v>285</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -2710,7 +2749,7 @@
       </c>
       <c r="G6" s="9"/>
       <c r="H6" s="9" t="s">
-        <v>269</v>
+        <v>285</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -2734,7 +2773,7 @@
       </c>
       <c r="G7" s="9"/>
       <c r="H7" s="9" t="s">
-        <v>269</v>
+        <v>285</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -2756,7 +2795,7 @@
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
       <c r="H8" s="9" t="s">
-        <v>269</v>
+        <v>285</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -2780,7 +2819,7 @@
       </c>
       <c r="G9" s="9"/>
       <c r="H9" s="9" t="s">
-        <v>269</v>
+        <v>285</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -2802,7 +2841,7 @@
       <c r="F10" s="9"/>
       <c r="G10" s="9"/>
       <c r="H10" s="9" t="s">
-        <v>269</v>
+        <v>285</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -2826,7 +2865,7 @@
       </c>
       <c r="G11" s="9"/>
       <c r="H11" s="9" t="s">
-        <v>269</v>
+        <v>285</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -2848,7 +2887,7 @@
       <c r="F12" s="9"/>
       <c r="G12" s="9"/>
       <c r="H12" s="9" t="s">
-        <v>269</v>
+        <v>285</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -2872,7 +2911,7 @@
       </c>
       <c r="G13" s="9"/>
       <c r="H13" s="9" t="s">
-        <v>269</v>
+        <v>285</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -2894,7 +2933,7 @@
       <c r="F14" s="9"/>
       <c r="G14" s="9"/>
       <c r="H14" s="9" t="s">
-        <v>269</v>
+        <v>285</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -2918,7 +2957,7 @@
       </c>
       <c r="G15" s="9"/>
       <c r="H15" s="9" t="s">
-        <v>269</v>
+        <v>285</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -2942,7 +2981,7 @@
       </c>
       <c r="G16" s="9"/>
       <c r="H16" s="9" t="s">
-        <v>269</v>
+        <v>285</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -2966,7 +3005,7 @@
       </c>
       <c r="G17" s="9"/>
       <c r="H17" s="9" t="s">
-        <v>269</v>
+        <v>286</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -2988,7 +3027,7 @@
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
       <c r="H18" s="9" t="s">
-        <v>269</v>
+        <v>285</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -3012,7 +3051,7 @@
       </c>
       <c r="G19" s="3"/>
       <c r="H19" s="9" t="s">
-        <v>269</v>
+        <v>286</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -3036,7 +3075,7 @@
       </c>
       <c r="G20" s="3"/>
       <c r="H20" s="9" t="s">
-        <v>269</v>
+        <v>286</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -3058,7 +3097,7 @@
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
       <c r="H21" s="9" t="s">
-        <v>269</v>
+        <v>286</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -3082,7 +3121,7 @@
       </c>
       <c r="G22" s="7"/>
       <c r="H22" s="9" t="s">
-        <v>269</v>
+        <v>285</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -3103,9 +3142,7 @@
       </c>
       <c r="F23" s="7"/>
       <c r="G23" s="7"/>
-      <c r="H23" s="9" t="s">
-        <v>269</v>
-      </c>
+      <c r="H23" s="9"/>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="3" t="s">
@@ -3125,9 +3162,7 @@
       </c>
       <c r="F24" s="9"/>
       <c r="G24" s="9"/>
-      <c r="H24" s="9" t="s">
-        <v>269</v>
-      </c>
+      <c r="H24" s="9"/>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="3" t="s">
@@ -3147,9 +3182,7 @@
       </c>
       <c r="F25" s="9"/>
       <c r="G25" s="9"/>
-      <c r="H25" s="9" t="s">
-        <v>270</v>
-      </c>
+      <c r="H25" s="9"/>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="3" t="s">
@@ -3169,9 +3202,7 @@
       </c>
       <c r="F26" s="9"/>
       <c r="G26" s="9"/>
-      <c r="H26" s="9" t="s">
-        <v>269</v>
-      </c>
+      <c r="H26" s="9"/>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="3" t="s">
@@ -3191,9 +3222,7 @@
       </c>
       <c r="F27" s="9"/>
       <c r="G27" s="9"/>
-      <c r="H27" s="9" t="s">
-        <v>269</v>
-      </c>
+      <c r="H27" s="9"/>
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="3" t="s">
@@ -3215,9 +3244,7 @@
         <v>3000</v>
       </c>
       <c r="G28" s="7"/>
-      <c r="H28" s="9" t="s">
-        <v>269</v>
-      </c>
+      <c r="H28" s="9"/>
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="3" t="s">
@@ -3237,9 +3264,7 @@
       </c>
       <c r="F29" s="9"/>
       <c r="G29" s="9"/>
-      <c r="H29" s="9" t="s">
-        <v>269</v>
-      </c>
+      <c r="H29" s="9"/>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="3" t="s">
@@ -3259,9 +3284,7 @@
       </c>
       <c r="F30" s="9"/>
       <c r="G30" s="9"/>
-      <c r="H30" s="9" t="s">
-        <v>269</v>
-      </c>
+      <c r="H30" s="9"/>
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="3" t="s">
@@ -3283,9 +3306,7 @@
         <v>186</v>
       </c>
       <c r="G31" s="9"/>
-      <c r="H31" s="9" t="s">
-        <v>269</v>
-      </c>
+      <c r="H31" s="9"/>
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="3" t="s">
@@ -3307,9 +3328,7 @@
         <v>186</v>
       </c>
       <c r="G32" s="9"/>
-      <c r="H32" s="9" t="s">
-        <v>269</v>
-      </c>
+      <c r="H32" s="9"/>
     </row>
     <row r="33" spans="1:8">
       <c r="A33" s="3" t="s">
@@ -3331,9 +3350,7 @@
         <v>43525</v>
       </c>
       <c r="G33" s="12"/>
-      <c r="H33" s="9" t="s">
-        <v>269</v>
-      </c>
+      <c r="H33" s="9"/>
     </row>
     <row r="34" spans="1:8">
       <c r="A34" s="3" t="s">
@@ -3355,9 +3372,7 @@
         <v>45743</v>
       </c>
       <c r="G34" s="12"/>
-      <c r="H34" s="9" t="s">
-        <v>269</v>
-      </c>
+      <c r="H34" s="9"/>
     </row>
     <row r="35" spans="1:8">
       <c r="A35" s="3" t="s">
@@ -3377,9 +3392,7 @@
       </c>
       <c r="F35" s="9"/>
       <c r="G35" s="9"/>
-      <c r="H35" s="9" t="s">
-        <v>269</v>
-      </c>
+      <c r="H35" s="9"/>
     </row>
     <row r="36" spans="1:8">
       <c r="A36" s="3" t="s">
@@ -3399,9 +3412,7 @@
       </c>
       <c r="F36" s="9"/>
       <c r="G36" s="9"/>
-      <c r="H36" s="9" t="s">
-        <v>269</v>
-      </c>
+      <c r="H36" s="9"/>
     </row>
     <row r="37" spans="1:8">
       <c r="A37" s="3" t="s">
@@ -3423,9 +3434,7 @@
         <v>153</v>
       </c>
       <c r="G37" s="3"/>
-      <c r="H37" s="9" t="s">
-        <v>269</v>
-      </c>
+      <c r="H37" s="9"/>
     </row>
     <row r="38" spans="1:8">
       <c r="A38" s="3" t="s">
@@ -3445,9 +3454,7 @@
       </c>
       <c r="F38" s="3"/>
       <c r="G38" s="3"/>
-      <c r="H38" s="9" t="s">
-        <v>269</v>
-      </c>
+      <c r="H38" s="9"/>
     </row>
     <row r="39" spans="1:8">
       <c r="A39" s="3" t="s">
@@ -3469,9 +3476,7 @@
         <v>156</v>
       </c>
       <c r="G39" s="3"/>
-      <c r="H39" s="9" t="s">
-        <v>269</v>
-      </c>
+      <c r="H39" s="9"/>
     </row>
     <row r="40" spans="1:8">
       <c r="A40" s="3" t="s">
@@ -3491,9 +3496,7 @@
       </c>
       <c r="F40" s="9"/>
       <c r="G40" s="9"/>
-      <c r="H40" s="9" t="s">
-        <v>269</v>
-      </c>
+      <c r="H40" s="9"/>
     </row>
     <row r="41" spans="1:8">
       <c r="A41" s="3" t="s">
@@ -3515,9 +3518,7 @@
         <v>5000</v>
       </c>
       <c r="G41" s="9"/>
-      <c r="H41" s="9" t="s">
-        <v>269</v>
-      </c>
+      <c r="H41" s="9"/>
     </row>
     <row r="42" spans="1:8">
       <c r="A42" s="3" t="s">
@@ -3537,9 +3538,7 @@
       </c>
       <c r="F42" s="9"/>
       <c r="G42" s="9"/>
-      <c r="H42" s="9" t="s">
-        <v>269</v>
-      </c>
+      <c r="H42" s="9"/>
     </row>
     <row r="43" spans="1:8">
       <c r="A43" s="3" t="s">
@@ -3561,9 +3560,7 @@
         <v>10000</v>
       </c>
       <c r="G43" s="9"/>
-      <c r="H43" s="9" t="s">
-        <v>269</v>
-      </c>
+      <c r="H43" s="9"/>
     </row>
     <row r="44" spans="1:8">
       <c r="A44" s="3" t="s">
@@ -3583,9 +3580,7 @@
       </c>
       <c r="F44" s="9"/>
       <c r="G44" s="9"/>
-      <c r="H44" s="9" t="s">
-        <v>269</v>
-      </c>
+      <c r="H44" s="9"/>
     </row>
     <row r="45" spans="1:8">
       <c r="A45" s="3" t="s">
@@ -3605,9 +3600,7 @@
       </c>
       <c r="F45" s="9"/>
       <c r="G45" s="9"/>
-      <c r="H45" s="9" t="s">
-        <v>269</v>
-      </c>
+      <c r="H45" s="9"/>
     </row>
     <row r="46" spans="1:8">
       <c r="A46" s="3" t="s">
@@ -3629,9 +3622,7 @@
         <v>20000</v>
       </c>
       <c r="G46" s="7"/>
-      <c r="H46" s="3" t="s">
-        <v>269</v>
-      </c>
+      <c r="H46" s="3"/>
     </row>
     <row r="47" spans="1:8">
       <c r="A47" s="3" t="s">
@@ -3651,9 +3642,7 @@
       </c>
       <c r="F47" s="3"/>
       <c r="G47" s="3"/>
-      <c r="H47" s="3" t="s">
-        <v>269</v>
-      </c>
+      <c r="H47" s="3"/>
     </row>
     <row r="48" spans="1:8">
       <c r="A48" s="3" t="s">
@@ -3673,9 +3662,7 @@
       </c>
       <c r="F48" s="3"/>
       <c r="G48" s="3"/>
-      <c r="H48" s="3" t="s">
-        <v>270</v>
-      </c>
+      <c r="H48" s="3"/>
     </row>
     <row r="49" spans="1:8">
       <c r="A49" s="3" t="s">
@@ -3697,9 +3684,7 @@
         <v>10000</v>
       </c>
       <c r="G49" s="3"/>
-      <c r="H49" s="3" t="s">
-        <v>269</v>
-      </c>
+      <c r="H49" s="3"/>
     </row>
     <row r="50" spans="1:8">
       <c r="A50" s="3" t="s">
@@ -3719,9 +3704,7 @@
       </c>
       <c r="F50" s="3"/>
       <c r="G50" s="3"/>
-      <c r="H50" s="3" t="s">
-        <v>270</v>
-      </c>
+      <c r="H50" s="3"/>
     </row>
     <row r="51" spans="1:8">
       <c r="A51" s="3" t="s">
@@ -3743,9 +3726,7 @@
         <v>10000</v>
       </c>
       <c r="G51" s="3"/>
-      <c r="H51" s="3" t="s">
-        <v>269</v>
-      </c>
+      <c r="H51" s="3"/>
     </row>
     <row r="52" spans="1:8">
       <c r="A52" s="3" t="s">
@@ -3765,9 +3746,7 @@
       </c>
       <c r="F52" s="3"/>
       <c r="G52" s="3"/>
-      <c r="H52" s="3" t="s">
-        <v>270</v>
-      </c>
+      <c r="H52" s="3"/>
     </row>
     <row r="53" spans="1:8">
       <c r="A53" s="3" t="s">
@@ -3787,9 +3766,7 @@
       </c>
       <c r="F53" s="3"/>
       <c r="G53" s="3"/>
-      <c r="H53" s="3" t="s">
-        <v>270</v>
-      </c>
+      <c r="H53" s="3"/>
     </row>
     <row r="54" spans="1:8">
       <c r="A54" s="3" t="s">
@@ -3811,9 +3788,7 @@
         <v>30000</v>
       </c>
       <c r="G54" s="3"/>
-      <c r="H54" s="3" t="s">
-        <v>269</v>
-      </c>
+      <c r="H54" s="3"/>
     </row>
     <row r="55" spans="1:8">
       <c r="A55" s="3" t="s">
@@ -3833,9 +3808,7 @@
       </c>
       <c r="F55" s="3"/>
       <c r="G55" s="3"/>
-      <c r="H55" s="3" t="s">
-        <v>269</v>
-      </c>
+      <c r="H55" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -3848,6 +3821,1019 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D61013C2-7F35-4D0B-B54C-3015EDB52E25}">
+  <dimension ref="A1:I48"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0" zoomScale="85" zoomScaleNormal="85">
+      <selection activeCell="F50" sqref="F50"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="39.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="27.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="32.5703125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="31.42578125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="31.42578125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="7.85546875" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="24"/>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="22" t="s">
+        <v>157</v>
+      </c>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="24"/>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="25"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="27"/>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row customFormat="1" r="5" s="33" spans="1:8">
+      <c r="A5" s="16" t="s">
+        <v>269</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+    </row>
+    <row customFormat="1" r="6" s="33" spans="1:8">
+      <c r="A6" s="16" t="s">
+        <v>269</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="F6" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
+    </row>
+    <row customFormat="1" r="7" s="33" spans="1:8">
+      <c r="A7" s="16" t="s">
+        <v>269</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="F7" s="35">
+        <v>5000</v>
+      </c>
+      <c r="G7" s="35"/>
+      <c r="H7" s="16"/>
+    </row>
+    <row customFormat="1" r="8" s="33" spans="1:8">
+      <c r="A8" s="16" t="s">
+        <v>269</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
+    </row>
+    <row customFormat="1" r="9" s="33" spans="1:8">
+      <c r="A9" s="16" t="s">
+        <v>269</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="F9" s="36" t="s">
+        <v>57</v>
+      </c>
+      <c r="G9" s="36"/>
+      <c r="H9" s="16"/>
+    </row>
+    <row customFormat="1" r="10" s="33" spans="1:8">
+      <c r="A10" s="16" t="s">
+        <v>269</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16"/>
+    </row>
+    <row customFormat="1" r="11" s="33" spans="1:8">
+      <c r="A11" s="16" t="s">
+        <v>269</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="D11" s="37" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="F11" s="36" t="s">
+        <v>62</v>
+      </c>
+      <c r="G11" s="36"/>
+      <c r="H11" s="16"/>
+    </row>
+    <row customFormat="1" r="12" s="33" spans="1:8">
+      <c r="A12" s="16" t="s">
+        <v>269</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="37" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="F12" s="16"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="16"/>
+    </row>
+    <row customFormat="1" r="13" s="33" spans="1:8">
+      <c r="A13" s="16" t="s">
+        <v>269</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="F13" s="36" t="s">
+        <v>62</v>
+      </c>
+      <c r="G13" s="36"/>
+      <c r="H13" s="16"/>
+    </row>
+    <row customFormat="1" r="14" s="33" spans="1:8">
+      <c r="A14" s="16" t="s">
+        <v>269</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="E14" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16"/>
+    </row>
+    <row customFormat="1" r="15" s="33" spans="1:8">
+      <c r="A15" s="16" t="s">
+        <v>269</v>
+      </c>
+      <c r="B15" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="E15" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="F15" s="36" t="s">
+        <v>62</v>
+      </c>
+      <c r="G15" s="36"/>
+      <c r="H15" s="16"/>
+    </row>
+    <row customFormat="1" r="16" s="33" spans="1:8">
+      <c r="A16" s="16" t="s">
+        <v>269</v>
+      </c>
+      <c r="B16" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="E16" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="F16" s="36" t="s">
+        <v>143</v>
+      </c>
+      <c r="G16" s="36"/>
+      <c r="H16" s="16"/>
+    </row>
+    <row customFormat="1" r="17" s="33" spans="1:8">
+      <c r="A17" s="16" t="s">
+        <v>269</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>144</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="E17" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="F17" s="36">
+        <v>5000</v>
+      </c>
+      <c r="G17" s="36"/>
+      <c r="H17" s="16"/>
+    </row>
+    <row customFormat="1" r="18" s="33" spans="1:8">
+      <c r="A18" s="16" t="s">
+        <v>269</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="E18" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="F18" s="16"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="16"/>
+    </row>
+    <row customFormat="1" r="19" s="33" spans="1:8">
+      <c r="A19" s="16" t="s">
+        <v>269</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="E19" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="F19" s="16" t="s">
+        <v>270</v>
+      </c>
+      <c r="G19" s="16"/>
+      <c r="H19" s="16"/>
+    </row>
+    <row customFormat="1" r="20" s="33" spans="1:8">
+      <c r="A20" s="16" t="s">
+        <v>269</v>
+      </c>
+      <c r="B20" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D20" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="E20" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="F20" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="G20" s="16"/>
+      <c r="H20" s="16"/>
+    </row>
+    <row customFormat="1" r="21" s="33" spans="1:8">
+      <c r="A21" s="16" t="s">
+        <v>269</v>
+      </c>
+      <c r="B21" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="D21" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="E21" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="F21" s="16"/>
+      <c r="G21" s="16"/>
+      <c r="H21" s="16"/>
+    </row>
+    <row customFormat="1" r="22" s="33" spans="1:8">
+      <c r="A22" s="16" t="s">
+        <v>269</v>
+      </c>
+      <c r="B22" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="D22" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="E22" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="F22" s="36">
+        <v>3000</v>
+      </c>
+      <c r="G22" s="36"/>
+      <c r="H22" s="16"/>
+    </row>
+    <row customFormat="1" r="23" s="33" spans="1:8">
+      <c r="A23" s="16" t="s">
+        <v>269</v>
+      </c>
+      <c r="B23" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C23" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="D23" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="E23" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="F23" s="36"/>
+      <c r="G23" s="36"/>
+      <c r="H23" s="16"/>
+    </row>
+    <row customFormat="1" r="24" s="33" spans="1:8">
+      <c r="A24" s="16" t="s">
+        <v>269</v>
+      </c>
+      <c r="B24" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="C24" s="16" t="s">
+        <v>140</v>
+      </c>
+      <c r="D24" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="E24" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="F24" s="36"/>
+      <c r="G24" s="36"/>
+      <c r="H24" s="16"/>
+    </row>
+    <row customFormat="1" r="25" s="33" spans="1:8">
+      <c r="A25" s="16" t="s">
+        <v>269</v>
+      </c>
+      <c r="B25" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="C25" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="D25" s="16" t="s">
+        <v>147</v>
+      </c>
+      <c r="E25" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="F25" s="36"/>
+      <c r="G25" s="36"/>
+      <c r="H25" s="16"/>
+    </row>
+    <row customFormat="1" r="26" s="33" spans="1:8">
+      <c r="A26" s="16" t="s">
+        <v>269</v>
+      </c>
+      <c r="B26" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="C26" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="D26" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="E26" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="F26" s="16"/>
+      <c r="G26" s="16"/>
+      <c r="H26" s="16"/>
+    </row>
+    <row customFormat="1" r="27" s="33" spans="1:8">
+      <c r="A27" s="16" t="s">
+        <v>269</v>
+      </c>
+      <c r="B27" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C27" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="D27" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="E27" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="F27" s="36">
+        <v>3000</v>
+      </c>
+      <c r="G27" s="36"/>
+      <c r="H27" s="16"/>
+    </row>
+    <row customFormat="1" r="28" s="34" spans="1:8">
+      <c r="A28" s="16" t="s">
+        <v>269</v>
+      </c>
+      <c r="B28" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="C28" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="D28" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="E28" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="F28" s="16"/>
+      <c r="G28" s="16"/>
+      <c r="H28" s="16"/>
+    </row>
+    <row customFormat="1" r="29" s="33" spans="1:8">
+      <c r="A29" s="16" t="s">
+        <v>269</v>
+      </c>
+      <c r="B29" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="C29" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="D29" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="E29" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="F29" s="36">
+        <v>8000</v>
+      </c>
+      <c r="G29" s="36"/>
+      <c r="H29" s="16"/>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30" s="16" t="s">
+        <v>269</v>
+      </c>
+      <c r="B30" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="C30" s="16" t="s">
+        <v>271</v>
+      </c>
+      <c r="D30" s="16" t="s">
+        <v>272</v>
+      </c>
+      <c r="E30" s="16" t="s">
+        <v>273</v>
+      </c>
+      <c r="F30" s="36" t="s">
+        <v>274</v>
+      </c>
+      <c r="G30" s="36"/>
+      <c r="H30" s="16"/>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31" s="16" t="s">
+        <v>269</v>
+      </c>
+      <c r="B31" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="C31" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="D31" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="E31" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="F31" s="36">
+        <v>8000</v>
+      </c>
+      <c r="G31" s="36"/>
+      <c r="H31" s="16"/>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32" s="16" t="s">
+        <v>269</v>
+      </c>
+      <c r="B32" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="C32" s="16" t="s">
+        <v>275</v>
+      </c>
+      <c r="D32" s="16" t="s">
+        <v>276</v>
+      </c>
+      <c r="E32" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="F32" s="36"/>
+      <c r="G32" s="36"/>
+      <c r="H32" s="16"/>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33" s="16" t="s">
+        <v>269</v>
+      </c>
+      <c r="B33" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="C33" s="16" t="s">
+        <v>277</v>
+      </c>
+      <c r="D33" s="16" t="s">
+        <v>278</v>
+      </c>
+      <c r="E33" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="F33" s="36"/>
+      <c r="G33" s="36"/>
+      <c r="H33" s="16"/>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34" s="16" t="s">
+        <v>269</v>
+      </c>
+      <c r="B34" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="C34" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="D34" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="E34" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="F34" s="36">
+        <v>3000</v>
+      </c>
+      <c r="G34" s="36"/>
+      <c r="H34" s="16"/>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="A35" s="16" t="s">
+        <v>269</v>
+      </c>
+      <c r="B35" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="C35" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="D35" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="E35" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="F35" s="36"/>
+      <c r="G35" s="36"/>
+      <c r="H35" s="16"/>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="A36" s="16" t="s">
+        <v>269</v>
+      </c>
+      <c r="B36" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="C36" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="D36" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="E36" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="F36" s="36">
+        <v>3000</v>
+      </c>
+      <c r="G36" s="36"/>
+      <c r="H36" s="16"/>
+    </row>
+    <row r="37" spans="1:8">
+      <c r="A37" s="16" t="s">
+        <v>269</v>
+      </c>
+      <c r="B37" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="C37" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="D37" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="E37" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="F37" s="36"/>
+      <c r="G37" s="36"/>
+      <c r="H37" s="16"/>
+    </row>
+    <row r="38" spans="1:8">
+      <c r="A38" s="16" t="s">
+        <v>269</v>
+      </c>
+      <c r="B38" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="C38" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="D38" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="E38" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="F38" s="36"/>
+      <c r="G38" s="36"/>
+      <c r="H38" s="16"/>
+    </row>
+    <row r="39" spans="1:8">
+      <c r="A39" s="16" t="s">
+        <v>269</v>
+      </c>
+      <c r="B39" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="C39" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="D39" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="E39" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="F39" s="36">
+        <v>20000</v>
+      </c>
+      <c r="G39" s="36"/>
+      <c r="H39" s="16"/>
+    </row>
+    <row r="40" spans="1:8">
+      <c r="A40" s="16" t="s">
+        <v>269</v>
+      </c>
+      <c r="B40" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="C40" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="D40" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="E40" s="16" t="s">
+        <v>267</v>
+      </c>
+      <c r="F40" s="36"/>
+      <c r="G40" s="36"/>
+      <c r="H40" s="16"/>
+    </row>
+    <row r="41" spans="1:8">
+      <c r="A41" s="16" t="s">
+        <v>269</v>
+      </c>
+      <c r="B41" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="C41" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="D41" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="E41" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="F41" s="36"/>
+      <c r="G41" s="36"/>
+      <c r="H41" s="16"/>
+    </row>
+    <row r="42" spans="1:8">
+      <c r="A42" s="16" t="s">
+        <v>269</v>
+      </c>
+      <c r="B42" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="C42" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="D42" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="E42" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="F42" s="36">
+        <v>10000</v>
+      </c>
+      <c r="G42" s="36"/>
+      <c r="H42" s="16"/>
+    </row>
+    <row r="43" spans="1:8">
+      <c r="A43" s="16" t="s">
+        <v>269</v>
+      </c>
+      <c r="B43" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="C43" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="D43" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="E43" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="F43" s="36"/>
+      <c r="G43" s="36"/>
+      <c r="H43" s="16"/>
+    </row>
+    <row r="44" spans="1:8">
+      <c r="A44" s="16" t="s">
+        <v>269</v>
+      </c>
+      <c r="B44" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="C44" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="D44" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="E44" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="F44" s="36">
+        <v>10000</v>
+      </c>
+      <c r="G44" s="36"/>
+      <c r="H44" s="16"/>
+    </row>
+    <row r="45" spans="1:8">
+      <c r="A45" s="16" t="s">
+        <v>269</v>
+      </c>
+      <c r="B45" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="C45" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="D45" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="E45" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="F45" s="36"/>
+      <c r="G45" s="36"/>
+      <c r="H45" s="16"/>
+    </row>
+    <row r="46" spans="1:8">
+      <c r="A46" s="16" t="s">
+        <v>269</v>
+      </c>
+      <c r="B46" s="16" t="s">
+        <v>279</v>
+      </c>
+      <c r="C46" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="D46" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="E46" s="16" t="s">
+        <v>267</v>
+      </c>
+      <c r="F46" s="36"/>
+      <c r="G46" s="36"/>
+      <c r="H46" s="16"/>
+    </row>
+    <row r="47" spans="1:8">
+      <c r="A47" s="16" t="s">
+        <v>269</v>
+      </c>
+      <c r="B47" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="C47" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="D47" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="E47" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="F47" s="36">
+        <v>30000</v>
+      </c>
+      <c r="G47" s="36"/>
+      <c r="H47" s="16"/>
+    </row>
+    <row r="48" spans="1:8">
+      <c r="A48" s="16" t="s">
+        <v>269</v>
+      </c>
+      <c r="B48" s="16" t="s">
+        <v>280</v>
+      </c>
+      <c r="C48" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="D48" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="E48" s="16" t="s">
+        <v>228</v>
+      </c>
+      <c r="F48" s="36"/>
+      <c r="G48" s="36"/>
+      <c r="H48" s="16"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A3:H3"/>
+  </mergeCells>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" r:id="rId1" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84C8C304-D672-42E3-8009-BB544F384D0E}">
   <dimension ref="A1:I62"/>
   <sheetViews>
@@ -3946,7 +4932,7 @@
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="3" t="s">
-        <v>269</v>
+        <v>285</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -3970,7 +4956,7 @@
       </c>
       <c r="G6" s="3"/>
       <c r="H6" s="3" t="s">
-        <v>269</v>
+        <v>285</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -3994,7 +4980,7 @@
       </c>
       <c r="G7" s="6"/>
       <c r="H7" s="3" t="s">
-        <v>269</v>
+        <v>285</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -4016,7 +5002,7 @@
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3" t="s">
-        <v>269</v>
+        <v>285</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -4040,7 +5026,7 @@
       </c>
       <c r="G9" s="7"/>
       <c r="H9" s="3" t="s">
-        <v>269</v>
+        <v>285</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -4062,7 +5048,7 @@
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3" t="s">
-        <v>269</v>
+        <v>285</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -4086,7 +5072,7 @@
       </c>
       <c r="G11" s="7"/>
       <c r="H11" s="3" t="s">
-        <v>269</v>
+        <v>285</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -4110,7 +5096,7 @@
       </c>
       <c r="G12" s="3"/>
       <c r="H12" s="3" t="s">
-        <v>269</v>
+        <v>285</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -4134,7 +5120,7 @@
       </c>
       <c r="G13" s="7"/>
       <c r="H13" s="3" t="s">
-        <v>269</v>
+        <v>285</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -4156,7 +5142,7 @@
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
       <c r="H14" s="3" t="s">
-        <v>269</v>
+        <v>285</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -4180,7 +5166,7 @@
       </c>
       <c r="G15" s="7"/>
       <c r="H15" s="3" t="s">
-        <v>269</v>
+        <v>285</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -4202,7 +5188,7 @@
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
       <c r="H16" s="3" t="s">
-        <v>269</v>
+        <v>285</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -4224,7 +5210,7 @@
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
       <c r="H17" s="3" t="s">
-        <v>269</v>
+        <v>285</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -4246,7 +5232,7 @@
       <c r="F18" s="7"/>
       <c r="G18" s="7"/>
       <c r="H18" s="3" t="s">
-        <v>269</v>
+        <v>285</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -4268,7 +5254,7 @@
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
       <c r="H19" s="3" t="s">
-        <v>269</v>
+        <v>285</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -4292,7 +5278,7 @@
       </c>
       <c r="G20" s="7"/>
       <c r="H20" s="3" t="s">
-        <v>269</v>
+        <v>285</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -4316,7 +5302,7 @@
       </c>
       <c r="G21" s="7"/>
       <c r="H21" s="3" t="s">
-        <v>269</v>
+        <v>285</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -4340,7 +5326,7 @@
       </c>
       <c r="G22" s="7"/>
       <c r="H22" s="3" t="s">
-        <v>270</v>
+        <v>286</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -4364,7 +5350,7 @@
       </c>
       <c r="G23" s="7"/>
       <c r="H23" s="3" t="s">
-        <v>269</v>
+        <v>285</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -4386,7 +5372,7 @@
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
       <c r="H24" s="3" t="s">
-        <v>270</v>
+        <v>286</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -4410,7 +5396,7 @@
       </c>
       <c r="G25" s="3"/>
       <c r="H25" s="3" t="s">
-        <v>270</v>
+        <v>286</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -4434,7 +5420,7 @@
       </c>
       <c r="G26" s="3"/>
       <c r="H26" s="3" t="s">
-        <v>270</v>
+        <v>286</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -4456,7 +5442,7 @@
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
       <c r="H27" s="3" t="s">
-        <v>270</v>
+        <v>286</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -4480,7 +5466,7 @@
       </c>
       <c r="G28" s="7"/>
       <c r="H28" s="3" t="s">
-        <v>269</v>
+        <v>285</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -5210,7 +6196,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B59FADFD-33E9-4E6D-B86E-1A88AF7CF694}">
   <dimension ref="A1:I44"/>
   <sheetViews>
@@ -6134,20 +7120,20 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38793A77-4CB9-44FE-853A-5596922718C4}">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="22.140625" collapsed="true"/>
     <col min="2" max="2" customWidth="true" width="18.7109375" collapsed="true"/>
     <col min="3" max="3" customWidth="true" width="21.42578125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="19.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="28.0" collapsed="true"/>
     <col min="5" max="5" bestFit="true" customWidth="true" width="18.85546875" collapsed="true"/>
     <col min="6" max="6" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
     <col min="7" max="7" customWidth="true" width="19.5703125" collapsed="true"/>
@@ -6293,6 +7279,23 @@
         <v>86</v>
       </c>
     </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="16" t="s">
+        <v>269</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>274</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>284</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:H1"/>
@@ -6303,7 +7306,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B52690B1-76B3-48CD-AA9A-87FEE1811DD3}">
   <dimension ref="A2:C3"/>
   <sheetViews>

</xml_diff>

<commit_message>
Updated POM for commons-io dependency
</commit_message>
<xml_diff>
--- a/TestDataAndResults/Run1/SophieAutomation.xlsx
+++ b/TestDataAndResults/Run1/SophieAutomation.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr documentId="13_ncr:1_{1C1D9540-4568-420E-91B6-3A27BB8435DB}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43"/>
+  <xr:revisionPtr documentId="13_ncr:1_{9F2F17D2-DEBD-4FDB-88DC-8ECCBA13A062}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43"/>
   <bookViews>
-    <workbookView activeTab="4" firstSheet="4" windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
+    <workbookView activeTab="4" firstSheet="1" windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" r:id="rId1" sheetId="8"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1405" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1347" uniqueCount="286">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -465,9 +465,6 @@
     <t>rollBackToBaselineVersion</t>
   </si>
   <si>
-    <t>7.143.113..NA.01-01-01</t>
-  </si>
-  <si>
     <t>wait time</t>
   </si>
   <si>
@@ -891,10 +888,10 @@
     <t>Not Available</t>
   </si>
   <si>
+    <t>23.218.94.2.NA.01-01-01</t>
+  </si>
+  <si>
     <t>Pass</t>
-  </si>
-  <si>
-    <t>Fail</t>
   </si>
 </sst>
 </file>
@@ -937,7 +934,7 @@
       <name val="Calibiri"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -959,18 +956,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1082,7 +1067,7 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="36">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
     <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
@@ -1105,6 +1090,8 @@
     <xf applyBorder="1" applyFont="1" borderId="8" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" applyFill="1" applyFont="1" borderId="3" fillId="2" fontId="1" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" applyFont="1" borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="1" fillId="0" fontId="3" numFmtId="0" quotePrefix="1" xfId="1"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="0" fontId="2" numFmtId="0" quotePrefix="1" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="2" fillId="3" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
@@ -1144,11 +1131,7 @@
     <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="7" fillId="3" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyFill="1" borderId="0" fillId="5" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="6" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="1" fillId="0" fontId="3" numFmtId="0" quotePrefix="1" xfId="1"/>
-    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="0" fontId="2" numFmtId="0" quotePrefix="1" xfId="0"/>
-    <xf applyFill="1" applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
@@ -1489,7 +1472,7 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>94</v>
@@ -1518,7 +1501,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1532,22 +1515,22 @@
   </cols>
   <sheetData>
     <row customFormat="1" ht="14.25" r="1" s="5" spans="1:5">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
     </row>
     <row customFormat="1" ht="14.25" r="2" s="5" spans="1:5">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="23" t="s">
         <v>132</v>
       </c>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
     </row>
     <row customFormat="1" ht="14.25" r="3" s="5" spans="1:5">
       <c r="A3" s="10"/>
@@ -1575,76 +1558,76 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>32</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E5" s="3"/>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>101</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E6" s="3"/>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>266</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>185</v>
-      </c>
       <c r="D7" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E7" s="3"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>282</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>281</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>283</v>
-      </c>
       <c r="D8" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E8" s="3"/>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="C9" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>205</v>
-      </c>
       <c r="D9" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E9" s="3"/>
     </row>
@@ -1661,8 +1644,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32EA4E71-0B53-4881-A15A-C454293CD34C}">
   <dimension ref="A1:I44"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1678,38 +1661,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="24"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="26"/>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="22" t="s">
-        <v>157</v>
-      </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="24"/>
+      <c r="A2" s="24" t="s">
+        <v>156</v>
+      </c>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="26"/>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="25"/>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
-      <c r="G3" s="26"/>
-      <c r="H3" s="27"/>
+      <c r="A3" s="27"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="29"/>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="18" t="s">
@@ -1731,7 +1714,7 @@
         <v>33</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H4" s="4" t="s">
         <v>3</v>
@@ -1739,7 +1722,7 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>6</v>
@@ -1763,7 +1746,7 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>10</v>
@@ -1787,7 +1770,7 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>11</v>
@@ -1811,7 +1794,7 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>12</v>
@@ -1827,13 +1810,11 @@
       </c>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
-      <c r="H8" s="3" t="s">
-        <v>285</v>
-      </c>
+      <c r="H8" s="3"/>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B9" s="9" t="s">
         <v>13</v>
@@ -1851,13 +1832,11 @@
         <v>2000</v>
       </c>
       <c r="G9" s="9"/>
-      <c r="H9" s="3" t="s">
-        <v>285</v>
-      </c>
+      <c r="H9" s="3"/>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B10" s="9" t="s">
         <v>14</v>
@@ -1873,13 +1852,11 @@
       </c>
       <c r="F10" s="9"/>
       <c r="G10" s="9"/>
-      <c r="H10" s="3" t="s">
-        <v>285</v>
-      </c>
+      <c r="H10" s="3"/>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B11" s="9" t="s">
         <v>15</v>
@@ -1897,13 +1874,11 @@
         <v>3000</v>
       </c>
       <c r="G11" s="9"/>
-      <c r="H11" s="3" t="s">
-        <v>285</v>
-      </c>
+      <c r="H11" s="3"/>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B12" s="9" t="s">
         <v>16</v>
@@ -1919,13 +1894,11 @@
       </c>
       <c r="F12" s="9"/>
       <c r="G12" s="9"/>
-      <c r="H12" s="3" t="s">
-        <v>285</v>
-      </c>
+      <c r="H12" s="3"/>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B13" s="9" t="s">
         <v>23</v>
@@ -1943,13 +1916,11 @@
         <v>3000</v>
       </c>
       <c r="G13" s="9"/>
-      <c r="H13" s="3" t="s">
-        <v>285</v>
-      </c>
+      <c r="H13" s="3"/>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B14" s="9" t="s">
         <v>89</v>
@@ -1965,13 +1936,11 @@
       </c>
       <c r="F14" s="9"/>
       <c r="G14" s="9"/>
-      <c r="H14" s="3" t="s">
-        <v>285</v>
-      </c>
+      <c r="H14" s="3"/>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B15" s="9" t="s">
         <v>26</v>
@@ -1989,13 +1958,11 @@
         <v>3000</v>
       </c>
       <c r="G15" s="9"/>
-      <c r="H15" s="3" t="s">
-        <v>285</v>
-      </c>
+      <c r="H15" s="3"/>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B16" s="9" t="s">
         <v>26</v>
@@ -2007,19 +1974,17 @@
         <v>31</v>
       </c>
       <c r="E16" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="F16" s="9" t="s">
         <v>199</v>
       </c>
-      <c r="F16" s="9" t="s">
-        <v>200</v>
-      </c>
       <c r="G16" s="9"/>
-      <c r="H16" s="3" t="s">
-        <v>285</v>
-      </c>
+      <c r="H16" s="3"/>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B17" s="9" t="s">
         <v>27</v>
@@ -2034,22 +1999,20 @@
         <v>142</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>143</v>
+        <v>284</v>
       </c>
       <c r="G17" s="9"/>
-      <c r="H17" s="3" t="s">
-        <v>286</v>
-      </c>
+      <c r="H17" s="3"/>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="19" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>27</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>31</v>
@@ -2061,13 +2024,11 @@
         <v>5000</v>
       </c>
       <c r="G18" s="7"/>
-      <c r="H18" s="3" t="s">
-        <v>285</v>
-      </c>
+      <c r="H18" s="3"/>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="19" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>27</v>
@@ -2083,13 +2044,11 @@
       </c>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
-      <c r="H19" s="3" t="s">
-        <v>285</v>
-      </c>
+      <c r="H19" s="3"/>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="19" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>28</v>
@@ -2107,13 +2066,11 @@
         <v>131</v>
       </c>
       <c r="G20" s="3"/>
-      <c r="H20" s="3" t="s">
-        <v>286</v>
-      </c>
+      <c r="H20" s="3"/>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="19" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>29</v>
@@ -2131,13 +2088,11 @@
         <v>65</v>
       </c>
       <c r="G21" s="3"/>
-      <c r="H21" s="3" t="s">
-        <v>286</v>
-      </c>
+      <c r="H21" s="3"/>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="19" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>36</v>
@@ -2153,13 +2108,11 @@
       </c>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
-      <c r="H22" s="3" t="s">
-        <v>286</v>
-      </c>
+      <c r="H22" s="3"/>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="19" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>37</v>
@@ -2177,13 +2130,11 @@
         <v>3000</v>
       </c>
       <c r="G23" s="7"/>
-      <c r="H23" s="3" t="s">
-        <v>285</v>
-      </c>
+      <c r="H23" s="3"/>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="19" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>37</v>
@@ -2195,7 +2146,7 @@
         <v>108</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F24" s="7"/>
       <c r="G24" s="7"/>
@@ -2203,7 +2154,7 @@
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="19" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>51</v>
@@ -2215,7 +2166,7 @@
         <v>139</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F25" s="7"/>
       <c r="G25" s="7"/>
@@ -2223,19 +2174,19 @@
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="19" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>51</v>
       </c>
       <c r="C26" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="D26" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="D26" s="3" t="s">
-        <v>147</v>
-      </c>
       <c r="E26" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F26" s="7"/>
       <c r="G26" s="7"/>
@@ -2243,7 +2194,7 @@
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="19" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>51</v>
@@ -2263,7 +2214,7 @@
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="19" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>52</v>
@@ -2285,7 +2236,7 @@
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="19" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>53</v>
@@ -2305,7 +2256,7 @@
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="19" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>59</v>
@@ -2327,7 +2278,7 @@
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="19" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>60</v>
@@ -2347,7 +2298,7 @@
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="19" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>61</v>
@@ -2369,7 +2320,7 @@
     </row>
     <row r="33" spans="1:8">
       <c r="A33" s="19" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>90</v>
@@ -2389,7 +2340,7 @@
     </row>
     <row r="34" spans="1:8">
       <c r="A34" s="19" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>91</v>
@@ -2409,7 +2360,7 @@
     </row>
     <row r="35" spans="1:8">
       <c r="A35" s="19" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>92</v>
@@ -2431,7 +2382,7 @@
     </row>
     <row r="36" spans="1:8">
       <c r="A36" s="19" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>93</v>
@@ -2443,7 +2394,7 @@
         <v>50</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F36" s="3"/>
       <c r="G36" s="3"/>
@@ -2451,7 +2402,7 @@
     </row>
     <row r="37" spans="1:8">
       <c r="A37" s="19" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>95</v>
@@ -2471,7 +2422,7 @@
     </row>
     <row r="38" spans="1:8">
       <c r="A38" s="19" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>92</v>
@@ -2493,7 +2444,7 @@
     </row>
     <row r="39" spans="1:8">
       <c r="A39" s="19" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>96</v>
@@ -2513,7 +2464,7 @@
     </row>
     <row r="40" spans="1:8">
       <c r="A40" s="19" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>96</v>
@@ -2535,7 +2486,7 @@
     </row>
     <row r="41" spans="1:8">
       <c r="A41" s="19" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>97</v>
@@ -2555,7 +2506,7 @@
     </row>
     <row r="42" spans="1:8">
       <c r="A42" s="19" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>98</v>
@@ -2567,7 +2518,7 @@
         <v>124</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F42" s="3"/>
       <c r="G42" s="3"/>
@@ -2575,7 +2526,7 @@
     </row>
     <row r="43" spans="1:8">
       <c r="A43" s="19" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>99</v>
@@ -2597,7 +2548,7 @@
     </row>
     <row r="44" spans="1:8">
       <c r="A44" s="19" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>100</v>
@@ -2609,7 +2560,7 @@
         <v>31</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F44" s="3"/>
       <c r="G44" s="3"/>
@@ -2630,8 +2581,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F162030-4240-4061-B605-62E03F55BA7B}">
   <dimension ref="A1:I55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2641,42 +2592,41 @@
     <col min="4" max="4" bestFit="true" customWidth="true" width="22.140625" collapsed="true"/>
     <col min="5" max="5" bestFit="true" customWidth="true" width="30.85546875" collapsed="true"/>
     <col min="6" max="6" bestFit="true" customWidth="true" width="26.5703125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="7.86328125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="24"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="26"/>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="22" t="s">
-        <v>157</v>
-      </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="24"/>
+      <c r="A2" s="24" t="s">
+        <v>156</v>
+      </c>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="26"/>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="25"/>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
-      <c r="G3" s="26"/>
-      <c r="H3" s="27"/>
+      <c r="A3" s="27"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="29"/>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="4" t="s">
@@ -2698,7 +2648,7 @@
         <v>33</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H4" s="4" t="s">
         <v>3</v>
@@ -2706,7 +2656,7 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>6</v>
@@ -2724,13 +2674,11 @@
         <v>31</v>
       </c>
       <c r="G5" s="9"/>
-      <c r="H5" s="9" t="s">
-        <v>285</v>
-      </c>
+      <c r="H5" s="9"/>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>10</v>
@@ -2748,13 +2696,11 @@
         <v>31</v>
       </c>
       <c r="G6" s="9"/>
-      <c r="H6" s="9" t="s">
-        <v>285</v>
-      </c>
+      <c r="H6" s="9"/>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>11</v>
@@ -2772,13 +2718,11 @@
         <v>5000</v>
       </c>
       <c r="G7" s="9"/>
-      <c r="H7" s="9" t="s">
-        <v>285</v>
-      </c>
+      <c r="H7" s="9"/>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>12</v>
@@ -2794,13 +2738,11 @@
       </c>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
-      <c r="H8" s="9" t="s">
-        <v>285</v>
-      </c>
+      <c r="H8" s="9"/>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B9" s="9" t="s">
         <v>13</v>
@@ -2818,13 +2760,11 @@
         <v>2000</v>
       </c>
       <c r="G9" s="9"/>
-      <c r="H9" s="9" t="s">
-        <v>285</v>
-      </c>
+      <c r="H9" s="9"/>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B10" s="9" t="s">
         <v>14</v>
@@ -2840,13 +2780,11 @@
       </c>
       <c r="F10" s="9"/>
       <c r="G10" s="9"/>
-      <c r="H10" s="9" t="s">
-        <v>285</v>
-      </c>
+      <c r="H10" s="9"/>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B11" s="9" t="s">
         <v>15</v>
@@ -2864,13 +2802,11 @@
         <v>3000</v>
       </c>
       <c r="G11" s="9"/>
-      <c r="H11" s="9" t="s">
-        <v>285</v>
-      </c>
+      <c r="H11" s="9"/>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B12" s="9" t="s">
         <v>16</v>
@@ -2886,13 +2822,11 @@
       </c>
       <c r="F12" s="9"/>
       <c r="G12" s="9"/>
-      <c r="H12" s="9" t="s">
-        <v>285</v>
-      </c>
+      <c r="H12" s="9"/>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B13" s="9" t="s">
         <v>23</v>
@@ -2910,13 +2844,11 @@
         <v>3000</v>
       </c>
       <c r="G13" s="9"/>
-      <c r="H13" s="9" t="s">
-        <v>285</v>
-      </c>
+      <c r="H13" s="9"/>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B14" s="9" t="s">
         <v>89</v>
@@ -2932,13 +2864,11 @@
       </c>
       <c r="F14" s="9"/>
       <c r="G14" s="9"/>
-      <c r="H14" s="9" t="s">
-        <v>285</v>
-      </c>
+      <c r="H14" s="9"/>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B15" s="9" t="s">
         <v>26</v>
@@ -2956,13 +2886,11 @@
         <v>3000</v>
       </c>
       <c r="G15" s="9"/>
-      <c r="H15" s="9" t="s">
-        <v>285</v>
-      </c>
+      <c r="H15" s="9"/>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B16" s="9" t="s">
         <v>26</v>
@@ -2974,19 +2902,17 @@
         <v>31</v>
       </c>
       <c r="E16" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="F16" s="9" t="s">
         <v>199</v>
       </c>
-      <c r="F16" s="9" t="s">
-        <v>200</v>
-      </c>
       <c r="G16" s="9"/>
-      <c r="H16" s="9" t="s">
-        <v>285</v>
-      </c>
+      <c r="H16" s="9"/>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B17" s="9" t="s">
         <v>27</v>
@@ -3001,16 +2927,14 @@
         <v>142</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>143</v>
+        <v>284</v>
       </c>
       <c r="G17" s="9"/>
-      <c r="H17" s="9" t="s">
-        <v>286</v>
-      </c>
+      <c r="H17" s="9"/>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>27</v>
@@ -3026,13 +2950,11 @@
       </c>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
-      <c r="H18" s="9" t="s">
-        <v>285</v>
-      </c>
+      <c r="H18" s="9"/>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>28</v>
@@ -3050,13 +2972,11 @@
         <v>133</v>
       </c>
       <c r="G19" s="3"/>
-      <c r="H19" s="9" t="s">
-        <v>286</v>
-      </c>
+      <c r="H19" s="9"/>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>29</v>
@@ -3074,13 +2994,11 @@
         <v>65</v>
       </c>
       <c r="G20" s="3"/>
-      <c r="H20" s="9" t="s">
-        <v>286</v>
-      </c>
+      <c r="H20" s="9"/>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>36</v>
@@ -3096,13 +3014,11 @@
       </c>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
-      <c r="H21" s="9" t="s">
-        <v>286</v>
-      </c>
+      <c r="H21" s="9"/>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>37</v>
@@ -3120,13 +3036,11 @@
         <v>3000</v>
       </c>
       <c r="G22" s="7"/>
-      <c r="H22" s="9" t="s">
-        <v>285</v>
-      </c>
+      <c r="H22" s="9"/>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>51</v>
@@ -3138,7 +3052,7 @@
         <v>107</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F23" s="7"/>
       <c r="G23" s="7"/>
@@ -3146,7 +3060,7 @@
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>52</v>
@@ -3158,7 +3072,7 @@
         <v>108</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F24" s="9"/>
       <c r="G24" s="9"/>
@@ -3166,7 +3080,7 @@
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>53</v>
@@ -3186,19 +3100,19 @@
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>53</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F26" s="9"/>
       <c r="G26" s="9"/>
@@ -3206,7 +3120,7 @@
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>59</v>
@@ -3226,7 +3140,7 @@
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>37</v>
@@ -3248,7 +3162,7 @@
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>60</v>
@@ -3268,7 +3182,7 @@
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>61</v>
@@ -3288,7 +3202,7 @@
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>90</v>
@@ -3303,14 +3217,14 @@
         <v>44</v>
       </c>
       <c r="F31" s="9" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G31" s="9"/>
       <c r="H31" s="9"/>
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>91</v>
@@ -3325,14 +3239,14 @@
         <v>44</v>
       </c>
       <c r="F32" s="9" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G32" s="9"/>
       <c r="H32" s="9"/>
     </row>
     <row r="33" spans="1:8">
       <c r="A33" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>92</v>
@@ -3354,7 +3268,7 @@
     </row>
     <row r="34" spans="1:8">
       <c r="A34" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>93</v>
@@ -3376,7 +3290,7 @@
     </row>
     <row r="35" spans="1:8">
       <c r="A35" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>96</v>
@@ -3396,7 +3310,7 @@
     </row>
     <row r="36" spans="1:8">
       <c r="A36" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>96</v>
@@ -3405,7 +3319,7 @@
         <v>126</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E36" s="3" t="s">
         <v>43</v>
@@ -3416,7 +3330,7 @@
     </row>
     <row r="37" spans="1:8">
       <c r="A37" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>97</v>
@@ -3425,20 +3339,20 @@
         <v>127</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E37" s="3" t="s">
         <v>119</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G37" s="3"/>
       <c r="H37" s="9"/>
     </row>
     <row r="38" spans="1:8">
       <c r="A38" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>97</v>
@@ -3447,7 +3361,7 @@
         <v>128</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E38" s="3" t="s">
         <v>43</v>
@@ -3458,7 +3372,7 @@
     </row>
     <row r="39" spans="1:8">
       <c r="A39" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>99</v>
@@ -3467,20 +3381,20 @@
         <v>135</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E39" s="3" t="s">
         <v>119</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G39" s="3"/>
       <c r="H39" s="9"/>
     </row>
     <row r="40" spans="1:8">
       <c r="A40" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>122</v>
@@ -3500,7 +3414,7 @@
     </row>
     <row r="41" spans="1:8">
       <c r="A41" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>122</v>
@@ -3522,7 +3436,7 @@
     </row>
     <row r="42" spans="1:8">
       <c r="A42" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>123</v>
@@ -3542,7 +3456,7 @@
     </row>
     <row r="43" spans="1:8">
       <c r="A43" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>130</v>
@@ -3564,7 +3478,7 @@
     </row>
     <row r="44" spans="1:8">
       <c r="A44" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>129</v>
@@ -3584,7 +3498,7 @@
     </row>
     <row r="45" spans="1:8">
       <c r="A45" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>129</v>
@@ -3604,7 +3518,7 @@
     </row>
     <row r="46" spans="1:8">
       <c r="A46" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>92</v>
@@ -3626,7 +3540,7 @@
     </row>
     <row r="47" spans="1:8">
       <c r="A47" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>93</v>
@@ -3638,7 +3552,7 @@
         <v>50</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F47" s="3"/>
       <c r="G47" s="3"/>
@@ -3646,7 +3560,7 @@
     </row>
     <row r="48" spans="1:8">
       <c r="A48" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>95</v>
@@ -3666,7 +3580,7 @@
     </row>
     <row r="49" spans="1:8">
       <c r="A49" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>92</v>
@@ -3688,7 +3602,7 @@
     </row>
     <row r="50" spans="1:8">
       <c r="A50" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>96</v>
@@ -3708,7 +3622,7 @@
     </row>
     <row r="51" spans="1:8">
       <c r="A51" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>96</v>
@@ -3730,7 +3644,7 @@
     </row>
     <row r="52" spans="1:8">
       <c r="A52" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B52" s="3" t="s">
         <v>97</v>
@@ -3750,7 +3664,7 @@
     </row>
     <row r="53" spans="1:8">
       <c r="A53" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B53" s="3" t="s">
         <v>98</v>
@@ -3762,7 +3676,7 @@
         <v>124</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F53" s="3"/>
       <c r="G53" s="3"/>
@@ -3770,7 +3684,7 @@
     </row>
     <row r="54" spans="1:8">
       <c r="A54" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B54" s="3" t="s">
         <v>99</v>
@@ -3792,7 +3706,7 @@
     </row>
     <row r="55" spans="1:8">
       <c r="A55" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B55" s="3" t="s">
         <v>100</v>
@@ -3804,7 +3718,7 @@
         <v>31</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F55" s="3"/>
       <c r="G55" s="3"/>
@@ -3824,8 +3738,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D61013C2-7F35-4D0B-B54C-3015EDB52E25}">
   <dimension ref="A1:I48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0" zoomScale="85" zoomScaleNormal="85">
-      <selection activeCell="F50" sqref="F50"/>
+    <sheetView tabSelected="1" workbookViewId="0" zoomScale="85" zoomScaleNormal="85">
+      <selection activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3838,41 +3752,42 @@
     <col min="6" max="6" customWidth="true" width="31.42578125" collapsed="true"/>
     <col min="7" max="7" customWidth="true" width="31.42578125" collapsed="true"/>
     <col min="8" max="8" bestFit="true" customWidth="true" width="7.85546875" collapsed="true"/>
+    <col min="9" max="16384" style="35" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="24"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="26"/>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="22" t="s">
-        <v>157</v>
-      </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="24"/>
+      <c r="A2" s="24" t="s">
+        <v>156</v>
+      </c>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="26"/>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="25"/>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
-      <c r="G3" s="26"/>
-      <c r="H3" s="27"/>
+      <c r="A3" s="27"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="29"/>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="4" t="s">
@@ -3894,15 +3809,15 @@
         <v>33</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H4" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row customFormat="1" r="5" s="33" spans="1:8">
+    <row r="5" spans="1:8">
       <c r="A5" s="16" t="s">
-        <v>269</v>
+        <v>281</v>
       </c>
       <c r="B5" s="16" t="s">
         <v>6</v>
@@ -3920,9 +3835,9 @@
       <c r="G5" s="16"/>
       <c r="H5" s="16"/>
     </row>
-    <row customFormat="1" r="6" s="33" spans="1:8">
+    <row r="6" spans="1:8">
       <c r="A6" s="16" t="s">
-        <v>269</v>
+        <v>281</v>
       </c>
       <c r="B6" s="16" t="s">
         <v>10</v>
@@ -3942,9 +3857,9 @@
       <c r="G6" s="16"/>
       <c r="H6" s="16"/>
     </row>
-    <row customFormat="1" r="7" s="33" spans="1:8">
+    <row r="7" spans="1:8">
       <c r="A7" s="16" t="s">
-        <v>269</v>
+        <v>281</v>
       </c>
       <c r="B7" s="16" t="s">
         <v>11</v>
@@ -3958,15 +3873,15 @@
       <c r="E7" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="F7" s="35">
+      <c r="F7" s="20">
         <v>5000</v>
       </c>
-      <c r="G7" s="35"/>
+      <c r="G7" s="20"/>
       <c r="H7" s="16"/>
     </row>
-    <row customFormat="1" r="8" s="33" spans="1:8">
+    <row r="8" spans="1:8">
       <c r="A8" s="16" t="s">
-        <v>269</v>
+        <v>281</v>
       </c>
       <c r="B8" s="16" t="s">
         <v>12</v>
@@ -3984,9 +3899,9 @@
       <c r="G8" s="16"/>
       <c r="H8" s="16"/>
     </row>
-    <row customFormat="1" r="9" s="33" spans="1:8">
+    <row r="9" spans="1:8">
       <c r="A9" s="16" t="s">
-        <v>269</v>
+        <v>281</v>
       </c>
       <c r="B9" s="16" t="s">
         <v>13</v>
@@ -4000,15 +3915,15 @@
       <c r="E9" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="F9" s="36" t="s">
+      <c r="F9" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="G9" s="36"/>
+      <c r="G9" s="21"/>
       <c r="H9" s="16"/>
     </row>
-    <row customFormat="1" r="10" s="33" spans="1:8">
+    <row r="10" spans="1:8">
       <c r="A10" s="16" t="s">
-        <v>269</v>
+        <v>281</v>
       </c>
       <c r="B10" s="16" t="s">
         <v>14</v>
@@ -4026,9 +3941,9 @@
       <c r="G10" s="16"/>
       <c r="H10" s="16"/>
     </row>
-    <row customFormat="1" r="11" s="33" spans="1:8">
+    <row r="11" spans="1:8">
       <c r="A11" s="16" t="s">
-        <v>269</v>
+        <v>281</v>
       </c>
       <c r="B11" s="16" t="s">
         <v>15</v>
@@ -4036,21 +3951,21 @@
       <c r="C11" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="D11" s="37" t="s">
+      <c r="D11" s="16" t="s">
         <v>31</v>
       </c>
       <c r="E11" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="F11" s="36" t="s">
+      <c r="F11" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="G11" s="36"/>
+      <c r="G11" s="21"/>
       <c r="H11" s="16"/>
     </row>
-    <row customFormat="1" r="12" s="33" spans="1:8">
+    <row r="12" spans="1:8">
       <c r="A12" s="16" t="s">
-        <v>269</v>
+        <v>281</v>
       </c>
       <c r="B12" s="16" t="s">
         <v>16</v>
@@ -4058,7 +3973,7 @@
       <c r="C12" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="37" t="s">
+      <c r="D12" s="16" t="s">
         <v>31</v>
       </c>
       <c r="E12" s="16" t="s">
@@ -4068,9 +3983,9 @@
       <c r="G12" s="16"/>
       <c r="H12" s="16"/>
     </row>
-    <row customFormat="1" r="13" s="33" spans="1:8">
+    <row r="13" spans="1:8">
       <c r="A13" s="16" t="s">
-        <v>269</v>
+        <v>281</v>
       </c>
       <c r="B13" s="16" t="s">
         <v>23</v>
@@ -4084,15 +3999,15 @@
       <c r="E13" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="F13" s="36" t="s">
+      <c r="F13" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="G13" s="36"/>
+      <c r="G13" s="21"/>
       <c r="H13" s="16"/>
     </row>
-    <row customFormat="1" r="14" s="33" spans="1:8">
+    <row r="14" spans="1:8">
       <c r="A14" s="16" t="s">
-        <v>269</v>
+        <v>281</v>
       </c>
       <c r="B14" s="16" t="s">
         <v>89</v>
@@ -4110,9 +4025,9 @@
       <c r="G14" s="16"/>
       <c r="H14" s="16"/>
     </row>
-    <row customFormat="1" r="15" s="33" spans="1:8">
+    <row r="15" spans="1:8">
       <c r="A15" s="16" t="s">
-        <v>269</v>
+        <v>281</v>
       </c>
       <c r="B15" s="16" t="s">
         <v>26</v>
@@ -4126,15 +4041,15 @@
       <c r="E15" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="F15" s="36" t="s">
+      <c r="F15" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="G15" s="36"/>
+      <c r="G15" s="21"/>
       <c r="H15" s="16"/>
     </row>
-    <row customFormat="1" r="16" s="33" spans="1:8">
+    <row r="16" spans="1:8">
       <c r="A16" s="16" t="s">
-        <v>269</v>
+        <v>281</v>
       </c>
       <c r="B16" s="16" t="s">
         <v>27</v>
@@ -4148,21 +4063,21 @@
       <c r="E16" s="16" t="s">
         <v>142</v>
       </c>
-      <c r="F16" s="36" t="s">
-        <v>143</v>
-      </c>
-      <c r="G16" s="36"/>
+      <c r="F16" s="21" t="s">
+        <v>284</v>
+      </c>
+      <c r="G16" s="21"/>
       <c r="H16" s="16"/>
     </row>
-    <row customFormat="1" r="17" s="33" spans="1:8">
+    <row r="17" spans="1:8">
       <c r="A17" s="16" t="s">
-        <v>269</v>
+        <v>281</v>
       </c>
       <c r="B17" s="16" t="s">
         <v>27</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D17" s="16" t="s">
         <v>31</v>
@@ -4170,15 +4085,15 @@
       <c r="E17" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="F17" s="36">
+      <c r="F17" s="21">
         <v>5000</v>
       </c>
-      <c r="G17" s="36"/>
+      <c r="G17" s="21"/>
       <c r="H17" s="16"/>
     </row>
-    <row customFormat="1" r="18" s="33" spans="1:8">
+    <row r="18" spans="1:8">
       <c r="A18" s="16" t="s">
-        <v>269</v>
+        <v>281</v>
       </c>
       <c r="B18" s="16" t="s">
         <v>27</v>
@@ -4196,9 +4111,9 @@
       <c r="G18" s="16"/>
       <c r="H18" s="16"/>
     </row>
-    <row customFormat="1" r="19" s="33" spans="1:8">
+    <row r="19" spans="1:8">
       <c r="A19" s="16" t="s">
-        <v>269</v>
+        <v>281</v>
       </c>
       <c r="B19" s="16" t="s">
         <v>28</v>
@@ -4213,14 +4128,14 @@
         <v>44</v>
       </c>
       <c r="F19" s="16" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="G19" s="16"/>
       <c r="H19" s="16"/>
     </row>
-    <row customFormat="1" r="20" s="33" spans="1:8">
+    <row r="20" spans="1:8">
       <c r="A20" s="16" t="s">
-        <v>269</v>
+        <v>281</v>
       </c>
       <c r="B20" s="16" t="s">
         <v>29</v>
@@ -4240,9 +4155,9 @@
       <c r="G20" s="16"/>
       <c r="H20" s="16"/>
     </row>
-    <row customFormat="1" r="21" s="33" spans="1:8">
+    <row r="21" spans="1:8">
       <c r="A21" s="16" t="s">
-        <v>269</v>
+        <v>281</v>
       </c>
       <c r="B21" s="16" t="s">
         <v>36</v>
@@ -4260,9 +4175,9 @@
       <c r="G21" s="16"/>
       <c r="H21" s="16"/>
     </row>
-    <row customFormat="1" r="22" s="33" spans="1:8">
+    <row r="22" spans="1:8">
       <c r="A22" s="16" t="s">
-        <v>269</v>
+        <v>281</v>
       </c>
       <c r="B22" s="16" t="s">
         <v>37</v>
@@ -4276,15 +4191,15 @@
       <c r="E22" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="F22" s="36">
+      <c r="F22" s="21">
         <v>3000</v>
       </c>
-      <c r="G22" s="36"/>
+      <c r="G22" s="21"/>
       <c r="H22" s="16"/>
     </row>
-    <row customFormat="1" r="23" s="33" spans="1:8">
+    <row r="23" spans="1:8">
       <c r="A23" s="16" t="s">
-        <v>269</v>
+        <v>281</v>
       </c>
       <c r="B23" s="16" t="s">
         <v>37</v>
@@ -4296,15 +4211,15 @@
         <v>108</v>
       </c>
       <c r="E23" s="16" t="s">
-        <v>148</v>
-      </c>
-      <c r="F23" s="36"/>
-      <c r="G23" s="36"/>
+        <v>147</v>
+      </c>
+      <c r="F23" s="21"/>
+      <c r="G23" s="21"/>
       <c r="H23" s="16"/>
     </row>
-    <row customFormat="1" r="24" s="33" spans="1:8">
+    <row r="24" spans="1:8">
       <c r="A24" s="16" t="s">
-        <v>269</v>
+        <v>281</v>
       </c>
       <c r="B24" s="16" t="s">
         <v>51</v>
@@ -4316,35 +4231,35 @@
         <v>139</v>
       </c>
       <c r="E24" s="16" t="s">
-        <v>148</v>
-      </c>
-      <c r="F24" s="36"/>
-      <c r="G24" s="36"/>
+        <v>147</v>
+      </c>
+      <c r="F24" s="21"/>
+      <c r="G24" s="21"/>
       <c r="H24" s="16"/>
     </row>
-    <row customFormat="1" r="25" s="33" spans="1:8">
+    <row r="25" spans="1:8">
       <c r="A25" s="16" t="s">
-        <v>269</v>
+        <v>281</v>
       </c>
       <c r="B25" s="16" t="s">
         <v>51</v>
       </c>
       <c r="C25" s="16" t="s">
+        <v>145</v>
+      </c>
+      <c r="D25" s="16" t="s">
         <v>146</v>
       </c>
-      <c r="D25" s="16" t="s">
-        <v>147</v>
-      </c>
       <c r="E25" s="16" t="s">
-        <v>149</v>
-      </c>
-      <c r="F25" s="36"/>
-      <c r="G25" s="36"/>
+        <v>148</v>
+      </c>
+      <c r="F25" s="21"/>
+      <c r="G25" s="21"/>
       <c r="H25" s="16"/>
     </row>
-    <row customFormat="1" r="26" s="33" spans="1:8">
+    <row r="26" spans="1:8">
       <c r="A26" s="16" t="s">
-        <v>269</v>
+        <v>281</v>
       </c>
       <c r="B26" s="16" t="s">
         <v>51</v>
@@ -4362,9 +4277,9 @@
       <c r="G26" s="16"/>
       <c r="H26" s="16"/>
     </row>
-    <row customFormat="1" r="27" s="33" spans="1:8">
+    <row r="27" spans="1:8">
       <c r="A27" s="16" t="s">
-        <v>269</v>
+        <v>281</v>
       </c>
       <c r="B27" s="16" t="s">
         <v>52</v>
@@ -4378,15 +4293,15 @@
       <c r="E27" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="F27" s="36">
+      <c r="F27" s="21">
         <v>3000</v>
       </c>
-      <c r="G27" s="36"/>
+      <c r="G27" s="21"/>
       <c r="H27" s="16"/>
     </row>
-    <row customFormat="1" r="28" s="34" spans="1:8">
+    <row r="28" spans="1:8">
       <c r="A28" s="16" t="s">
-        <v>269</v>
+        <v>281</v>
       </c>
       <c r="B28" s="16" t="s">
         <v>53</v>
@@ -4404,9 +4319,9 @@
       <c r="G28" s="16"/>
       <c r="H28" s="16"/>
     </row>
-    <row customFormat="1" r="29" s="33" spans="1:8">
+    <row r="29" spans="1:8">
       <c r="A29" s="16" t="s">
-        <v>269</v>
+        <v>281</v>
       </c>
       <c r="B29" s="16" t="s">
         <v>59</v>
@@ -4420,37 +4335,37 @@
       <c r="E29" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="F29" s="36">
+      <c r="F29" s="21">
         <v>8000</v>
       </c>
-      <c r="G29" s="36"/>
+      <c r="G29" s="21"/>
       <c r="H29" s="16"/>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="16" t="s">
-        <v>269</v>
+        <v>281</v>
       </c>
       <c r="B30" s="16" t="s">
         <v>60</v>
       </c>
       <c r="C30" s="16" t="s">
+        <v>270</v>
+      </c>
+      <c r="D30" s="16" t="s">
         <v>271</v>
       </c>
-      <c r="D30" s="16" t="s">
+      <c r="E30" s="16" t="s">
         <v>272</v>
       </c>
-      <c r="E30" s="16" t="s">
+      <c r="F30" s="21" t="s">
         <v>273</v>
       </c>
-      <c r="F30" s="36" t="s">
-        <v>274</v>
-      </c>
-      <c r="G30" s="36"/>
+      <c r="G30" s="21"/>
       <c r="H30" s="16"/>
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="16" t="s">
-        <v>269</v>
+        <v>281</v>
       </c>
       <c r="B31" s="16" t="s">
         <v>61</v>
@@ -4464,55 +4379,55 @@
       <c r="E31" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="F31" s="36">
+      <c r="F31" s="21">
         <v>8000</v>
       </c>
-      <c r="G31" s="36"/>
+      <c r="G31" s="21"/>
       <c r="H31" s="16"/>
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="16" t="s">
-        <v>269</v>
+        <v>281</v>
       </c>
       <c r="B32" s="16" t="s">
         <v>90</v>
       </c>
       <c r="C32" s="16" t="s">
+        <v>274</v>
+      </c>
+      <c r="D32" s="16" t="s">
         <v>275</v>
-      </c>
-      <c r="D32" s="16" t="s">
-        <v>276</v>
       </c>
       <c r="E32" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="F32" s="36"/>
-      <c r="G32" s="36"/>
+      <c r="F32" s="21"/>
+      <c r="G32" s="21"/>
       <c r="H32" s="16"/>
     </row>
     <row r="33" spans="1:8">
       <c r="A33" s="16" t="s">
-        <v>269</v>
+        <v>281</v>
       </c>
       <c r="B33" s="16" t="s">
         <v>91</v>
       </c>
       <c r="C33" s="16" t="s">
+        <v>276</v>
+      </c>
+      <c r="D33" s="16" t="s">
         <v>277</v>
-      </c>
-      <c r="D33" s="16" t="s">
-        <v>278</v>
       </c>
       <c r="E33" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="F33" s="36"/>
-      <c r="G33" s="36"/>
+      <c r="F33" s="21"/>
+      <c r="G33" s="21"/>
       <c r="H33" s="16"/>
     </row>
     <row r="34" spans="1:8">
       <c r="A34" s="16" t="s">
-        <v>269</v>
+        <v>281</v>
       </c>
       <c r="B34" s="16" t="s">
         <v>92</v>
@@ -4526,15 +4441,15 @@
       <c r="E34" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="F34" s="36">
+      <c r="F34" s="21">
         <v>3000</v>
       </c>
-      <c r="G34" s="36"/>
+      <c r="G34" s="21"/>
       <c r="H34" s="16"/>
     </row>
     <row r="35" spans="1:8">
       <c r="A35" s="16" t="s">
-        <v>269</v>
+        <v>281</v>
       </c>
       <c r="B35" s="16" t="s">
         <v>93</v>
@@ -4548,13 +4463,13 @@
       <c r="E35" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="F35" s="36"/>
-      <c r="G35" s="36"/>
+      <c r="F35" s="21"/>
+      <c r="G35" s="21"/>
       <c r="H35" s="16"/>
     </row>
     <row r="36" spans="1:8">
       <c r="A36" s="16" t="s">
-        <v>269</v>
+        <v>281</v>
       </c>
       <c r="B36" s="16" t="s">
         <v>94</v>
@@ -4568,15 +4483,15 @@
       <c r="E36" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="F36" s="36">
+      <c r="F36" s="21">
         <v>3000</v>
       </c>
-      <c r="G36" s="36"/>
+      <c r="G36" s="21"/>
       <c r="H36" s="16"/>
     </row>
     <row r="37" spans="1:8">
       <c r="A37" s="16" t="s">
-        <v>269</v>
+        <v>281</v>
       </c>
       <c r="B37" s="16" t="s">
         <v>95</v>
@@ -4590,13 +4505,13 @@
       <c r="E37" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="F37" s="36"/>
-      <c r="G37" s="36"/>
+      <c r="F37" s="21"/>
+      <c r="G37" s="21"/>
       <c r="H37" s="16"/>
     </row>
     <row r="38" spans="1:8">
       <c r="A38" s="16" t="s">
-        <v>269</v>
+        <v>281</v>
       </c>
       <c r="B38" s="16" t="s">
         <v>96</v>
@@ -4610,13 +4525,13 @@
       <c r="E38" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="F38" s="36"/>
-      <c r="G38" s="36"/>
+      <c r="F38" s="21"/>
+      <c r="G38" s="21"/>
       <c r="H38" s="16"/>
     </row>
     <row r="39" spans="1:8">
       <c r="A39" s="16" t="s">
-        <v>269</v>
+        <v>281</v>
       </c>
       <c r="B39" s="16" t="s">
         <v>97</v>
@@ -4630,15 +4545,15 @@
       <c r="E39" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="F39" s="36">
+      <c r="F39" s="21">
         <v>20000</v>
       </c>
-      <c r="G39" s="36"/>
+      <c r="G39" s="21"/>
       <c r="H39" s="16"/>
     </row>
     <row r="40" spans="1:8">
       <c r="A40" s="16" t="s">
-        <v>269</v>
+        <v>281</v>
       </c>
       <c r="B40" s="16" t="s">
         <v>98</v>
@@ -4650,15 +4565,15 @@
         <v>50</v>
       </c>
       <c r="E40" s="16" t="s">
-        <v>267</v>
-      </c>
-      <c r="F40" s="36"/>
-      <c r="G40" s="36"/>
+        <v>266</v>
+      </c>
+      <c r="F40" s="21"/>
+      <c r="G40" s="21"/>
       <c r="H40" s="16"/>
     </row>
     <row r="41" spans="1:8">
       <c r="A41" s="16" t="s">
-        <v>269</v>
+        <v>281</v>
       </c>
       <c r="B41" s="16" t="s">
         <v>99</v>
@@ -4672,13 +4587,13 @@
       <c r="E41" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="F41" s="36"/>
-      <c r="G41" s="36"/>
+      <c r="F41" s="21"/>
+      <c r="G41" s="21"/>
       <c r="H41" s="16"/>
     </row>
     <row r="42" spans="1:8">
       <c r="A42" s="16" t="s">
-        <v>269</v>
+        <v>281</v>
       </c>
       <c r="B42" s="16" t="s">
         <v>100</v>
@@ -4692,15 +4607,15 @@
       <c r="E42" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="F42" s="36">
+      <c r="F42" s="21">
         <v>10000</v>
       </c>
-      <c r="G42" s="36"/>
+      <c r="G42" s="21"/>
       <c r="H42" s="16"/>
     </row>
     <row r="43" spans="1:8">
       <c r="A43" s="16" t="s">
-        <v>269</v>
+        <v>281</v>
       </c>
       <c r="B43" s="16" t="s">
         <v>122</v>
@@ -4714,13 +4629,13 @@
       <c r="E43" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="F43" s="36"/>
-      <c r="G43" s="36"/>
+      <c r="F43" s="21"/>
+      <c r="G43" s="21"/>
       <c r="H43" s="16"/>
     </row>
     <row r="44" spans="1:8">
       <c r="A44" s="16" t="s">
-        <v>269</v>
+        <v>281</v>
       </c>
       <c r="B44" s="16" t="s">
         <v>123</v>
@@ -4734,15 +4649,15 @@
       <c r="E44" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="F44" s="36">
+      <c r="F44" s="21">
         <v>10000</v>
       </c>
-      <c r="G44" s="36"/>
+      <c r="G44" s="21"/>
       <c r="H44" s="16"/>
     </row>
     <row r="45" spans="1:8">
       <c r="A45" s="16" t="s">
-        <v>269</v>
+        <v>281</v>
       </c>
       <c r="B45" s="16" t="s">
         <v>129</v>
@@ -4756,16 +4671,16 @@
       <c r="E45" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="F45" s="36"/>
-      <c r="G45" s="36"/>
+      <c r="F45" s="21"/>
+      <c r="G45" s="21"/>
       <c r="H45" s="16"/>
     </row>
     <row r="46" spans="1:8">
       <c r="A46" s="16" t="s">
-        <v>269</v>
+        <v>281</v>
       </c>
       <c r="B46" s="16" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C46" s="16" t="s">
         <v>87</v>
@@ -4774,15 +4689,15 @@
         <v>124</v>
       </c>
       <c r="E46" s="16" t="s">
-        <v>267</v>
-      </c>
-      <c r="F46" s="36"/>
-      <c r="G46" s="36"/>
+        <v>266</v>
+      </c>
+      <c r="F46" s="21"/>
+      <c r="G46" s="21"/>
       <c r="H46" s="16"/>
     </row>
     <row r="47" spans="1:8">
       <c r="A47" s="16" t="s">
-        <v>269</v>
+        <v>281</v>
       </c>
       <c r="B47" s="16" t="s">
         <v>130</v>
@@ -4796,18 +4711,18 @@
       <c r="E47" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="F47" s="36">
+      <c r="F47" s="21">
         <v>30000</v>
       </c>
-      <c r="G47" s="36"/>
+      <c r="G47" s="21"/>
       <c r="H47" s="16"/>
     </row>
     <row r="48" spans="1:8">
       <c r="A48" s="16" t="s">
-        <v>269</v>
+        <v>281</v>
       </c>
       <c r="B48" s="16" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C48" s="16" t="s">
         <v>88</v>
@@ -4816,10 +4731,10 @@
         <v>31</v>
       </c>
       <c r="E48" s="16" t="s">
-        <v>228</v>
-      </c>
-      <c r="F48" s="36"/>
-      <c r="G48" s="36"/>
+        <v>227</v>
+      </c>
+      <c r="F48" s="21"/>
+      <c r="G48" s="21"/>
       <c r="H48" s="16"/>
     </row>
   </sheetData>
@@ -4838,7 +4753,7 @@
   <dimension ref="A1:I62"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:I21"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4850,40 +4765,39 @@
     <col min="5" max="5" customWidth="true" width="33.140625" collapsed="true"/>
     <col min="6" max="6" bestFit="true" customWidth="true" width="21.85546875" collapsed="true"/>
     <col min="7" max="7" customWidth="true" width="21.85546875" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="7.86328125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="22" t="s">
-        <v>161</v>
-      </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="24"/>
+      <c r="A1" s="24" t="s">
+        <v>160</v>
+      </c>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="26"/>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="22"/>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="24"/>
+      <c r="A2" s="24"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="26"/>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="25"/>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
-      <c r="G3" s="26"/>
-      <c r="H3" s="27"/>
+      <c r="A3" s="27"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="29"/>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="4" t="s">
@@ -4905,7 +4819,7 @@
         <v>33</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H4" s="4" t="s">
         <v>3</v>
@@ -4913,7 +4827,7 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>6</v>
@@ -4931,13 +4845,11 @@
         <v>31</v>
       </c>
       <c r="G5" s="3"/>
-      <c r="H5" s="3" t="s">
-        <v>285</v>
-      </c>
+      <c r="H5" s="3"/>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>10</v>
@@ -4955,13 +4867,11 @@
         <v>31</v>
       </c>
       <c r="G6" s="3"/>
-      <c r="H6" s="3" t="s">
-        <v>285</v>
-      </c>
+      <c r="H6" s="3"/>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>11</v>
@@ -4979,13 +4889,11 @@
         <v>56</v>
       </c>
       <c r="G7" s="6"/>
-      <c r="H7" s="3" t="s">
-        <v>285</v>
-      </c>
+      <c r="H7" s="3"/>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>12</v>
@@ -5001,13 +4909,11 @@
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
-      <c r="H8" s="3" t="s">
-        <v>285</v>
-      </c>
+      <c r="H8" s="3"/>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>13</v>
@@ -5025,13 +4931,11 @@
         <v>57</v>
       </c>
       <c r="G9" s="7"/>
-      <c r="H9" s="3" t="s">
-        <v>285</v>
-      </c>
+      <c r="H9" s="3"/>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>14</v>
@@ -5047,13 +4951,11 @@
       </c>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
-      <c r="H10" s="3" t="s">
-        <v>285</v>
-      </c>
+      <c r="H10" s="3"/>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>15</v>
@@ -5071,13 +4973,11 @@
         <v>62</v>
       </c>
       <c r="G11" s="7"/>
-      <c r="H11" s="3" t="s">
-        <v>285</v>
-      </c>
+      <c r="H11" s="3"/>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>16</v>
@@ -5089,19 +4989,17 @@
         <v>31</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F12" s="3">
         <v>2</v>
       </c>
       <c r="G12" s="3"/>
-      <c r="H12" s="3" t="s">
-        <v>285</v>
-      </c>
+      <c r="H12" s="3"/>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>23</v>
@@ -5119,125 +5017,113 @@
         <v>62</v>
       </c>
       <c r="G13" s="7"/>
-      <c r="H13" s="3" t="s">
-        <v>285</v>
-      </c>
+      <c r="H13" s="3"/>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>89</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>43</v>
       </c>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
-      <c r="H14" s="3" t="s">
-        <v>285</v>
-      </c>
+      <c r="H14" s="3"/>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>89</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>31</v>
       </c>
       <c r="E15" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="F15" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="F15" s="3" t="s">
-        <v>200</v>
-      </c>
       <c r="G15" s="7"/>
-      <c r="H15" s="3" t="s">
-        <v>285</v>
-      </c>
+      <c r="H15" s="3"/>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>26</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>43</v>
       </c>
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
-      <c r="H16" s="3" t="s">
-        <v>285</v>
-      </c>
+      <c r="H16" s="3"/>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>27</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>43</v>
       </c>
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
-      <c r="H17" s="3" t="s">
-        <v>285</v>
-      </c>
+      <c r="H17" s="3"/>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>27</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>31</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F18" s="7"/>
       <c r="G18" s="7"/>
-      <c r="H18" s="3" t="s">
-        <v>285</v>
-      </c>
+      <c r="H18" s="3"/>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>89</v>
@@ -5253,13 +5139,11 @@
       </c>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
-      <c r="H19" s="3" t="s">
-        <v>285</v>
-      </c>
+      <c r="H19" s="3"/>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>26</v>
@@ -5277,13 +5161,11 @@
         <v>62</v>
       </c>
       <c r="G20" s="7"/>
-      <c r="H20" s="3" t="s">
-        <v>285</v>
-      </c>
+      <c r="H20" s="3"/>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>26</v>
@@ -5295,19 +5177,17 @@
         <v>31</v>
       </c>
       <c r="E21" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="F21" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="F21" s="3" t="s">
-        <v>200</v>
-      </c>
       <c r="G21" s="7"/>
-      <c r="H21" s="3" t="s">
-        <v>285</v>
-      </c>
+      <c r="H21" s="3"/>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>27</v>
@@ -5322,22 +5202,20 @@
         <v>142</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>143</v>
+        <v>284</v>
       </c>
       <c r="G22" s="7"/>
-      <c r="H22" s="3" t="s">
-        <v>286</v>
-      </c>
+      <c r="H22" s="3"/>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>27</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>31</v>
@@ -5349,13 +5227,11 @@
         <v>5000</v>
       </c>
       <c r="G23" s="7"/>
-      <c r="H23" s="3" t="s">
-        <v>285</v>
-      </c>
+      <c r="H23" s="3"/>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>27</v>
@@ -5371,13 +5247,11 @@
       </c>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
-      <c r="H24" s="3" t="s">
-        <v>286</v>
-      </c>
+      <c r="H24" s="3"/>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>28</v>
@@ -5392,16 +5266,14 @@
         <v>44</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G25" s="3"/>
-      <c r="H25" s="3" t="s">
-        <v>286</v>
-      </c>
+      <c r="H25" s="3"/>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>29</v>
@@ -5416,16 +5288,14 @@
         <v>44</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G26" s="3"/>
-      <c r="H26" s="3" t="s">
-        <v>286</v>
-      </c>
+      <c r="H26" s="3"/>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>36</v>
@@ -5441,13 +5311,11 @@
       </c>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
-      <c r="H27" s="3" t="s">
-        <v>286</v>
-      </c>
+      <c r="H27" s="3"/>
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>37</v>
@@ -5465,13 +5333,11 @@
         <v>3000</v>
       </c>
       <c r="G28" s="7"/>
-      <c r="H28" s="3" t="s">
-        <v>285</v>
-      </c>
+      <c r="H28" s="3"/>
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>51</v>
@@ -5483,7 +5349,7 @@
         <v>108</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F29" s="7"/>
       <c r="G29" s="7"/>
@@ -5491,7 +5357,7 @@
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>52</v>
@@ -5503,7 +5369,7 @@
         <v>139</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F30" s="7"/>
       <c r="G30" s="7"/>
@@ -5511,19 +5377,19 @@
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>53</v>
       </c>
       <c r="C31" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="D31" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="D31" s="3" t="s">
-        <v>147</v>
-      </c>
       <c r="E31" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F31" s="7"/>
       <c r="G31" s="7"/>
@@ -5531,16 +5397,16 @@
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>59</v>
       </c>
       <c r="C32" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="D32" s="3" t="s">
         <v>163</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>164</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>43</v>
@@ -5551,41 +5417,41 @@
     </row>
     <row r="33" spans="1:8">
       <c r="A33" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>60</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E33" s="3" t="s">
         <v>44</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G33" s="7"/>
       <c r="H33" s="3"/>
     </row>
     <row r="34" spans="1:8">
       <c r="A34" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>61</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F34" s="7"/>
       <c r="G34" s="7"/>
@@ -5593,29 +5459,29 @@
     </row>
     <row r="35" spans="1:8">
       <c r="A35" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>90</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D35" s="3" t="s">
         <v>31</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G35" s="7"/>
       <c r="H35" s="3"/>
     </row>
     <row r="36" spans="1:8">
       <c r="A36" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>91</v>
@@ -5635,7 +5501,7 @@
     </row>
     <row r="37" spans="1:8">
       <c r="A37" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>37</v>
@@ -5657,7 +5523,7 @@
     </row>
     <row r="38" spans="1:8">
       <c r="A38" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>60</v>
@@ -5677,7 +5543,7 @@
     </row>
     <row r="39" spans="1:8">
       <c r="A39" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>61</v>
@@ -5697,7 +5563,7 @@
     </row>
     <row r="40" spans="1:8">
       <c r="A40" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>90</v>
@@ -5712,14 +5578,14 @@
         <v>44</v>
       </c>
       <c r="F40" s="9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G40" s="9"/>
       <c r="H40" s="9"/>
     </row>
     <row r="41" spans="1:8">
       <c r="A41" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>91</v>
@@ -5734,14 +5600,14 @@
         <v>44</v>
       </c>
       <c r="F41" s="9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G41" s="9"/>
       <c r="H41" s="9"/>
     </row>
     <row r="42" spans="1:8">
       <c r="A42" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>92</v>
@@ -5763,7 +5629,7 @@
     </row>
     <row r="43" spans="1:8">
       <c r="A43" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>93</v>
@@ -5785,7 +5651,7 @@
     </row>
     <row r="44" spans="1:8">
       <c r="A44" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>96</v>
@@ -5805,7 +5671,7 @@
     </row>
     <row r="45" spans="1:8">
       <c r="A45" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>96</v>
@@ -5814,7 +5680,7 @@
         <v>126</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E45" s="3" t="s">
         <v>43</v>
@@ -5825,7 +5691,7 @@
     </row>
     <row r="46" spans="1:8">
       <c r="A46" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>97</v>
@@ -5834,20 +5700,20 @@
         <v>127</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E46" s="3" t="s">
         <v>119</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G46" s="3"/>
       <c r="H46" s="9"/>
     </row>
     <row r="47" spans="1:8">
       <c r="A47" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>97</v>
@@ -5856,7 +5722,7 @@
         <v>128</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E47" s="3" t="s">
         <v>43</v>
@@ -5867,7 +5733,7 @@
     </row>
     <row r="48" spans="1:8">
       <c r="A48" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>99</v>
@@ -5876,20 +5742,20 @@
         <v>135</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E48" s="3" t="s">
         <v>119</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G48" s="3"/>
       <c r="H48" s="9"/>
     </row>
     <row r="49" spans="1:8">
       <c r="A49" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>122</v>
@@ -5909,13 +5775,13 @@
     </row>
     <row r="50" spans="1:8">
       <c r="A50" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>129</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D50" s="3" t="s">
         <v>31</v>
@@ -5931,13 +5797,13 @@
     </row>
     <row r="51" spans="1:8">
       <c r="A51" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>130</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D51" s="3" t="s">
         <v>46</v>
@@ -5951,31 +5817,31 @@
     </row>
     <row r="52" spans="1:8">
       <c r="A52" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B52" s="3" t="s">
         <v>122</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D52" s="3" t="s">
         <v>31</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F52" s="9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G52" s="9" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H52" s="9"/>
     </row>
     <row r="53" spans="1:8">
       <c r="A53" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B53" s="13" t="s">
         <v>129</v>
@@ -5995,7 +5861,7 @@
     </row>
     <row r="54" spans="1:8">
       <c r="A54" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B54" s="3" t="s">
         <v>129</v>
@@ -6015,7 +5881,7 @@
     </row>
     <row r="55" spans="1:8">
       <c r="A55" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B55" s="3" t="s">
         <v>92</v>
@@ -6037,7 +5903,7 @@
     </row>
     <row r="56" spans="1:8">
       <c r="A56" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B56" s="3" t="s">
         <v>93</v>
@@ -6049,7 +5915,7 @@
         <v>50</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F56" s="3"/>
       <c r="G56" s="3"/>
@@ -6057,7 +5923,7 @@
     </row>
     <row r="57" spans="1:8">
       <c r="A57" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B57" s="3" t="s">
         <v>96</v>
@@ -6079,7 +5945,7 @@
     </row>
     <row r="58" spans="1:8">
       <c r="A58" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B58" s="3" t="s">
         <v>98</v>
@@ -6091,7 +5957,7 @@
         <v>124</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F58" s="3"/>
       <c r="G58" s="3"/>
@@ -6099,7 +5965,7 @@
     </row>
     <row r="59" spans="1:8">
       <c r="A59" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B59" s="3" t="s">
         <v>99</v>
@@ -6121,13 +5987,13 @@
     </row>
     <row r="60" spans="1:8">
       <c r="A60" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B60" s="3" t="s">
         <v>99</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D60" s="3" t="s">
         <v>68</v>
@@ -6136,38 +6002,38 @@
         <v>69</v>
       </c>
       <c r="F60" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G60" s="3"/>
       <c r="H60" s="9"/>
     </row>
     <row r="61" spans="1:8">
       <c r="A61" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B61" s="3" t="s">
         <v>99</v>
       </c>
       <c r="C61" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E61" s="3" t="s">
         <v>189</v>
-      </c>
-      <c r="D61" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E61" s="3" t="s">
-        <v>190</v>
       </c>
       <c r="F61" s="3">
         <v>123458</v>
       </c>
       <c r="G61" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H61" s="9"/>
     </row>
     <row r="62" spans="1:8">
       <c r="A62" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B62" s="3" t="s">
         <v>100</v>
@@ -6179,7 +6045,7 @@
         <v>31</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F62" s="3"/>
       <c r="G62" s="3"/>
@@ -6217,36 +6083,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="22" t="s">
-        <v>202</v>
-      </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="24"/>
+      <c r="A1" s="24" t="s">
+        <v>201</v>
+      </c>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="26"/>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="22"/>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="24"/>
+      <c r="A2" s="24"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="26"/>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="25"/>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
-      <c r="G3" s="26"/>
-      <c r="H3" s="27"/>
+      <c r="A3" s="27"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="29"/>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="4" t="s">
@@ -6268,7 +6134,7 @@
         <v>33</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H4" s="4" t="s">
         <v>3</v>
@@ -6276,7 +6142,7 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>6</v>
@@ -6298,7 +6164,7 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>10</v>
@@ -6320,7 +6186,7 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>11</v>
@@ -6342,38 +6208,38 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>44</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>43</v>
@@ -6384,16 +6250,16 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C10" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>212</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>213</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>43</v>
@@ -6404,38 +6270,38 @@
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C11" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="F11" s="3" t="s">
         <v>217</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>218</v>
       </c>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>43</v>
@@ -6446,16 +6312,16 @@
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C13" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>215</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>216</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>43</v>
@@ -6466,7 +6332,7 @@
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>16</v>
@@ -6486,7 +6352,7 @@
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>23</v>
@@ -6508,38 +6374,38 @@
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>119</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G16" s="7"/>
       <c r="H16" s="3"/>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C17" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="D17" s="3" t="s">
         <v>222</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>223</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>43</v>
@@ -6550,7 +6416,7 @@
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>11</v>
@@ -6572,19 +6438,19 @@
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>31</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F19" s="3">
         <v>3</v>
@@ -6594,19 +6460,19 @@
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>31</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F20" s="3"/>
       <c r="G20" s="7"/>
@@ -6614,19 +6480,19 @@
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>31</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F21" s="7">
         <v>2</v>
@@ -6636,19 +6502,19 @@
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>31</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F22" s="7"/>
       <c r="G22" s="7"/>
@@ -6656,19 +6522,19 @@
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>31</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F23" s="7">
         <v>1</v>
@@ -6678,16 +6544,16 @@
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C24" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="D24" s="3" t="s">
         <v>230</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>231</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>43</v>
@@ -6698,19 +6564,19 @@
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C25" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="E25" s="3" t="s">
         <v>233</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>232</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>234</v>
       </c>
       <c r="F25" s="7"/>
       <c r="G25" s="7"/>
@@ -6718,19 +6584,19 @@
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C26" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="D26" s="3" t="s">
         <v>235</v>
       </c>
-      <c r="D26" s="3" t="s">
-        <v>236</v>
-      </c>
       <c r="E26" s="3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F26" s="7"/>
       <c r="G26" s="7"/>
@@ -6738,16 +6604,16 @@
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C27" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="D27" s="3" t="s">
         <v>237</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>238</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>43</v>
@@ -6758,19 +6624,19 @@
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>31</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F28" s="7">
         <v>2</v>
@@ -6780,19 +6646,19 @@
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>31</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
@@ -6800,38 +6666,38 @@
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>31</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G30" s="3"/>
       <c r="H30" s="3"/>
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C31" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="D31" s="3" t="s">
         <v>241</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>242</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>43</v>
@@ -6842,19 +6708,19 @@
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D32" s="17" t="s">
         <v>31</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F32" s="3"/>
       <c r="G32" s="3"/>
@@ -6862,38 +6728,38 @@
     </row>
     <row r="33" spans="1:8">
       <c r="A33" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C33" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="D33" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="F33" s="3" t="s">
         <v>256</v>
-      </c>
-      <c r="D33" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="F33" s="3" t="s">
-        <v>257</v>
       </c>
       <c r="G33" s="3"/>
       <c r="H33" s="3"/>
     </row>
     <row r="34" spans="1:8">
       <c r="A34" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C34" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="D34" s="3" t="s">
         <v>243</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>244</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>43</v>
@@ -6904,16 +6770,16 @@
     </row>
     <row r="35" spans="1:8">
       <c r="A35" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C35" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="D35" s="3" t="s">
         <v>245</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>246</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>43</v>
@@ -6924,13 +6790,13 @@
     </row>
     <row r="36" spans="1:8">
       <c r="A36" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>31</v>
@@ -6946,19 +6812,19 @@
     </row>
     <row r="37" spans="1:8">
       <c r="A37" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D37" s="3" t="s">
         <v>31</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F37" s="7"/>
       <c r="G37" s="7"/>
@@ -6966,13 +6832,13 @@
     </row>
     <row r="38" spans="1:8">
       <c r="A38" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D38" s="3" t="s">
         <v>31</v>
@@ -6988,41 +6854,41 @@
     </row>
     <row r="39" spans="1:8">
       <c r="A39" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>31</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="G39" s="7"/>
       <c r="H39" s="3"/>
     </row>
     <row r="40" spans="1:8">
       <c r="A40" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C40" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="E40" s="3" t="s">
         <v>249</v>
-      </c>
-      <c r="D40" s="3" t="s">
-        <v>248</v>
-      </c>
-      <c r="E40" s="3" t="s">
-        <v>250</v>
       </c>
       <c r="F40" s="7"/>
       <c r="G40" s="7"/>
@@ -7030,16 +6896,16 @@
     </row>
     <row r="41" spans="1:8">
       <c r="A41" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C41" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="D41" s="3" t="s">
         <v>251</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>252</v>
       </c>
       <c r="E41" s="3" t="s">
         <v>43</v>
@@ -7050,19 +6916,19 @@
     </row>
     <row r="42" spans="1:8">
       <c r="A42" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D42" s="3" t="s">
         <v>31</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F42" s="3"/>
       <c r="G42" s="7"/>
@@ -7070,41 +6936,41 @@
     </row>
     <row r="43" spans="1:8">
       <c r="A43" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C43" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="F43" s="3" t="s">
         <v>260</v>
-      </c>
-      <c r="D43" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E43" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="F43" s="3" t="s">
-        <v>261</v>
       </c>
       <c r="G43" s="7"/>
       <c r="H43" s="3"/>
     </row>
     <row r="44" spans="1:8">
       <c r="A44" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C44" s="16" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D44" s="16" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E44" s="16" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F44" s="9"/>
       <c r="G44" s="9"/>
@@ -7141,36 +7007,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="28"/>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="30"/>
+      <c r="A1" s="30"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="32"/>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="28"/>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="30"/>
+      <c r="A2" s="30"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="32"/>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="31"/>
-      <c r="B3" s="31"/>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="31" t="s">
+      <c r="A3" s="33"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33" t="s">
         <v>81</v>
       </c>
-      <c r="G3" s="31"/>
-      <c r="H3" s="32"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="34"/>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="4" t="s">
@@ -7196,7 +7062,7 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>82</v>
@@ -7213,7 +7079,7 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>85</v>
@@ -7230,7 +7096,7 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>82</v>
@@ -7239,7 +7105,7 @@
         <v>83</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E7" s="8" t="s">
         <v>86</v>
@@ -7247,7 +7113,7 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>85</v>
@@ -7264,16 +7130,16 @@
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E9" s="8" t="s">
         <v>86</v>
@@ -7281,19 +7147,19 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="16" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B10" s="8" t="s">
         <v>82</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
   </sheetData>
@@ -7324,7 +7190,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -7332,7 +7198,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Made changes in test data , driverengine and test method
</commit_message>
<xml_diff>
--- a/TestDataAndResults/Run1/SophieAutomation.xlsx
+++ b/TestDataAndResults/Run1/SophieAutomation.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr documentId="13_ncr:1_{9F2F17D2-DEBD-4FDB-88DC-8ECCBA13A062}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43"/>
+  <xr:revisionPtr documentId="13_ncr:1_{AC3BCE6A-6F26-4D65-ACCD-2DB08400D9FD}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43"/>
   <bookViews>
-    <workbookView activeTab="4" firstSheet="1" windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
+    <workbookView activeTab="1" firstSheet="1" windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" r:id="rId1" sheetId="8"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1347" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1380" uniqueCount="288">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -891,7 +891,13 @@
     <t>23.218.94.2.NA.01-01-01</t>
   </si>
   <si>
+    <t>PegaGadget2Ifr</t>
+  </si>
+  <si>
     <t>Pass</t>
+  </si>
+  <si>
+    <t>Fail</t>
   </si>
 </sst>
 </file>
@@ -934,7 +940,7 @@
       <name val="Calibiri"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -956,6 +962,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1067,7 +1079,7 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
     <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
@@ -1092,6 +1104,7 @@
     <xf applyBorder="1" applyFont="1" borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" applyFill="1" borderId="1" fillId="0" fontId="3" numFmtId="0" quotePrefix="1" xfId="1"/>
     <xf applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="0" fontId="2" numFmtId="0" quotePrefix="1" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="2" fillId="3" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
@@ -1131,7 +1144,7 @@
     <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="7" fillId="3" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyFill="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="5" fontId="2" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
@@ -1500,8 +1513,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1515,22 +1528,22 @@
   </cols>
   <sheetData>
     <row customFormat="1" ht="14.25" r="1" s="5" spans="1:5">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
     </row>
     <row customFormat="1" ht="14.25" r="2" s="5" spans="1:5">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="24" t="s">
         <v>132</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
     </row>
     <row customFormat="1" ht="14.25" r="3" s="5" spans="1:5">
       <c r="A3" s="10"/>
@@ -1567,7 +1580,7 @@
         <v>32</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="E5" s="3"/>
     </row>
@@ -1582,7 +1595,7 @@
         <v>101</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="E6" s="3"/>
     </row>
@@ -1597,7 +1610,7 @@
         <v>184</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="E7" s="3"/>
     </row>
@@ -1644,8 +1657,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32EA4E71-0B53-4881-A15A-C454293CD34C}">
   <dimension ref="A1:I44"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1657,42 +1670,42 @@
     <col min="5" max="5" customWidth="true" width="32.5703125" collapsed="true"/>
     <col min="6" max="6" customWidth="true" width="31.42578125" collapsed="true"/>
     <col min="7" max="7" customWidth="true" width="31.42578125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="7.86328125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="7.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="26"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="27"/>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="25" t="s">
         <v>156</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="26"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="27"/>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="27"/>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
-      <c r="H3" s="29"/>
+      <c r="A3" s="28"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="30"/>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="18" t="s">
@@ -1740,9 +1753,7 @@
         <v>31</v>
       </c>
       <c r="G5" s="9"/>
-      <c r="H5" s="3" t="s">
-        <v>285</v>
-      </c>
+      <c r="H5" s="3"/>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
@@ -1764,9 +1775,7 @@
         <v>31</v>
       </c>
       <c r="G6" s="9"/>
-      <c r="H6" s="3" t="s">
-        <v>285</v>
-      </c>
+      <c r="H6" s="3"/>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
@@ -1788,9 +1797,7 @@
         <v>5000</v>
       </c>
       <c r="G7" s="9"/>
-      <c r="H7" s="3" t="s">
-        <v>285</v>
-      </c>
+      <c r="H7" s="3"/>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
@@ -2413,8 +2420,8 @@
       <c r="D37" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="E37" s="3" t="s">
-        <v>43</v>
+      <c r="E37" s="36" t="s">
+        <v>266</v>
       </c>
       <c r="F37" s="3"/>
       <c r="G37" s="3"/>
@@ -2455,8 +2462,8 @@
       <c r="D39" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="E39" s="3" t="s">
-        <v>43</v>
+      <c r="E39" s="36" t="s">
+        <v>266</v>
       </c>
       <c r="F39" s="3"/>
       <c r="G39" s="3"/>
@@ -2582,7 +2589,7 @@
   <dimension ref="A1:I55"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="E16" sqref="E16:F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2595,38 +2602,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="26"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="27"/>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="25" t="s">
         <v>156</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="26"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="27"/>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="27"/>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
-      <c r="H3" s="29"/>
+      <c r="A3" s="28"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="30"/>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="4" t="s">
@@ -3571,8 +3578,8 @@
       <c r="D48" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="E48" s="3" t="s">
-        <v>43</v>
+      <c r="E48" s="36" t="s">
+        <v>266</v>
       </c>
       <c r="F48" s="3"/>
       <c r="G48" s="3"/>
@@ -3613,8 +3620,8 @@
       <c r="D50" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="E50" s="3" t="s">
-        <v>43</v>
+      <c r="E50" s="36" t="s">
+        <v>266</v>
       </c>
       <c r="F50" s="3"/>
       <c r="G50" s="3"/>
@@ -3736,10 +3743,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D61013C2-7F35-4D0B-B54C-3015EDB52E25}">
-  <dimension ref="A1:I48"/>
+  <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" zoomScale="85" zoomScaleNormal="85">
-      <selection activeCell="P12" sqref="P12"/>
+    <sheetView workbookViewId="0" zoomScale="85" zoomScaleNormal="85">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3751,43 +3758,43 @@
     <col min="5" max="5" customWidth="true" width="32.5703125" collapsed="true"/>
     <col min="6" max="6" customWidth="true" width="31.42578125" collapsed="true"/>
     <col min="7" max="7" customWidth="true" width="31.42578125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="7.85546875" collapsed="true"/>
-    <col min="9" max="16384" style="35" width="9.140625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="7.86328125" collapsed="true"/>
+    <col min="9" max="16384" style="22" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="26"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="27"/>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="25" t="s">
         <v>156</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="26"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="27"/>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="27"/>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
-      <c r="H3" s="29"/>
+      <c r="A3" s="28"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="30"/>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="4" t="s">
@@ -3833,7 +3840,9 @@
       </c>
       <c r="F5" s="16"/>
       <c r="G5" s="16"/>
-      <c r="H5" s="16"/>
+      <c r="H5" s="16" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="16" t="s">
@@ -3855,7 +3864,9 @@
         <v>31</v>
       </c>
       <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
+      <c r="H6" s="16" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="16" t="s">
@@ -3877,7 +3888,9 @@
         <v>5000</v>
       </c>
       <c r="G7" s="20"/>
-      <c r="H7" s="16"/>
+      <c r="H7" s="16" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="16" t="s">
@@ -3897,7 +3910,9 @@
       </c>
       <c r="F8" s="16"/>
       <c r="G8" s="16"/>
-      <c r="H8" s="16"/>
+      <c r="H8" s="16" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="16" t="s">
@@ -3919,7 +3934,9 @@
         <v>57</v>
       </c>
       <c r="G9" s="21"/>
-      <c r="H9" s="16"/>
+      <c r="H9" s="16" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="16" t="s">
@@ -3939,7 +3956,9 @@
       </c>
       <c r="F10" s="16"/>
       <c r="G10" s="16"/>
-      <c r="H10" s="16"/>
+      <c r="H10" s="16" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="16" t="s">
@@ -3961,7 +3980,9 @@
         <v>62</v>
       </c>
       <c r="G11" s="21"/>
-      <c r="H11" s="16"/>
+      <c r="H11" s="16" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="16" t="s">
@@ -3981,7 +4002,9 @@
       </c>
       <c r="F12" s="16"/>
       <c r="G12" s="16"/>
-      <c r="H12" s="16"/>
+      <c r="H12" s="16" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="16" t="s">
@@ -4003,7 +4026,9 @@
         <v>62</v>
       </c>
       <c r="G13" s="21"/>
-      <c r="H13" s="16"/>
+      <c r="H13" s="16" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="16" t="s">
@@ -4023,7 +4048,9 @@
       </c>
       <c r="F14" s="16"/>
       <c r="G14" s="16"/>
-      <c r="H14" s="16"/>
+      <c r="H14" s="16" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="16" t="s">
@@ -4045,29 +4072,33 @@
         <v>62</v>
       </c>
       <c r="G15" s="21"/>
-      <c r="H15" s="16"/>
+      <c r="H15" s="16" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="16" t="s">
         <v>281</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C16" s="16" t="s">
-        <v>141</v>
+        <v>54</v>
       </c>
       <c r="D16" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="E16" s="16" t="s">
-        <v>142</v>
-      </c>
-      <c r="F16" s="21" t="s">
-        <v>284</v>
+      <c r="E16" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>199</v>
       </c>
       <c r="G16" s="21"/>
-      <c r="H16" s="16"/>
+      <c r="H16" s="16" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="16" t="s">
@@ -4077,19 +4108,21 @@
         <v>27</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D17" s="16" t="s">
         <v>31</v>
       </c>
       <c r="E17" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="F17" s="21">
-        <v>5000</v>
+        <v>142</v>
+      </c>
+      <c r="F17" s="21" t="s">
+        <v>284</v>
       </c>
       <c r="G17" s="21"/>
-      <c r="H17" s="16"/>
+      <c r="H17" s="16" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="16" t="s">
@@ -4099,103 +4132,113 @@
         <v>27</v>
       </c>
       <c r="C18" s="16" t="s">
-        <v>21</v>
+        <v>143</v>
       </c>
       <c r="D18" s="16" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="E18" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="F18" s="16"/>
-      <c r="G18" s="16"/>
-      <c r="H18" s="16"/>
+        <v>55</v>
+      </c>
+      <c r="F18" s="21">
+        <v>5000</v>
+      </c>
+      <c r="G18" s="21"/>
+      <c r="H18" s="16" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="16" t="s">
         <v>281</v>
       </c>
       <c r="B19" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C19" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D19" s="16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E19" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="F19" s="16" t="s">
-        <v>269</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="F19" s="16"/>
       <c r="G19" s="16"/>
-      <c r="H19" s="16"/>
+      <c r="H19" s="16" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="16" t="s">
         <v>281</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C20" s="16" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D20" s="16" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="E20" s="16" t="s">
         <v>44</v>
       </c>
       <c r="F20" s="16" t="s">
-        <v>65</v>
+        <v>269</v>
       </c>
       <c r="G20" s="16"/>
-      <c r="H20" s="16"/>
+      <c r="H20" s="16" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="16" t="s">
         <v>281</v>
       </c>
       <c r="B21" s="16" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="C21" s="16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D21" s="16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E21" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="F21" s="16"/>
+        <v>44</v>
+      </c>
+      <c r="F21" s="16" t="s">
+        <v>65</v>
+      </c>
       <c r="G21" s="16"/>
-      <c r="H21" s="16"/>
+      <c r="H21" s="16" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="16" t="s">
         <v>281</v>
       </c>
       <c r="B22" s="16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C22" s="16" t="s">
-        <v>54</v>
+        <v>25</v>
       </c>
       <c r="D22" s="16" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="E22" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="F22" s="21">
-        <v>3000</v>
-      </c>
-      <c r="G22" s="21"/>
-      <c r="H22" s="16"/>
+        <v>43</v>
+      </c>
+      <c r="F22" s="16"/>
+      <c r="G22" s="16"/>
+      <c r="H22" s="16" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="16" t="s">
@@ -4205,37 +4248,43 @@
         <v>37</v>
       </c>
       <c r="C23" s="16" t="s">
-        <v>103</v>
+        <v>54</v>
       </c>
       <c r="D23" s="16" t="s">
-        <v>108</v>
+        <v>31</v>
       </c>
       <c r="E23" s="16" t="s">
-        <v>147</v>
-      </c>
-      <c r="F23" s="21"/>
+        <v>55</v>
+      </c>
+      <c r="F23" s="21">
+        <v>3000</v>
+      </c>
       <c r="G23" s="21"/>
-      <c r="H23" s="16"/>
+      <c r="H23" s="16" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="16" t="s">
         <v>281</v>
       </c>
       <c r="B24" s="16" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="C24" s="16" t="s">
-        <v>140</v>
+        <v>103</v>
       </c>
       <c r="D24" s="16" t="s">
-        <v>139</v>
+        <v>108</v>
       </c>
       <c r="E24" s="16" t="s">
         <v>147</v>
       </c>
       <c r="F24" s="21"/>
       <c r="G24" s="21"/>
-      <c r="H24" s="16"/>
+      <c r="H24" s="16" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="16" t="s">
@@ -4245,17 +4294,19 @@
         <v>51</v>
       </c>
       <c r="C25" s="16" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="D25" s="16" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="E25" s="16" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F25" s="21"/>
       <c r="G25" s="21"/>
-      <c r="H25" s="16"/>
+      <c r="H25" s="16" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="16" t="s">
@@ -4265,122 +4316,130 @@
         <v>51</v>
       </c>
       <c r="C26" s="16" t="s">
-        <v>25</v>
+        <v>145</v>
       </c>
       <c r="D26" s="16" t="s">
-        <v>46</v>
+        <v>146</v>
       </c>
       <c r="E26" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="F26" s="16"/>
-      <c r="G26" s="16"/>
-      <c r="H26" s="16"/>
+        <v>148</v>
+      </c>
+      <c r="F26" s="21"/>
+      <c r="G26" s="21"/>
+      <c r="H26" s="16" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="16" t="s">
         <v>281</v>
       </c>
       <c r="B27" s="16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C27" s="16" t="s">
-        <v>54</v>
+        <v>25</v>
       </c>
       <c r="D27" s="16" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="E27" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="F27" s="21">
-        <v>3000</v>
-      </c>
-      <c r="G27" s="21"/>
-      <c r="H27" s="16"/>
+        <v>43</v>
+      </c>
+      <c r="F27" s="16"/>
+      <c r="G27" s="16"/>
+      <c r="H27" s="16" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="16" t="s">
         <v>281</v>
       </c>
       <c r="B28" s="16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C28" s="16" t="s">
-        <v>25</v>
+        <v>54</v>
       </c>
       <c r="D28" s="16" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="E28" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="F28" s="16"/>
-      <c r="G28" s="16"/>
-      <c r="H28" s="16"/>
+        <v>55</v>
+      </c>
+      <c r="F28" s="21">
+        <v>3000</v>
+      </c>
+      <c r="G28" s="21"/>
+      <c r="H28" s="16" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="16" t="s">
         <v>281</v>
       </c>
       <c r="B29" s="16" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C29" s="16" t="s">
-        <v>54</v>
+        <v>25</v>
       </c>
       <c r="D29" s="16" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="E29" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="F29" s="21">
-        <v>8000</v>
-      </c>
-      <c r="G29" s="21"/>
-      <c r="H29" s="16"/>
+        <v>43</v>
+      </c>
+      <c r="F29" s="16"/>
+      <c r="G29" s="16"/>
+      <c r="H29" s="16" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="16" t="s">
         <v>281</v>
       </c>
       <c r="B30" s="16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C30" s="16" t="s">
-        <v>270</v>
+        <v>54</v>
       </c>
       <c r="D30" s="16" t="s">
-        <v>271</v>
+        <v>31</v>
       </c>
       <c r="E30" s="16" t="s">
-        <v>272</v>
-      </c>
-      <c r="F30" s="21" t="s">
-        <v>273</v>
+        <v>55</v>
+      </c>
+      <c r="F30" s="21">
+        <v>8000</v>
       </c>
       <c r="G30" s="21"/>
-      <c r="H30" s="16"/>
+      <c r="H30" s="16" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="16" t="s">
         <v>281</v>
       </c>
       <c r="B31" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C31" s="16" t="s">
-        <v>54</v>
+        <v>270</v>
       </c>
       <c r="D31" s="16" t="s">
-        <v>31</v>
+        <v>271</v>
       </c>
       <c r="E31" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="F31" s="21">
-        <v>8000</v>
+        <v>272</v>
+      </c>
+      <c r="F31" s="21" t="s">
+        <v>273</v>
       </c>
       <c r="G31" s="21"/>
       <c r="H31" s="16"/>
@@ -4390,102 +4449,110 @@
         <v>281</v>
       </c>
       <c r="B32" s="16" t="s">
-        <v>90</v>
+        <v>61</v>
       </c>
       <c r="C32" s="16" t="s">
-        <v>274</v>
+        <v>54</v>
       </c>
       <c r="D32" s="16" t="s">
-        <v>275</v>
+        <v>31</v>
       </c>
       <c r="E32" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="F32" s="21"/>
+        <v>55</v>
+      </c>
+      <c r="F32" s="21">
+        <v>8000</v>
+      </c>
       <c r="G32" s="21"/>
-      <c r="H32" s="16"/>
+      <c r="H32" s="16" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="33" spans="1:8">
       <c r="A33" s="16" t="s">
         <v>281</v>
       </c>
       <c r="B33" s="16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C33" s="16" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D33" s="16" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E33" s="16" t="s">
         <v>43</v>
       </c>
       <c r="F33" s="21"/>
       <c r="G33" s="21"/>
-      <c r="H33" s="16"/>
+      <c r="H33" s="16" t="s">
+        <v>287</v>
+      </c>
     </row>
     <row r="34" spans="1:8">
       <c r="A34" s="16" t="s">
         <v>281</v>
       </c>
       <c r="B34" s="16" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C34" s="16" t="s">
-        <v>54</v>
+        <v>276</v>
       </c>
       <c r="D34" s="16" t="s">
-        <v>31</v>
+        <v>277</v>
       </c>
       <c r="E34" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="F34" s="21">
-        <v>3000</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="F34" s="21"/>
       <c r="G34" s="21"/>
-      <c r="H34" s="16"/>
+      <c r="H34" s="16" t="s">
+        <v>287</v>
+      </c>
     </row>
     <row r="35" spans="1:8">
       <c r="A35" s="16" t="s">
         <v>281</v>
       </c>
       <c r="B35" s="16" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C35" s="16" t="s">
-        <v>25</v>
+        <v>54</v>
       </c>
       <c r="D35" s="16" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="E35" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="F35" s="21"/>
+        <v>55</v>
+      </c>
+      <c r="F35" s="21">
+        <v>3000</v>
+      </c>
       <c r="G35" s="21"/>
-      <c r="H35" s="16"/>
+      <c r="H35" s="16" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="36" spans="1:8">
       <c r="A36" s="16" t="s">
         <v>281</v>
       </c>
       <c r="B36" s="16" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C36" s="16" t="s">
-        <v>54</v>
+        <v>25</v>
       </c>
       <c r="D36" s="16" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="E36" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="F36" s="21">
-        <v>3000</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="F36" s="21"/>
       <c r="G36" s="21"/>
       <c r="H36" s="16"/>
     </row>
@@ -4494,18 +4561,20 @@
         <v>281</v>
       </c>
       <c r="B37" s="16" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C37" s="16" t="s">
-        <v>30</v>
+        <v>54</v>
       </c>
       <c r="D37" s="16" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="E37" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="F37" s="21"/>
+        <v>55</v>
+      </c>
+      <c r="F37" s="21">
+        <v>3000</v>
+      </c>
       <c r="G37" s="21"/>
       <c r="H37" s="16"/>
     </row>
@@ -4514,13 +4583,13 @@
         <v>281</v>
       </c>
       <c r="B38" s="16" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C38" s="16" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="D38" s="16" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E38" s="16" t="s">
         <v>43</v>
@@ -4534,20 +4603,18 @@
         <v>281</v>
       </c>
       <c r="B39" s="16" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C39" s="16" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="D39" s="16" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="E39" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="F39" s="21">
-        <v>20000</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="F39" s="21"/>
       <c r="G39" s="21"/>
       <c r="H39" s="16"/>
     </row>
@@ -4556,18 +4623,20 @@
         <v>281</v>
       </c>
       <c r="B40" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C40" s="16" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="D40" s="16" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="E40" s="16" t="s">
-        <v>266</v>
-      </c>
-      <c r="F40" s="21"/>
+        <v>55</v>
+      </c>
+      <c r="F40" s="21">
+        <v>20000</v>
+      </c>
       <c r="G40" s="21"/>
       <c r="H40" s="16"/>
     </row>
@@ -4576,16 +4645,16 @@
         <v>281</v>
       </c>
       <c r="B41" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C41" s="16" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="D41" s="16" t="s">
-        <v>72</v>
+        <v>50</v>
       </c>
       <c r="E41" s="16" t="s">
-        <v>43</v>
+        <v>266</v>
       </c>
       <c r="F41" s="21"/>
       <c r="G41" s="21"/>
@@ -4596,20 +4665,18 @@
         <v>281</v>
       </c>
       <c r="B42" s="16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C42" s="16" t="s">
-        <v>54</v>
+        <v>71</v>
       </c>
       <c r="D42" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="E42" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="F42" s="21">
-        <v>10000</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="E42" s="36" t="s">
+        <v>266</v>
+      </c>
+      <c r="F42" s="21"/>
       <c r="G42" s="21"/>
       <c r="H42" s="16"/>
     </row>
@@ -4618,18 +4685,20 @@
         <v>281</v>
       </c>
       <c r="B43" s="16" t="s">
-        <v>122</v>
+        <v>100</v>
       </c>
       <c r="C43" s="16" t="s">
-        <v>73</v>
+        <v>54</v>
       </c>
       <c r="D43" s="16" t="s">
-        <v>74</v>
+        <v>31</v>
       </c>
       <c r="E43" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="F43" s="21"/>
+        <v>55</v>
+      </c>
+      <c r="F43" s="21">
+        <v>10000</v>
+      </c>
       <c r="G43" s="21"/>
       <c r="H43" s="16"/>
     </row>
@@ -4638,20 +4707,18 @@
         <v>281</v>
       </c>
       <c r="B44" s="16" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C44" s="16" t="s">
-        <v>137</v>
+        <v>73</v>
       </c>
       <c r="D44" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="E44" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="F44" s="21">
-        <v>10000</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="E44" s="36" t="s">
+        <v>266</v>
+      </c>
+      <c r="F44" s="21"/>
       <c r="G44" s="21"/>
       <c r="H44" s="16"/>
     </row>
@@ -4660,18 +4727,20 @@
         <v>281</v>
       </c>
       <c r="B45" s="16" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="C45" s="16" t="s">
-        <v>75</v>
+        <v>137</v>
       </c>
       <c r="D45" s="16" t="s">
         <v>31</v>
       </c>
       <c r="E45" s="16" t="s">
-        <v>76</v>
-      </c>
-      <c r="F45" s="21"/>
+        <v>55</v>
+      </c>
+      <c r="F45" s="21">
+        <v>10000</v>
+      </c>
       <c r="G45" s="21"/>
       <c r="H45" s="16"/>
     </row>
@@ -4680,16 +4749,16 @@
         <v>281</v>
       </c>
       <c r="B46" s="16" t="s">
-        <v>278</v>
+        <v>129</v>
       </c>
       <c r="C46" s="16" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="D46" s="16" t="s">
-        <v>124</v>
+        <v>31</v>
       </c>
       <c r="E46" s="16" t="s">
-        <v>266</v>
+        <v>76</v>
       </c>
       <c r="F46" s="21"/>
       <c r="G46" s="21"/>
@@ -4700,20 +4769,18 @@
         <v>281</v>
       </c>
       <c r="B47" s="16" t="s">
-        <v>130</v>
+        <v>278</v>
       </c>
       <c r="C47" s="16" t="s">
-        <v>54</v>
+        <v>87</v>
       </c>
       <c r="D47" s="16" t="s">
-        <v>31</v>
+        <v>124</v>
       </c>
       <c r="E47" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="F47" s="21">
-        <v>30000</v>
-      </c>
+        <v>266</v>
+      </c>
+      <c r="F47" s="21"/>
       <c r="G47" s="21"/>
       <c r="H47" s="16"/>
     </row>
@@ -4722,20 +4789,42 @@
         <v>281</v>
       </c>
       <c r="B48" s="16" t="s">
-        <v>279</v>
+        <v>130</v>
       </c>
       <c r="C48" s="16" t="s">
-        <v>88</v>
+        <v>54</v>
       </c>
       <c r="D48" s="16" t="s">
         <v>31</v>
       </c>
       <c r="E48" s="16" t="s">
-        <v>227</v>
-      </c>
-      <c r="F48" s="21"/>
+        <v>55</v>
+      </c>
+      <c r="F48" s="21">
+        <v>30000</v>
+      </c>
       <c r="G48" s="21"/>
       <c r="H48" s="16"/>
+    </row>
+    <row r="49" spans="1:8">
+      <c r="A49" s="16" t="s">
+        <v>281</v>
+      </c>
+      <c r="B49" s="16" t="s">
+        <v>279</v>
+      </c>
+      <c r="C49" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="D49" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="E49" s="16" t="s">
+        <v>227</v>
+      </c>
+      <c r="F49" s="21"/>
+      <c r="G49" s="21"/>
+      <c r="H49" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -4752,8 +4841,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84C8C304-D672-42E3-8009-BB544F384D0E}">
   <dimension ref="A1:I62"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4768,36 +4857,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="25" t="s">
         <v>160</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="26"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="27"/>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="24"/>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="26"/>
+      <c r="A2" s="25"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="27"/>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="27"/>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
-      <c r="H3" s="29"/>
+      <c r="A3" s="28"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="30"/>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="4" t="s">
@@ -5180,7 +5269,7 @@
         <v>198</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>199</v>
+        <v>285</v>
       </c>
       <c r="G21" s="7"/>
       <c r="H21" s="3"/>
@@ -6083,36 +6172,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="25" t="s">
         <v>201</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="26"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="27"/>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="24"/>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="26"/>
+      <c r="A2" s="25"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="27"/>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="27"/>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
-      <c r="H3" s="29"/>
+      <c r="A3" s="28"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="30"/>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="4" t="s">
@@ -7007,36 +7096,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="30"/>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="32"/>
+      <c r="A1" s="31"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="33"/>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="30"/>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="32"/>
+      <c r="A2" s="31"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="33"/>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="33"/>
-      <c r="B3" s="33"/>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33" t="s">
+      <c r="A3" s="34"/>
+      <c r="B3" s="34"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34" t="s">
         <v>81</v>
       </c>
-      <c r="G3" s="33"/>
-      <c r="H3" s="34"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="35"/>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="4" t="s">

</xml_diff>

<commit_message>
Made changes to check the os of the machine
</commit_message>
<xml_diff>
--- a/TestDataAndResults/Run1/SophieAutomation.xlsx
+++ b/TestDataAndResults/Run1/SophieAutomation.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr documentId="13_ncr:1_{AC3BCE6A-6F26-4D65-ACCD-2DB08400D9FD}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC3BCE6A-6F26-4D65-ACCD-2DB08400D9FD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="1" firstSheet="1" windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" r:id="rId1" sheetId="8"/>
-    <sheet name="DriverSheet" r:id="rId2" sheetId="1"/>
-    <sheet name="VerifyCSVForExistingVersion" r:id="rId3" sheetId="4"/>
-    <sheet name="VerifyCSVForNewVersion" r:id="rId4" sheetId="10"/>
-    <sheet name="VerifyDeleteOffer" r:id="rId5" sheetId="11"/>
-    <sheet name="VerifyEventAPI" r:id="rId6" sheetId="6"/>
-    <sheet name="Cases_RealTimeSpine" r:id="rId7" sheetId="9"/>
-    <sheet name="BatchDecisionOutputValidations" r:id="rId8" sheetId="5"/>
-    <sheet name="CheckLists" r:id="rId9" sheetId="7"/>
+    <sheet name="Sheet1" sheetId="8" r:id="rId1"/>
+    <sheet name="DriverSheet" sheetId="1" r:id="rId2"/>
+    <sheet name="VerifyCSVForExistingVersion" sheetId="4" r:id="rId3"/>
+    <sheet name="VerifyCSVForNewVersion" sheetId="10" r:id="rId4"/>
+    <sheet name="VerifyDeleteOffer" sheetId="11" r:id="rId5"/>
+    <sheet name="VerifyEventAPI" sheetId="6" r:id="rId6"/>
+    <sheet name="Cases_RealTimeSpine" sheetId="9" r:id="rId7"/>
+    <sheet name="BatchDecisionOutputValidations" sheetId="5" r:id="rId8"/>
+    <sheet name="CheckLists" sheetId="7" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1380" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1350" uniqueCount="286">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -892,19 +892,12 @@
   </si>
   <si>
     <t>PegaGadget2Ifr</t>
-  </si>
-  <si>
-    <t>Pass</t>
-  </si>
-  <si>
-    <t>Fail</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="5">
     <font>
       <sz val="11"/>
@@ -1076,82 +1069,82 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="37">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" applyFont="1" borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" borderId="1" fillId="0" fontId="3" numFmtId="0" quotePrefix="1" xfId="1"/>
-    <xf applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="2" numFmtId="0" quotePrefix="1" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="2" fillId="3" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="2" fontId="1" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="14" xfId="0"/>
-    <xf applyBorder="1" applyFont="1" borderId="6" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" borderId="6" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="8" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFont="1" borderId="8" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="3" fillId="2" fontId="1" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFont="1" borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="1" fillId="0" fontId="3" numFmtId="0" quotePrefix="1" xfId="1"/>
-    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="0" fontId="2" numFmtId="0" quotePrefix="1" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="2" fillId="3" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="4" fillId="3" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="3" fillId="3" fontId="2" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="4" fillId="3" fontId="2" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="5" fillId="3" fontId="2" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="3" fillId="3" fontId="2" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="4" fillId="3" fontId="2" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="5" fillId="3" fontId="2" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="3" fillId="3" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="4" fillId="3" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="5" fillId="3" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyFill="1" borderId="0" fillId="3" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="7" fillId="3" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="5" fontId="2" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1164,7 +1157,7 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -1217,10 +1210,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -1255,7 +1248,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1290,7 +1283,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1384,21 +1377,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1415,7 +1408,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -1467,15 +1460,15 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B890B66B-A108-4A1B-86CC-76F144B26418}">
-  <dimension ref="A1:G1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B890B66B-A108-4A1B-86CC-76F144B26418}">
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
@@ -1504,14 +1497,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
@@ -1519,15 +1512,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="2" width="14.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="27.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="2" width="70.7109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="2" width="19.140625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="2" width="24.42578125" collapsed="true"/>
-    <col min="6" max="16384" style="2" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="14.5703125" style="2" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="27.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="70.7109375" style="2" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="19.140625" style="2" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="24.42578125" style="2" customWidth="1" collapsed="1"/>
+    <col min="6" max="16384" width="9.140625" style="2" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" ht="14.25" r="1" s="5" spans="1:5">
+    <row r="1" spans="1:5" s="5" customFormat="1" ht="14.25">
       <c r="A1" s="23" t="s">
         <v>9</v>
       </c>
@@ -1536,7 +1529,7 @@
       <c r="D1" s="23"/>
       <c r="E1" s="23"/>
     </row>
-    <row customFormat="1" ht="14.25" r="2" s="5" spans="1:5">
+    <row r="2" spans="1:5" s="5" customFormat="1" ht="14.25">
       <c r="A2" s="24" t="s">
         <v>132</v>
       </c>
@@ -1545,14 +1538,14 @@
       <c r="D2" s="24"/>
       <c r="E2" s="24"/>
     </row>
-    <row customFormat="1" ht="14.25" r="3" s="5" spans="1:5">
+    <row r="3" spans="1:5" s="5" customFormat="1" ht="14.25">
       <c r="A3" s="10"/>
       <c r="B3" s="10"/>
       <c r="C3" s="10"/>
       <c r="D3" s="10"/>
       <c r="E3" s="10"/>
     </row>
-    <row customFormat="1" ht="14.25" r="4" s="1" spans="1:5">
+    <row r="4" spans="1:5" s="1" customFormat="1" ht="14.25">
       <c r="A4" s="11" t="s">
         <v>0</v>
       </c>
@@ -1649,13 +1642,13 @@
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A2:E2"/>
   </mergeCells>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32EA4E71-0B53-4881-A15A-C454293CD34C}">
-  <dimension ref="A1:I44"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32EA4E71-0B53-4881-A15A-C454293CD34C}">
+  <dimension ref="A1:H44"/>
   <sheetViews>
     <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="D42" sqref="D42"/>
@@ -1663,14 +1656,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="16.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="14.85546875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="39.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="27.85546875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="32.5703125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="31.42578125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="31.42578125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="7.85546875" collapsed="true"/>
+    <col min="1" max="1" width="16.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="39" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="27.85546875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="32.5703125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="31.42578125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="31.42578125" customWidth="1"/>
+    <col min="8" max="8" width="7.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -2579,14 +2572,14 @@
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A3:H3"/>
   </mergeCells>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="0" orientation="portrait" r:id="rId1" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F162030-4240-4061-B605-62E03F55BA7B}">
-  <dimension ref="A1:I55"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F162030-4240-4061-B605-62E03F55BA7B}">
+  <dimension ref="A1:H55"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="E16" sqref="E16:F16"/>
@@ -2594,11 +2587,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="34.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="22.140625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="30.85546875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="26.5703125" collapsed="true"/>
+    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -3737,29 +3730,29 @@
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A3:H3"/>
   </mergeCells>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D61013C2-7F35-4D0B-B54C-3015EDB52E25}">
-  <dimension ref="A1:I49"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D61013C2-7F35-4D0B-B54C-3015EDB52E25}">
+  <dimension ref="A1:H49"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="85" zoomScaleNormal="85">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="16.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="14.85546875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="39.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="27.85546875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="32.5703125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="31.42578125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="31.42578125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="7.86328125" collapsed="true"/>
-    <col min="9" max="16384" style="22" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="16.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="39" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="27.85546875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="32.5703125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="31.42578125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="31.42578125" customWidth="1"/>
+    <col min="8" max="8" width="7.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="16384" width="9.140625" style="22"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -3840,9 +3833,7 @@
       </c>
       <c r="F5" s="16"/>
       <c r="G5" s="16"/>
-      <c r="H5" s="16" t="s">
-        <v>286</v>
-      </c>
+      <c r="H5" s="16"/>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="16" t="s">
@@ -3864,9 +3855,7 @@
         <v>31</v>
       </c>
       <c r="G6" s="16"/>
-      <c r="H6" s="16" t="s">
-        <v>286</v>
-      </c>
+      <c r="H6" s="16"/>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="16" t="s">
@@ -3888,9 +3877,7 @@
         <v>5000</v>
       </c>
       <c r="G7" s="20"/>
-      <c r="H7" s="16" t="s">
-        <v>286</v>
-      </c>
+      <c r="H7" s="16"/>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="16" t="s">
@@ -3910,9 +3897,7 @@
       </c>
       <c r="F8" s="16"/>
       <c r="G8" s="16"/>
-      <c r="H8" s="16" t="s">
-        <v>286</v>
-      </c>
+      <c r="H8" s="16"/>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="16" t="s">
@@ -3934,9 +3919,7 @@
         <v>57</v>
       </c>
       <c r="G9" s="21"/>
-      <c r="H9" s="16" t="s">
-        <v>286</v>
-      </c>
+      <c r="H9" s="16"/>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="16" t="s">
@@ -3956,9 +3939,7 @@
       </c>
       <c r="F10" s="16"/>
       <c r="G10" s="16"/>
-      <c r="H10" s="16" t="s">
-        <v>286</v>
-      </c>
+      <c r="H10" s="16"/>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="16" t="s">
@@ -3980,9 +3961,7 @@
         <v>62</v>
       </c>
       <c r="G11" s="21"/>
-      <c r="H11" s="16" t="s">
-        <v>286</v>
-      </c>
+      <c r="H11" s="16"/>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="16" t="s">
@@ -4002,9 +3981,7 @@
       </c>
       <c r="F12" s="16"/>
       <c r="G12" s="16"/>
-      <c r="H12" s="16" t="s">
-        <v>286</v>
-      </c>
+      <c r="H12" s="16"/>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="16" t="s">
@@ -4026,9 +4003,7 @@
         <v>62</v>
       </c>
       <c r="G13" s="21"/>
-      <c r="H13" s="16" t="s">
-        <v>286</v>
-      </c>
+      <c r="H13" s="16"/>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="16" t="s">
@@ -4048,9 +4023,7 @@
       </c>
       <c r="F14" s="16"/>
       <c r="G14" s="16"/>
-      <c r="H14" s="16" t="s">
-        <v>286</v>
-      </c>
+      <c r="H14" s="16"/>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="16" t="s">
@@ -4072,9 +4045,7 @@
         <v>62</v>
       </c>
       <c r="G15" s="21"/>
-      <c r="H15" s="16" t="s">
-        <v>286</v>
-      </c>
+      <c r="H15" s="16"/>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="16" t="s">
@@ -4096,9 +4067,7 @@
         <v>199</v>
       </c>
       <c r="G16" s="21"/>
-      <c r="H16" s="16" t="s">
-        <v>286</v>
-      </c>
+      <c r="H16" s="16"/>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="16" t="s">
@@ -4120,9 +4089,7 @@
         <v>284</v>
       </c>
       <c r="G17" s="21"/>
-      <c r="H17" s="16" t="s">
-        <v>286</v>
-      </c>
+      <c r="H17" s="16"/>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="16" t="s">
@@ -4144,9 +4111,7 @@
         <v>5000</v>
       </c>
       <c r="G18" s="21"/>
-      <c r="H18" s="16" t="s">
-        <v>286</v>
-      </c>
+      <c r="H18" s="16"/>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="16" t="s">
@@ -4166,9 +4131,7 @@
       </c>
       <c r="F19" s="16"/>
       <c r="G19" s="16"/>
-      <c r="H19" s="16" t="s">
-        <v>286</v>
-      </c>
+      <c r="H19" s="16"/>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="16" t="s">
@@ -4190,9 +4153,7 @@
         <v>269</v>
       </c>
       <c r="G20" s="16"/>
-      <c r="H20" s="16" t="s">
-        <v>286</v>
-      </c>
+      <c r="H20" s="16"/>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="16" t="s">
@@ -4214,9 +4175,7 @@
         <v>65</v>
       </c>
       <c r="G21" s="16"/>
-      <c r="H21" s="16" t="s">
-        <v>286</v>
-      </c>
+      <c r="H21" s="16"/>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="16" t="s">
@@ -4236,9 +4195,7 @@
       </c>
       <c r="F22" s="16"/>
       <c r="G22" s="16"/>
-      <c r="H22" s="16" t="s">
-        <v>286</v>
-      </c>
+      <c r="H22" s="16"/>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="16" t="s">
@@ -4260,9 +4217,7 @@
         <v>3000</v>
       </c>
       <c r="G23" s="21"/>
-      <c r="H23" s="16" t="s">
-        <v>286</v>
-      </c>
+      <c r="H23" s="16"/>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="16" t="s">
@@ -4282,9 +4237,7 @@
       </c>
       <c r="F24" s="21"/>
       <c r="G24" s="21"/>
-      <c r="H24" s="16" t="s">
-        <v>286</v>
-      </c>
+      <c r="H24" s="16"/>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="16" t="s">
@@ -4304,9 +4257,7 @@
       </c>
       <c r="F25" s="21"/>
       <c r="G25" s="21"/>
-      <c r="H25" s="16" t="s">
-        <v>286</v>
-      </c>
+      <c r="H25" s="16"/>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="16" t="s">
@@ -4326,9 +4277,7 @@
       </c>
       <c r="F26" s="21"/>
       <c r="G26" s="21"/>
-      <c r="H26" s="16" t="s">
-        <v>286</v>
-      </c>
+      <c r="H26" s="16"/>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="16" t="s">
@@ -4348,9 +4297,7 @@
       </c>
       <c r="F27" s="16"/>
       <c r="G27" s="16"/>
-      <c r="H27" s="16" t="s">
-        <v>286</v>
-      </c>
+      <c r="H27" s="16"/>
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="16" t="s">
@@ -4372,9 +4319,7 @@
         <v>3000</v>
       </c>
       <c r="G28" s="21"/>
-      <c r="H28" s="16" t="s">
-        <v>286</v>
-      </c>
+      <c r="H28" s="16"/>
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="16" t="s">
@@ -4394,9 +4339,7 @@
       </c>
       <c r="F29" s="16"/>
       <c r="G29" s="16"/>
-      <c r="H29" s="16" t="s">
-        <v>286</v>
-      </c>
+      <c r="H29" s="16"/>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="16" t="s">
@@ -4418,9 +4361,7 @@
         <v>8000</v>
       </c>
       <c r="G30" s="21"/>
-      <c r="H30" s="16" t="s">
-        <v>286</v>
-      </c>
+      <c r="H30" s="16"/>
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="16" t="s">
@@ -4464,9 +4405,7 @@
         <v>8000</v>
       </c>
       <c r="G32" s="21"/>
-      <c r="H32" s="16" t="s">
-        <v>286</v>
-      </c>
+      <c r="H32" s="16"/>
     </row>
     <row r="33" spans="1:8">
       <c r="A33" s="16" t="s">
@@ -4486,9 +4425,7 @@
       </c>
       <c r="F33" s="21"/>
       <c r="G33" s="21"/>
-      <c r="H33" s="16" t="s">
-        <v>287</v>
-      </c>
+      <c r="H33" s="16"/>
     </row>
     <row r="34" spans="1:8">
       <c r="A34" s="16" t="s">
@@ -4508,9 +4445,7 @@
       </c>
       <c r="F34" s="21"/>
       <c r="G34" s="21"/>
-      <c r="H34" s="16" t="s">
-        <v>287</v>
-      </c>
+      <c r="H34" s="16"/>
     </row>
     <row r="35" spans="1:8">
       <c r="A35" s="16" t="s">
@@ -4532,9 +4467,7 @@
         <v>3000</v>
       </c>
       <c r="G35" s="21"/>
-      <c r="H35" s="16" t="s">
-        <v>286</v>
-      </c>
+      <c r="H35" s="16"/>
     </row>
     <row r="36" spans="1:8">
       <c r="A36" s="16" t="s">
@@ -4832,14 +4765,14 @@
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A3:H3"/>
   </mergeCells>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="0" orientation="portrait" r:id="rId1" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84C8C304-D672-42E3-8009-BB544F384D0E}">
-  <dimension ref="A1:I62"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84C8C304-D672-42E3-8009-BB544F384D0E}">
+  <dimension ref="A1:H62"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="F21" sqref="F21"/>
@@ -4847,13 +4780,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="7.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="28.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="22.140625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="33.140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="21.85546875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="21.85546875" collapsed="true"/>
+    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.140625" customWidth="1"/>
+    <col min="6" max="6" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -6146,14 +6079,14 @@
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A3:H3"/>
   </mergeCells>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="0" orientation="portrait" r:id="rId1" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B59FADFD-33E9-4E6D-B86E-1A88AF7CF694}">
-  <dimension ref="A1:I44"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B59FADFD-33E9-4E6D-B86E-1A88AF7CF694}">
+  <dimension ref="A1:H44"/>
   <sheetViews>
     <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="F38" sqref="F38"/>
@@ -6161,14 +6094,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="7.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="35.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="38.7109375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="24.42578125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="21.85546875" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="8.140625" collapsed="true"/>
+    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.85546875" customWidth="1"/>
+    <col min="4" max="4" width="38.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -7071,13 +7004,13 @@
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A3:H3"/>
   </mergeCells>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38793A77-4CB9-44FE-853A-5596922718C4}">
-  <dimension ref="A1:I10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38793A77-4CB9-44FE-853A-5596922718C4}">
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
@@ -7085,14 +7018,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="22.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="18.7109375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="21.42578125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="28.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="18.85546875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="19.5703125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="1" max="1" width="22.140625" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="21.42578125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="28" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="18.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="19.5703125" customWidth="1"/>
+    <col min="8" max="8" width="18" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -7257,13 +7190,13 @@
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A3:H3"/>
   </mergeCells>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B52690B1-76B3-48CD-AA9A-87FEE1811DD3}">
-  <dimension ref="A2:C3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B52690B1-76B3-48CD-AA9A-87FEE1811DD3}">
+  <dimension ref="A2:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
@@ -7271,7 +7204,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:2">
@@ -7291,6 +7224,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Code changes in the test class
</commit_message>
<xml_diff>
--- a/TestDataAndResults/Run1/SophieAutomation.xlsx
+++ b/TestDataAndResults/Run1/SophieAutomation.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC3BCE6A-6F26-4D65-ACCD-2DB08400D9FD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{AC3BCE6A-6F26-4D65-ACCD-2DB08400D9FD}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="1" firstSheet="1" windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="8" r:id="rId1"/>
-    <sheet name="DriverSheet" sheetId="1" r:id="rId2"/>
-    <sheet name="VerifyCSVForExistingVersion" sheetId="4" r:id="rId3"/>
-    <sheet name="VerifyCSVForNewVersion" sheetId="10" r:id="rId4"/>
-    <sheet name="VerifyDeleteOffer" sheetId="11" r:id="rId5"/>
-    <sheet name="VerifyEventAPI" sheetId="6" r:id="rId6"/>
-    <sheet name="Cases_RealTimeSpine" sheetId="9" r:id="rId7"/>
-    <sheet name="BatchDecisionOutputValidations" sheetId="5" r:id="rId8"/>
-    <sheet name="CheckLists" sheetId="7" r:id="rId9"/>
+    <sheet name="Sheet1" r:id="rId1" sheetId="8"/>
+    <sheet name="DriverSheet" r:id="rId2" sheetId="1"/>
+    <sheet name="VerifyCSVForExistingVersion" r:id="rId3" sheetId="4"/>
+    <sheet name="VerifyCSVForNewVersion" r:id="rId4" sheetId="10"/>
+    <sheet name="VerifyDeleteOffer" r:id="rId5" sheetId="11"/>
+    <sheet name="VerifyEventAPI" r:id="rId6" sheetId="6"/>
+    <sheet name="Cases_RealTimeSpine" r:id="rId7" sheetId="9"/>
+    <sheet name="BatchDecisionOutputValidations" r:id="rId8" sheetId="5"/>
+    <sheet name="CheckLists" r:id="rId9" sheetId="7"/>
   </sheets>
   <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1350" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1354" uniqueCount="287">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -892,12 +892,16 @@
   </si>
   <si>
     <t>PegaGadget2Ifr</t>
+  </si>
+  <si>
+    <t>Pass</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="5">
     <font>
       <sz val="11"/>
@@ -1069,82 +1073,82 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="37">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" applyFont="1" borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" borderId="1" fillId="0" fontId="3" numFmtId="0" quotePrefix="1" xfId="1"/>
+    <xf applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="2" numFmtId="0" quotePrefix="1" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="2" fillId="3" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="2" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="14" xfId="0"/>
+    <xf applyBorder="1" applyFont="1" borderId="6" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" borderId="6" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="8" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFont="1" borderId="8" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="3" fillId="2" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFont="1" borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="1" fillId="0" fontId="3" numFmtId="0" quotePrefix="1" xfId="1"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="0" fontId="2" numFmtId="0" quotePrefix="1" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="2" fillId="3" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="4" fillId="3" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="3" fillId="3" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="4" fillId="3" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="5" fillId="3" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="3" fillId="3" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="4" fillId="3" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="5" fillId="3" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="3" fillId="3" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="4" fillId="3" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="5" fillId="3" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" borderId="0" fillId="3" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="7" fillId="3" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="5" fontId="2" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1157,7 +1161,7 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+<xdr:wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -1210,10 +1214,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -1248,7 +1252,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1283,7 +1287,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1377,21 +1381,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1408,7 +1412,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -1460,15 +1464,15 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B890B66B-A108-4A1B-86CC-76F144B26418}">
-  <dimension ref="A1:F1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B890B66B-A108-4A1B-86CC-76F144B26418}">
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
@@ -1497,14 +1501,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
@@ -1512,15 +1516,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" style="2" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="27.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="70.7109375" style="2" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="19.140625" style="2" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="24.42578125" style="2" customWidth="1" collapsed="1"/>
-    <col min="6" max="16384" width="9.140625" style="2" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="2" width="14.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="27.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="2" width="70.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="2" width="19.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="2" width="24.42578125" collapsed="true"/>
+    <col min="6" max="16384" style="2" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="5" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="1" s="5" spans="1:5">
       <c r="A1" s="23" t="s">
         <v>9</v>
       </c>
@@ -1529,7 +1533,7 @@
       <c r="D1" s="23"/>
       <c r="E1" s="23"/>
     </row>
-    <row r="2" spans="1:5" s="5" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="2" s="5" spans="1:5">
       <c r="A2" s="24" t="s">
         <v>132</v>
       </c>
@@ -1538,14 +1542,14 @@
       <c r="D2" s="24"/>
       <c r="E2" s="24"/>
     </row>
-    <row r="3" spans="1:5" s="5" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="3" s="5" spans="1:5">
       <c r="A3" s="10"/>
       <c r="B3" s="10"/>
       <c r="C3" s="10"/>
       <c r="D3" s="10"/>
       <c r="E3" s="10"/>
     </row>
-    <row r="4" spans="1:5" s="1" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="4" s="1" spans="1:5">
       <c r="A4" s="11" t="s">
         <v>0</v>
       </c>
@@ -1642,13 +1646,13 @@
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A2:E2"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32EA4E71-0B53-4881-A15A-C454293CD34C}">
-  <dimension ref="A1:H44"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32EA4E71-0B53-4881-A15A-C454293CD34C}">
+  <dimension ref="A1:I44"/>
   <sheetViews>
     <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="D42" sqref="D42"/>
@@ -1656,14 +1660,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="39" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="27.85546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="32.5703125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="31.42578125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="31.42578125" customWidth="1"/>
-    <col min="8" max="8" width="7.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="39.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="27.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="32.5703125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="31.42578125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="31.42578125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="7.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -2572,14 +2576,14 @@
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A3:H3"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" r:id="rId1" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F162030-4240-4061-B605-62E03F55BA7B}">
-  <dimension ref="A1:H55"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F162030-4240-4061-B605-62E03F55BA7B}">
+  <dimension ref="A1:I55"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="E16" sqref="E16:F16"/>
@@ -2587,11 +2591,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="34.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="22.140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="30.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="26.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -3730,29 +3734,29 @@
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A3:H3"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D61013C2-7F35-4D0B-B54C-3015EDB52E25}">
-  <dimension ref="A1:H49"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D61013C2-7F35-4D0B-B54C-3015EDB52E25}">
+  <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView workbookViewId="0" zoomScale="85" zoomScaleNormal="85">
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="39" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="27.85546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="32.5703125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="31.42578125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="31.42578125" customWidth="1"/>
-    <col min="8" max="8" width="7.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="16384" width="9.140625" style="22"/>
+    <col min="1" max="1" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="39.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="27.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="32.5703125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="31.42578125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="31.42578125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="7.86328125" collapsed="true"/>
+    <col min="9" max="16384" style="22" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -3833,7 +3837,9 @@
       </c>
       <c r="F5" s="16"/>
       <c r="G5" s="16"/>
-      <c r="H5" s="16"/>
+      <c r="H5" s="16" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="16" t="s">
@@ -3855,7 +3861,9 @@
         <v>31</v>
       </c>
       <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
+      <c r="H6" s="16" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="16" t="s">
@@ -3877,7 +3885,9 @@
         <v>5000</v>
       </c>
       <c r="G7" s="20"/>
-      <c r="H7" s="16"/>
+      <c r="H7" s="16" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="16" t="s">
@@ -3897,7 +3907,9 @@
       </c>
       <c r="F8" s="16"/>
       <c r="G8" s="16"/>
-      <c r="H8" s="16"/>
+      <c r="H8" s="16" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="16" t="s">
@@ -4765,14 +4777,14 @@
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A3:H3"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" r:id="rId1" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84C8C304-D672-42E3-8009-BB544F384D0E}">
-  <dimension ref="A1:H62"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84C8C304-D672-42E3-8009-BB544F384D0E}">
+  <dimension ref="A1:I62"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="F21" sqref="F21"/>
@@ -4780,13 +4792,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="33.140625" customWidth="1"/>
-    <col min="6" max="6" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.85546875" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="7.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="28.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="22.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="33.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="21.85546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="21.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -6079,14 +6091,14 @@
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A3:H3"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" r:id="rId1" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B59FADFD-33E9-4E6D-B86E-1A88AF7CF694}">
-  <dimension ref="A1:H44"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B59FADFD-33E9-4E6D-B86E-1A88AF7CF694}">
+  <dimension ref="A1:I44"/>
   <sheetViews>
     <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="F38" sqref="F38"/>
@@ -6094,14 +6106,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.85546875" customWidth="1"/>
-    <col min="4" max="4" width="38.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="7.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="35.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="38.7109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="24.42578125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="21.85546875" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="8.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -7004,13 +7016,13 @@
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A3:H3"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38793A77-4CB9-44FE-853A-5596922718C4}">
-  <dimension ref="A1:H10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38793A77-4CB9-44FE-853A-5596922718C4}">
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
@@ -7018,14 +7030,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="22.140625" customWidth="1"/>
-    <col min="2" max="2" width="18.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="21.42578125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="28" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="18.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="19.5703125" customWidth="1"/>
-    <col min="8" max="8" width="18" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="22.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="21.42578125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="28.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="19.5703125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="18.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -7190,13 +7202,13 @@
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A3:H3"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B52690B1-76B3-48CD-AA9A-87FEE1811DD3}">
-  <dimension ref="A2:B3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B52690B1-76B3-48CD-AA9A-87FEE1811DD3}">
+  <dimension ref="A2:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
@@ -7204,7 +7216,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:2">
@@ -7224,6 +7236,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Code change to display the data
</commit_message>
<xml_diff>
--- a/TestDataAndResults/Run1/SophieAutomation.xlsx
+++ b/TestDataAndResults/Run1/SophieAutomation.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr documentId="13_ncr:1_{AC3BCE6A-6F26-4D65-ACCD-2DB08400D9FD}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43"/>
+  <xr:revisionPtr documentId="13_ncr:1_{8D8477B9-B660-4478-965D-1C32BB43AD9F}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43"/>
   <bookViews>
     <workbookView activeTab="1" firstSheet="1" windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1354" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1363" uniqueCount="288">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -895,6 +895,9 @@
   </si>
   <si>
     <t>Pass</t>
+  </si>
+  <si>
+    <t>Fail</t>
   </si>
 </sst>
 </file>
@@ -1102,6 +1105,7 @@
     <xf applyBorder="1" applyFill="1" borderId="1" fillId="0" fontId="3" numFmtId="0" quotePrefix="1" xfId="1"/>
     <xf applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="0" fontId="2" numFmtId="0" quotePrefix="1" xfId="0"/>
     <xf applyFill="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="5" fontId="2" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="2" fillId="3" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
@@ -1141,7 +1145,6 @@
     <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="7" fillId="3" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="5" fontId="2" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
@@ -1511,7 +1514,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1525,22 +1528,22 @@
   </cols>
   <sheetData>
     <row customFormat="1" ht="14.25" r="1" s="5" spans="1:5">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
     </row>
     <row customFormat="1" ht="14.25" r="2" s="5" spans="1:5">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="25" t="s">
         <v>132</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
     </row>
     <row customFormat="1" ht="14.25" r="3" s="5" spans="1:5">
       <c r="A3" s="10"/>
@@ -1577,7 +1580,7 @@
         <v>32</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E5" s="3"/>
     </row>
@@ -1592,7 +1595,7 @@
         <v>101</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E6" s="3"/>
     </row>
@@ -1607,7 +1610,7 @@
         <v>184</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E7" s="3"/>
     </row>
@@ -1622,7 +1625,7 @@
         <v>282</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="E8" s="3"/>
     </row>
@@ -1667,42 +1670,42 @@
     <col min="5" max="5" customWidth="true" width="32.5703125" collapsed="true"/>
     <col min="6" max="6" customWidth="true" width="31.42578125" collapsed="true"/>
     <col min="7" max="7" customWidth="true" width="31.42578125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="7.85546875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="7.86328125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="27"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="28"/>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="26" t="s">
         <v>156</v>
       </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="27"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="28"/>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="28"/>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="30"/>
+      <c r="A3" s="29"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="31"/>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="18" t="s">
@@ -1750,7 +1753,9 @@
         <v>31</v>
       </c>
       <c r="G5" s="9"/>
-      <c r="H5" s="3"/>
+      <c r="H5" s="3" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
@@ -1772,7 +1777,9 @@
         <v>31</v>
       </c>
       <c r="G6" s="9"/>
-      <c r="H6" s="3"/>
+      <c r="H6" s="3" t="s">
+        <v>287</v>
+      </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
@@ -1794,7 +1801,9 @@
         <v>5000</v>
       </c>
       <c r="G7" s="9"/>
-      <c r="H7" s="3"/>
+      <c r="H7" s="3" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
@@ -1814,7 +1823,9 @@
       </c>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
-      <c r="H8" s="3"/>
+      <c r="H8" s="3" t="s">
+        <v>287</v>
+      </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
@@ -1836,7 +1847,9 @@
         <v>2000</v>
       </c>
       <c r="G9" s="9"/>
-      <c r="H9" s="3"/>
+      <c r="H9" s="3" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
@@ -1856,7 +1869,9 @@
       </c>
       <c r="F10" s="9"/>
       <c r="G10" s="9"/>
-      <c r="H10" s="3"/>
+      <c r="H10" s="3" t="s">
+        <v>287</v>
+      </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
@@ -1878,7 +1893,9 @@
         <v>3000</v>
       </c>
       <c r="G11" s="9"/>
-      <c r="H11" s="3"/>
+      <c r="H11" s="3" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
@@ -1898,7 +1915,9 @@
       </c>
       <c r="F12" s="9"/>
       <c r="G12" s="9"/>
-      <c r="H12" s="3"/>
+      <c r="H12" s="3" t="s">
+        <v>287</v>
+      </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
@@ -1920,7 +1939,9 @@
         <v>3000</v>
       </c>
       <c r="G13" s="9"/>
-      <c r="H13" s="3"/>
+      <c r="H13" s="3" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" t="s">
@@ -1940,7 +1961,9 @@
       </c>
       <c r="F14" s="9"/>
       <c r="G14" s="9"/>
-      <c r="H14" s="3"/>
+      <c r="H14" s="3" t="s">
+        <v>287</v>
+      </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
@@ -1962,7 +1985,9 @@
         <v>3000</v>
       </c>
       <c r="G15" s="9"/>
-      <c r="H15" s="3"/>
+      <c r="H15" s="3" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" t="s">
@@ -1984,7 +2009,9 @@
         <v>199</v>
       </c>
       <c r="G16" s="9"/>
-      <c r="H16" s="3"/>
+      <c r="H16" s="3" t="s">
+        <v>287</v>
+      </c>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" t="s">
@@ -2006,7 +2033,9 @@
         <v>284</v>
       </c>
       <c r="G17" s="9"/>
-      <c r="H17" s="3"/>
+      <c r="H17" s="3" t="s">
+        <v>287</v>
+      </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="19" t="s">
@@ -2417,7 +2446,7 @@
       <c r="D37" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="E37" s="36" t="s">
+      <c r="E37" s="23" t="s">
         <v>266</v>
       </c>
       <c r="F37" s="3"/>
@@ -2459,7 +2488,7 @@
       <c r="D39" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="E39" s="36" t="s">
+      <c r="E39" s="23" t="s">
         <v>266</v>
       </c>
       <c r="F39" s="3"/>
@@ -2599,38 +2628,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="27"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="28"/>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="26" t="s">
         <v>156</v>
       </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="27"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="28"/>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="28"/>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="30"/>
+      <c r="A3" s="29"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="31"/>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="4" t="s">
@@ -3575,7 +3604,7 @@
       <c r="D48" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="E48" s="36" t="s">
+      <c r="E48" s="23" t="s">
         <v>266</v>
       </c>
       <c r="F48" s="3"/>
@@ -3617,7 +3646,7 @@
       <c r="D50" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="E50" s="36" t="s">
+      <c r="E50" s="23" t="s">
         <v>266</v>
       </c>
       <c r="F50" s="3"/>
@@ -3755,43 +3784,43 @@
     <col min="5" max="5" customWidth="true" width="32.5703125" collapsed="true"/>
     <col min="6" max="6" customWidth="true" width="31.42578125" collapsed="true"/>
     <col min="7" max="7" customWidth="true" width="31.42578125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="7.86328125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="7.85546875" collapsed="true"/>
     <col min="9" max="16384" style="22" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="27"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="28"/>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="26" t="s">
         <v>156</v>
       </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="27"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="28"/>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="28"/>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="30"/>
+      <c r="A3" s="29"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="31"/>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="4" t="s">
@@ -3837,9 +3866,7 @@
       </c>
       <c r="F5" s="16"/>
       <c r="G5" s="16"/>
-      <c r="H5" s="16" t="s">
-        <v>286</v>
-      </c>
+      <c r="H5" s="16"/>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="16" t="s">
@@ -3861,9 +3888,7 @@
         <v>31</v>
       </c>
       <c r="G6" s="16"/>
-      <c r="H6" s="16" t="s">
-        <v>286</v>
-      </c>
+      <c r="H6" s="16"/>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="16" t="s">
@@ -3885,9 +3910,7 @@
         <v>5000</v>
       </c>
       <c r="G7" s="20"/>
-      <c r="H7" s="16" t="s">
-        <v>286</v>
-      </c>
+      <c r="H7" s="16"/>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="16" t="s">
@@ -3907,9 +3930,7 @@
       </c>
       <c r="F8" s="16"/>
       <c r="G8" s="16"/>
-      <c r="H8" s="16" t="s">
-        <v>286</v>
-      </c>
+      <c r="H8" s="16"/>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="16" t="s">
@@ -4618,7 +4639,7 @@
       <c r="D42" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="E42" s="36" t="s">
+      <c r="E42" s="23" t="s">
         <v>266</v>
       </c>
       <c r="F42" s="21"/>
@@ -4660,7 +4681,7 @@
       <c r="D44" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="E44" s="36" t="s">
+      <c r="E44" s="23" t="s">
         <v>266</v>
       </c>
       <c r="F44" s="21"/>
@@ -4802,36 +4823,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="26" t="s">
         <v>160</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="27"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="28"/>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="25"/>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="27"/>
+      <c r="A2" s="26"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="28"/>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="28"/>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="30"/>
+      <c r="A3" s="29"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="31"/>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="4" t="s">
@@ -6117,36 +6138,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="26" t="s">
         <v>201</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="27"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="28"/>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="25"/>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="27"/>
+      <c r="A2" s="26"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="28"/>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="28"/>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="30"/>
+      <c r="A3" s="29"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="31"/>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="4" t="s">
@@ -7041,36 +7062,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="31"/>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="33"/>
+      <c r="A1" s="32"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="34"/>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="31"/>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="33"/>
+      <c r="A2" s="32"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="34"/>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="34"/>
-      <c r="B3" s="34"/>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34" t="s">
+      <c r="A3" s="35"/>
+      <c r="B3" s="35"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35" t="s">
         <v>81</v>
       </c>
-      <c r="G3" s="34"/>
-      <c r="H3" s="35"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="36"/>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="4" t="s">

</xml_diff>

<commit_message>
Modified the code to handle the os name
</commit_message>
<xml_diff>
--- a/TestDataAndResults/Run1/SophieAutomation.xlsx
+++ b/TestDataAndResults/Run1/SophieAutomation.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr documentId="13_ncr:1_{8D8477B9-B660-4478-965D-1C32BB43AD9F}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43"/>
+  <xr:revisionPtr documentId="13_ncr:1_{4AF254F7-357C-499B-A90D-CF8D5F70E2D3}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43"/>
   <bookViews>
     <workbookView activeTab="1" firstSheet="1" windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1363" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1466" uniqueCount="288">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -1514,7 +1514,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1657,7 +1657,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32EA4E71-0B53-4881-A15A-C454293CD34C}">
   <dimension ref="A1:I44"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
+    <sheetView topLeftCell="A43" workbookViewId="0">
       <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
@@ -1778,7 +1778,7 @@
       </c>
       <c r="G6" s="9"/>
       <c r="H6" s="3" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -1824,7 +1824,7 @@
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
       <c r="H8" s="3" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -1870,7 +1870,7 @@
       <c r="F10" s="9"/>
       <c r="G10" s="9"/>
       <c r="H10" s="3" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -1916,7 +1916,7 @@
       <c r="F12" s="9"/>
       <c r="G12" s="9"/>
       <c r="H12" s="3" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -1962,7 +1962,7 @@
       <c r="F14" s="9"/>
       <c r="G14" s="9"/>
       <c r="H14" s="3" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -2010,7 +2010,7 @@
       </c>
       <c r="G16" s="9"/>
       <c r="H16" s="3" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -2034,7 +2034,7 @@
       </c>
       <c r="G17" s="9"/>
       <c r="H17" s="3" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -2057,7 +2057,9 @@
         <v>5000</v>
       </c>
       <c r="G18" s="7"/>
-      <c r="H18" s="3"/>
+      <c r="H18" s="3" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="19" t="s">
@@ -2077,7 +2079,9 @@
       </c>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
+      <c r="H19" s="3" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="19" t="s">
@@ -2099,7 +2103,9 @@
         <v>131</v>
       </c>
       <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
+      <c r="H20" s="3" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="19" t="s">
@@ -2121,7 +2127,9 @@
         <v>65</v>
       </c>
       <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
+      <c r="H21" s="3" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="19" t="s">
@@ -2141,7 +2149,9 @@
       </c>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
+      <c r="H22" s="3" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="19" t="s">
@@ -2163,7 +2173,9 @@
         <v>3000</v>
       </c>
       <c r="G23" s="7"/>
-      <c r="H23" s="3"/>
+      <c r="H23" s="3" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="19" t="s">
@@ -2183,7 +2195,9 @@
       </c>
       <c r="F24" s="7"/>
       <c r="G24" s="7"/>
-      <c r="H24" s="3"/>
+      <c r="H24" s="3" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="19" t="s">
@@ -2203,7 +2217,9 @@
       </c>
       <c r="F25" s="7"/>
       <c r="G25" s="7"/>
-      <c r="H25" s="3"/>
+      <c r="H25" s="3" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="19" t="s">
@@ -2223,7 +2239,9 @@
       </c>
       <c r="F26" s="7"/>
       <c r="G26" s="7"/>
-      <c r="H26" s="3"/>
+      <c r="H26" s="3" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="19" t="s">
@@ -2243,7 +2261,9 @@
       </c>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
-      <c r="H27" s="3"/>
+      <c r="H27" s="3" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="19" t="s">
@@ -2265,7 +2285,9 @@
         <v>3000</v>
       </c>
       <c r="G28" s="7"/>
-      <c r="H28" s="3"/>
+      <c r="H28" s="3" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="19" t="s">
@@ -2285,7 +2307,9 @@
       </c>
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
-      <c r="H29" s="3"/>
+      <c r="H29" s="3" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="19" t="s">
@@ -2307,7 +2331,9 @@
         <v>3000</v>
       </c>
       <c r="G30" s="7"/>
-      <c r="H30" s="3"/>
+      <c r="H30" s="3" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="19" t="s">
@@ -2327,7 +2353,9 @@
       </c>
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
-      <c r="H31" s="3"/>
+      <c r="H31" s="3" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="19" t="s">
@@ -2349,7 +2377,9 @@
         <v>3000</v>
       </c>
       <c r="G32" s="7"/>
-      <c r="H32" s="3"/>
+      <c r="H32" s="3" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="33" spans="1:8">
       <c r="A33" s="19" t="s">
@@ -2369,7 +2399,9 @@
       </c>
       <c r="F33" s="3"/>
       <c r="G33" s="3"/>
-      <c r="H33" s="3"/>
+      <c r="H33" s="3" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="34" spans="1:8">
       <c r="A34" s="19" t="s">
@@ -2389,7 +2421,9 @@
       </c>
       <c r="F34" s="3"/>
       <c r="G34" s="3"/>
-      <c r="H34" s="3"/>
+      <c r="H34" s="3" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="35" spans="1:8">
       <c r="A35" s="19" t="s">
@@ -2411,7 +2445,9 @@
         <v>20000</v>
       </c>
       <c r="G35" s="7"/>
-      <c r="H35" s="3"/>
+      <c r="H35" s="3" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="36" spans="1:8">
       <c r="A36" s="19" t="s">
@@ -2431,7 +2467,9 @@
       </c>
       <c r="F36" s="3"/>
       <c r="G36" s="3"/>
-      <c r="H36" s="3"/>
+      <c r="H36" s="3" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="37" spans="1:8">
       <c r="A37" s="19" t="s">
@@ -2451,7 +2489,9 @@
       </c>
       <c r="F37" s="3"/>
       <c r="G37" s="3"/>
-      <c r="H37" s="3"/>
+      <c r="H37" s="3" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="38" spans="1:8">
       <c r="A38" s="19" t="s">
@@ -2473,7 +2513,9 @@
         <v>10000</v>
       </c>
       <c r="G38" s="3"/>
-      <c r="H38" s="3"/>
+      <c r="H38" s="3" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="39" spans="1:8">
       <c r="A39" s="19" t="s">
@@ -2493,7 +2535,9 @@
       </c>
       <c r="F39" s="3"/>
       <c r="G39" s="3"/>
-      <c r="H39" s="3"/>
+      <c r="H39" s="3" t="s">
+        <v>287</v>
+      </c>
     </row>
     <row r="40" spans="1:8">
       <c r="A40" s="19" t="s">
@@ -2515,7 +2559,9 @@
         <v>10000</v>
       </c>
       <c r="G40" s="3"/>
-      <c r="H40" s="3"/>
+      <c r="H40" s="3" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="41" spans="1:8">
       <c r="A41" s="19" t="s">
@@ -2535,7 +2581,9 @@
       </c>
       <c r="F41" s="3"/>
       <c r="G41" s="3"/>
-      <c r="H41" s="3"/>
+      <c r="H41" s="3" t="s">
+        <v>287</v>
+      </c>
     </row>
     <row r="42" spans="1:8">
       <c r="A42" s="19" t="s">
@@ -2555,7 +2603,9 @@
       </c>
       <c r="F42" s="3"/>
       <c r="G42" s="3"/>
-      <c r="H42" s="3"/>
+      <c r="H42" s="3" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="43" spans="1:8">
       <c r="A43" s="19" t="s">
@@ -2577,7 +2627,9 @@
         <v>30000</v>
       </c>
       <c r="G43" s="3"/>
-      <c r="H43" s="3"/>
+      <c r="H43" s="3" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="44" spans="1:8">
       <c r="A44" s="19" t="s">
@@ -2597,7 +2649,9 @@
       </c>
       <c r="F44" s="3"/>
       <c r="G44" s="3"/>
-      <c r="H44" s="3"/>
+      <c r="H44" s="3" t="s">
+        <v>286</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2614,7 +2668,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F162030-4240-4061-B605-62E03F55BA7B}">
   <dimension ref="A1:I55"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E16" sqref="E16:F16"/>
     </sheetView>
   </sheetViews>
@@ -2625,6 +2679,7 @@
     <col min="4" max="4" bestFit="true" customWidth="true" width="22.140625" collapsed="true"/>
     <col min="5" max="5" bestFit="true" customWidth="true" width="30.85546875" collapsed="true"/>
     <col min="6" max="6" bestFit="true" customWidth="true" width="26.5703125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="7.86328125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -2707,7 +2762,9 @@
         <v>31</v>
       </c>
       <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
+      <c r="H5" s="9" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="3" t="s">
@@ -2729,7 +2786,9 @@
         <v>31</v>
       </c>
       <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
+      <c r="H6" s="9" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="3" t="s">
@@ -2751,7 +2810,9 @@
         <v>5000</v>
       </c>
       <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
+      <c r="H7" s="9" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="3" t="s">
@@ -2771,7 +2832,9 @@
       </c>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
+      <c r="H8" s="9" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="3" t="s">
@@ -2793,7 +2856,9 @@
         <v>2000</v>
       </c>
       <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
+      <c r="H9" s="9" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="3" t="s">
@@ -2813,7 +2878,9 @@
       </c>
       <c r="F10" s="9"/>
       <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
+      <c r="H10" s="9" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="3" t="s">
@@ -2835,7 +2902,9 @@
         <v>3000</v>
       </c>
       <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
+      <c r="H11" s="9" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="3" t="s">
@@ -2855,7 +2924,9 @@
       </c>
       <c r="F12" s="9"/>
       <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
+      <c r="H12" s="9" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="3" t="s">
@@ -2877,7 +2948,9 @@
         <v>3000</v>
       </c>
       <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
+      <c r="H13" s="9" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="3" t="s">
@@ -2897,7 +2970,9 @@
       </c>
       <c r="F14" s="9"/>
       <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
+      <c r="H14" s="9" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="3" t="s">
@@ -2919,7 +2994,9 @@
         <v>3000</v>
       </c>
       <c r="G15" s="9"/>
-      <c r="H15" s="9"/>
+      <c r="H15" s="9" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="3" t="s">
@@ -2941,7 +3018,9 @@
         <v>199</v>
       </c>
       <c r="G16" s="9"/>
-      <c r="H16" s="9"/>
+      <c r="H16" s="9" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="3" t="s">
@@ -2963,7 +3042,9 @@
         <v>284</v>
       </c>
       <c r="G17" s="9"/>
-      <c r="H17" s="9"/>
+      <c r="H17" s="9" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="3" t="s">
@@ -2983,7 +3064,9 @@
       </c>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
-      <c r="H18" s="9"/>
+      <c r="H18" s="9" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="3" t="s">
@@ -3005,7 +3088,9 @@
         <v>133</v>
       </c>
       <c r="G19" s="3"/>
-      <c r="H19" s="9"/>
+      <c r="H19" s="9" t="s">
+        <v>287</v>
+      </c>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="3" t="s">
@@ -3027,7 +3112,9 @@
         <v>65</v>
       </c>
       <c r="G20" s="3"/>
-      <c r="H20" s="9"/>
+      <c r="H20" s="9" t="s">
+        <v>287</v>
+      </c>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="3" t="s">
@@ -3047,7 +3134,9 @@
       </c>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
-      <c r="H21" s="9"/>
+      <c r="H21" s="9" t="s">
+        <v>287</v>
+      </c>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="3" t="s">
@@ -3069,7 +3158,9 @@
         <v>3000</v>
       </c>
       <c r="G22" s="7"/>
-      <c r="H22" s="9"/>
+      <c r="H22" s="9" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="3" t="s">
@@ -4820,6 +4911,7 @@
     <col min="5" max="5" customWidth="true" width="33.140625" collapsed="true"/>
     <col min="6" max="6" bestFit="true" customWidth="true" width="21.85546875" collapsed="true"/>
     <col min="7" max="7" customWidth="true" width="21.85546875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="7.86328125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -4900,7 +4992,9 @@
         <v>31</v>
       </c>
       <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
+      <c r="H5" s="3" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="3" t="s">
@@ -4922,7 +5016,9 @@
         <v>31</v>
       </c>
       <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
+      <c r="H6" s="3" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="3" t="s">
@@ -4944,7 +5040,9 @@
         <v>56</v>
       </c>
       <c r="G7" s="6"/>
-      <c r="H7" s="3"/>
+      <c r="H7" s="3" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="3" t="s">
@@ -4964,7 +5062,9 @@
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
+      <c r="H8" s="3" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="3" t="s">
@@ -4986,7 +5086,9 @@
         <v>57</v>
       </c>
       <c r="G9" s="7"/>
-      <c r="H9" s="3"/>
+      <c r="H9" s="3" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="3" t="s">
@@ -5006,7 +5108,9 @@
       </c>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
+      <c r="H10" s="3" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="3" t="s">
@@ -5028,7 +5132,9 @@
         <v>62</v>
       </c>
       <c r="G11" s="7"/>
-      <c r="H11" s="3"/>
+      <c r="H11" s="3" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="3" t="s">
@@ -5050,7 +5156,9 @@
         <v>2</v>
       </c>
       <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
+      <c r="H12" s="3" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="3" t="s">
@@ -5072,7 +5180,9 @@
         <v>62</v>
       </c>
       <c r="G13" s="7"/>
-      <c r="H13" s="3"/>
+      <c r="H13" s="3" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="3" t="s">
@@ -5092,7 +5202,9 @@
       </c>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
-      <c r="H14" s="3"/>
+      <c r="H14" s="3" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="3" t="s">
@@ -5114,7 +5226,9 @@
         <v>199</v>
       </c>
       <c r="G15" s="7"/>
-      <c r="H15" s="3"/>
+      <c r="H15" s="3" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="3" t="s">
@@ -5134,7 +5248,9 @@
       </c>
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
-      <c r="H16" s="3"/>
+      <c r="H16" s="3" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="3" t="s">
@@ -5154,7 +5270,9 @@
       </c>
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
-      <c r="H17" s="3"/>
+      <c r="H17" s="3" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="3" t="s">
@@ -5174,7 +5292,9 @@
       </c>
       <c r="F18" s="7"/>
       <c r="G18" s="7"/>
-      <c r="H18" s="3"/>
+      <c r="H18" s="3" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="3" t="s">
@@ -5194,7 +5314,9 @@
       </c>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
+      <c r="H19" s="3" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="3" t="s">
@@ -5216,7 +5338,9 @@
         <v>62</v>
       </c>
       <c r="G20" s="7"/>
-      <c r="H20" s="3"/>
+      <c r="H20" s="3" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="3" t="s">
@@ -5238,7 +5362,9 @@
         <v>285</v>
       </c>
       <c r="G21" s="7"/>
-      <c r="H21" s="3"/>
+      <c r="H21" s="3" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="3" t="s">
@@ -5260,7 +5386,9 @@
         <v>284</v>
       </c>
       <c r="G22" s="7"/>
-      <c r="H22" s="3"/>
+      <c r="H22" s="3" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="3" t="s">
@@ -5282,7 +5410,9 @@
         <v>5000</v>
       </c>
       <c r="G23" s="7"/>
-      <c r="H23" s="3"/>
+      <c r="H23" s="3" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="3" t="s">
@@ -5302,7 +5432,9 @@
       </c>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
+      <c r="H24" s="3" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="3" t="s">
@@ -5324,7 +5456,9 @@
         <v>161</v>
       </c>
       <c r="G25" s="3"/>
-      <c r="H25" s="3"/>
+      <c r="H25" s="3" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="3" t="s">
@@ -5346,7 +5480,9 @@
         <v>161</v>
       </c>
       <c r="G26" s="3"/>
-      <c r="H26" s="3"/>
+      <c r="H26" s="3" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="3" t="s">
@@ -5366,7 +5502,9 @@
       </c>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
-      <c r="H27" s="3"/>
+      <c r="H27" s="3" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="3" t="s">
@@ -5388,7 +5526,9 @@
         <v>3000</v>
       </c>
       <c r="G28" s="7"/>
-      <c r="H28" s="3"/>
+      <c r="H28" s="3" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="3" t="s">
@@ -5408,7 +5548,9 @@
       </c>
       <c r="F29" s="7"/>
       <c r="G29" s="7"/>
-      <c r="H29" s="3"/>
+      <c r="H29" s="3" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="3" t="s">
@@ -5428,7 +5570,9 @@
       </c>
       <c r="F30" s="7"/>
       <c r="G30" s="7"/>
-      <c r="H30" s="3"/>
+      <c r="H30" s="3" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="3" t="s">
@@ -5448,7 +5592,9 @@
       </c>
       <c r="F31" s="7"/>
       <c r="G31" s="7"/>
-      <c r="H31" s="3"/>
+      <c r="H31" s="3" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="3" t="s">
@@ -5468,7 +5614,9 @@
       </c>
       <c r="F32" s="7"/>
       <c r="G32" s="7"/>
-      <c r="H32" s="3"/>
+      <c r="H32" s="3" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="33" spans="1:8">
       <c r="A33" s="3" t="s">
@@ -5490,7 +5638,9 @@
         <v>166</v>
       </c>
       <c r="G33" s="7"/>
-      <c r="H33" s="3"/>
+      <c r="H33" s="3" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="34" spans="1:8">
       <c r="A34" s="3" t="s">
@@ -5510,7 +5660,9 @@
       </c>
       <c r="F34" s="7"/>
       <c r="G34" s="7"/>
-      <c r="H34" s="3"/>
+      <c r="H34" s="3" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="35" spans="1:8">
       <c r="A35" s="3" t="s">
@@ -5532,7 +5684,9 @@
         <v>166</v>
       </c>
       <c r="G35" s="7"/>
-      <c r="H35" s="3"/>
+      <c r="H35" s="3" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="36" spans="1:8">
       <c r="A36" s="3" t="s">
@@ -5552,7 +5706,9 @@
       </c>
       <c r="F36" s="3"/>
       <c r="G36" s="3"/>
-      <c r="H36" s="3"/>
+      <c r="H36" s="3" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="37" spans="1:8">
       <c r="A37" s="3" t="s">
@@ -5574,7 +5730,9 @@
         <v>3000</v>
       </c>
       <c r="G37" s="7"/>
-      <c r="H37" s="9"/>
+      <c r="H37" s="9" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="38" spans="1:8">
       <c r="A38" s="3" t="s">
@@ -5594,7 +5752,9 @@
       </c>
       <c r="F38" s="9"/>
       <c r="G38" s="9"/>
-      <c r="H38" s="9"/>
+      <c r="H38" s="9" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="39" spans="1:8">
       <c r="A39" s="3" t="s">
@@ -5614,7 +5774,9 @@
       </c>
       <c r="F39" s="9"/>
       <c r="G39" s="9"/>
-      <c r="H39" s="9"/>
+      <c r="H39" s="9" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="40" spans="1:8">
       <c r="A40" s="3" t="s">
@@ -5636,7 +5798,9 @@
         <v>171</v>
       </c>
       <c r="G40" s="9"/>
-      <c r="H40" s="9"/>
+      <c r="H40" s="9" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="41" spans="1:8">
       <c r="A41" s="3" t="s">
@@ -5658,7 +5822,9 @@
         <v>171</v>
       </c>
       <c r="G41" s="9"/>
-      <c r="H41" s="9"/>
+      <c r="H41" s="9" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="42" spans="1:8">
       <c r="A42" s="3" t="s">
@@ -5680,7 +5846,9 @@
         <v>43526</v>
       </c>
       <c r="G42" s="12"/>
-      <c r="H42" s="9"/>
+      <c r="H42" s="9" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="43" spans="1:8">
       <c r="A43" s="3" t="s">
@@ -5702,7 +5870,9 @@
         <v>45743</v>
       </c>
       <c r="G43" s="12"/>
-      <c r="H43" s="9"/>
+      <c r="H43" s="9" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="44" spans="1:8">
       <c r="A44" s="3" t="s">
@@ -5722,7 +5892,9 @@
       </c>
       <c r="F44" s="9"/>
       <c r="G44" s="9"/>
-      <c r="H44" s="9"/>
+      <c r="H44" s="9" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="45" spans="1:8">
       <c r="A45" s="3" t="s">
@@ -5742,7 +5914,9 @@
       </c>
       <c r="F45" s="9"/>
       <c r="G45" s="9"/>
-      <c r="H45" s="9"/>
+      <c r="H45" s="9" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="46" spans="1:8">
       <c r="A46" s="3" t="s">
@@ -5764,7 +5938,9 @@
         <v>152</v>
       </c>
       <c r="G46" s="3"/>
-      <c r="H46" s="9"/>
+      <c r="H46" s="9" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="47" spans="1:8">
       <c r="A47" s="3" t="s">
@@ -5784,7 +5960,9 @@
       </c>
       <c r="F47" s="3"/>
       <c r="G47" s="3"/>
-      <c r="H47" s="9"/>
+      <c r="H47" s="9" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="48" spans="1:8">
       <c r="A48" s="3" t="s">
@@ -5806,7 +5984,9 @@
         <v>176</v>
       </c>
       <c r="G48" s="3"/>
-      <c r="H48" s="9"/>
+      <c r="H48" s="9" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="49" spans="1:8">
       <c r="A49" s="3" t="s">
@@ -5826,7 +6006,9 @@
       </c>
       <c r="F49" s="9"/>
       <c r="G49" s="9"/>
-      <c r="H49" s="9"/>
+      <c r="H49" s="9" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="50" spans="1:8">
       <c r="A50" s="3" t="s">
@@ -5848,7 +6030,9 @@
         <v>5000</v>
       </c>
       <c r="G50" s="9"/>
-      <c r="H50" s="9"/>
+      <c r="H50" s="9" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="51" spans="1:8">
       <c r="A51" s="3" t="s">
@@ -5868,7 +6052,9 @@
       </c>
       <c r="F51" s="9"/>
       <c r="G51" s="9"/>
-      <c r="H51" s="9"/>
+      <c r="H51" s="9" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="52" spans="1:8">
       <c r="A52" s="3" t="s">
@@ -5892,7 +6078,9 @@
       <c r="G52" s="9" t="s">
         <v>166</v>
       </c>
-      <c r="H52" s="9"/>
+      <c r="H52" s="9" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="53" spans="1:8">
       <c r="A53" s="3" t="s">
@@ -5912,7 +6100,9 @@
       </c>
       <c r="F53" s="14"/>
       <c r="G53" s="14"/>
-      <c r="H53" s="9"/>
+      <c r="H53" s="9" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="54" spans="1:8">
       <c r="A54" s="3" t="s">
@@ -5932,7 +6122,9 @@
       </c>
       <c r="F54" s="9"/>
       <c r="G54" s="9"/>
-      <c r="H54" s="9"/>
+      <c r="H54" s="9" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="55" spans="1:8">
       <c r="A55" s="3" t="s">
@@ -5954,7 +6146,9 @@
         <v>20000</v>
       </c>
       <c r="G55" s="3"/>
-      <c r="H55" s="9"/>
+      <c r="H55" s="9" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="56" spans="1:8">
       <c r="A56" s="3" t="s">
@@ -5974,7 +6168,9 @@
       </c>
       <c r="F56" s="3"/>
       <c r="G56" s="3"/>
-      <c r="H56" s="9"/>
+      <c r="H56" s="9" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="57" spans="1:8">
       <c r="A57" s="3" t="s">
@@ -5996,7 +6192,9 @@
         <v>60000</v>
       </c>
       <c r="G57" s="3"/>
-      <c r="H57" s="9"/>
+      <c r="H57" s="9" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="58" spans="1:8">
       <c r="A58" s="3" t="s">
@@ -6016,7 +6214,9 @@
       </c>
       <c r="F58" s="3"/>
       <c r="G58" s="3"/>
-      <c r="H58" s="9"/>
+      <c r="H58" s="9" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="59" spans="1:8">
       <c r="A59" s="3" t="s">
@@ -6038,7 +6238,9 @@
         <v>30000</v>
       </c>
       <c r="G59" s="3"/>
-      <c r="H59" s="9"/>
+      <c r="H59" s="9" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="60" spans="1:8">
       <c r="A60" s="3" t="s">
@@ -6060,7 +6262,9 @@
         <v>187</v>
       </c>
       <c r="G60" s="3"/>
-      <c r="H60" s="9"/>
+      <c r="H60" s="9" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="61" spans="1:8">
       <c r="A61" s="3" t="s">
@@ -6084,7 +6288,9 @@
       <c r="G61" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="H61" s="9"/>
+      <c r="H61" s="9" t="s">
+        <v>287</v>
+      </c>
     </row>
     <row r="62" spans="1:8">
       <c r="A62" s="3" t="s">
@@ -6104,7 +6310,9 @@
       </c>
       <c r="F62" s="3"/>
       <c r="G62" s="3"/>
-      <c r="H62" s="9"/>
+      <c r="H62" s="9" t="s">
+        <v>286</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
changes in action class openURL
</commit_message>
<xml_diff>
--- a/TestDataAndResults/Run1/SophieAutomation.xlsx
+++ b/TestDataAndResults/Run1/SophieAutomation.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1466" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1362" uniqueCount="288">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -1670,7 +1670,7 @@
     <col min="5" max="5" customWidth="true" width="32.5703125" collapsed="true"/>
     <col min="6" max="6" customWidth="true" width="31.42578125" collapsed="true"/>
     <col min="7" max="7" customWidth="true" width="31.42578125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="7.86328125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="7.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -1824,7 +1824,7 @@
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
       <c r="H8" s="3" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -1870,7 +1870,7 @@
       <c r="F10" s="9"/>
       <c r="G10" s="9"/>
       <c r="H10" s="3" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -1916,7 +1916,7 @@
       <c r="F12" s="9"/>
       <c r="G12" s="9"/>
       <c r="H12" s="3" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -1962,7 +1962,7 @@
       <c r="F14" s="9"/>
       <c r="G14" s="9"/>
       <c r="H14" s="3" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -2010,7 +2010,7 @@
       </c>
       <c r="G16" s="9"/>
       <c r="H16" s="3" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -2033,9 +2033,7 @@
         <v>284</v>
       </c>
       <c r="G17" s="9"/>
-      <c r="H17" s="3" t="s">
-        <v>286</v>
-      </c>
+      <c r="H17" s="3"/>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="19" t="s">
@@ -2057,9 +2055,7 @@
         <v>5000</v>
       </c>
       <c r="G18" s="7"/>
-      <c r="H18" s="3" t="s">
-        <v>286</v>
-      </c>
+      <c r="H18" s="3"/>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="19" t="s">
@@ -2079,9 +2075,7 @@
       </c>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
-      <c r="H19" s="3" t="s">
-        <v>286</v>
-      </c>
+      <c r="H19" s="3"/>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="19" t="s">
@@ -2103,9 +2097,7 @@
         <v>131</v>
       </c>
       <c r="G20" s="3"/>
-      <c r="H20" s="3" t="s">
-        <v>286</v>
-      </c>
+      <c r="H20" s="3"/>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="19" t="s">
@@ -2127,9 +2119,7 @@
         <v>65</v>
       </c>
       <c r="G21" s="3"/>
-      <c r="H21" s="3" t="s">
-        <v>286</v>
-      </c>
+      <c r="H21" s="3"/>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="19" t="s">
@@ -2149,9 +2139,7 @@
       </c>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
-      <c r="H22" s="3" t="s">
-        <v>286</v>
-      </c>
+      <c r="H22" s="3"/>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="19" t="s">
@@ -2173,9 +2161,7 @@
         <v>3000</v>
       </c>
       <c r="G23" s="7"/>
-      <c r="H23" s="3" t="s">
-        <v>286</v>
-      </c>
+      <c r="H23" s="3"/>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="19" t="s">
@@ -2195,9 +2181,7 @@
       </c>
       <c r="F24" s="7"/>
       <c r="G24" s="7"/>
-      <c r="H24" s="3" t="s">
-        <v>286</v>
-      </c>
+      <c r="H24" s="3"/>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="19" t="s">
@@ -2217,9 +2201,7 @@
       </c>
       <c r="F25" s="7"/>
       <c r="G25" s="7"/>
-      <c r="H25" s="3" t="s">
-        <v>286</v>
-      </c>
+      <c r="H25" s="3"/>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="19" t="s">
@@ -2239,9 +2221,7 @@
       </c>
       <c r="F26" s="7"/>
       <c r="G26" s="7"/>
-      <c r="H26" s="3" t="s">
-        <v>286</v>
-      </c>
+      <c r="H26" s="3"/>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="19" t="s">
@@ -2261,9 +2241,7 @@
       </c>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
-      <c r="H27" s="3" t="s">
-        <v>286</v>
-      </c>
+      <c r="H27" s="3"/>
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="19" t="s">
@@ -2285,9 +2263,7 @@
         <v>3000</v>
       </c>
       <c r="G28" s="7"/>
-      <c r="H28" s="3" t="s">
-        <v>286</v>
-      </c>
+      <c r="H28" s="3"/>
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="19" t="s">
@@ -2307,9 +2283,7 @@
       </c>
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
-      <c r="H29" s="3" t="s">
-        <v>286</v>
-      </c>
+      <c r="H29" s="3"/>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="19" t="s">
@@ -2331,9 +2305,7 @@
         <v>3000</v>
       </c>
       <c r="G30" s="7"/>
-      <c r="H30" s="3" t="s">
-        <v>286</v>
-      </c>
+      <c r="H30" s="3"/>
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="19" t="s">
@@ -2353,9 +2325,7 @@
       </c>
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
-      <c r="H31" s="3" t="s">
-        <v>286</v>
-      </c>
+      <c r="H31" s="3"/>
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="19" t="s">
@@ -2377,9 +2347,7 @@
         <v>3000</v>
       </c>
       <c r="G32" s="7"/>
-      <c r="H32" s="3" t="s">
-        <v>286</v>
-      </c>
+      <c r="H32" s="3"/>
     </row>
     <row r="33" spans="1:8">
       <c r="A33" s="19" t="s">
@@ -2399,9 +2367,7 @@
       </c>
       <c r="F33" s="3"/>
       <c r="G33" s="3"/>
-      <c r="H33" s="3" t="s">
-        <v>286</v>
-      </c>
+      <c r="H33" s="3"/>
     </row>
     <row r="34" spans="1:8">
       <c r="A34" s="19" t="s">
@@ -2421,9 +2387,7 @@
       </c>
       <c r="F34" s="3"/>
       <c r="G34" s="3"/>
-      <c r="H34" s="3" t="s">
-        <v>286</v>
-      </c>
+      <c r="H34" s="3"/>
     </row>
     <row r="35" spans="1:8">
       <c r="A35" s="19" t="s">
@@ -2445,9 +2409,7 @@
         <v>20000</v>
       </c>
       <c r="G35" s="7"/>
-      <c r="H35" s="3" t="s">
-        <v>286</v>
-      </c>
+      <c r="H35" s="3"/>
     </row>
     <row r="36" spans="1:8">
       <c r="A36" s="19" t="s">
@@ -2467,9 +2429,7 @@
       </c>
       <c r="F36" s="3"/>
       <c r="G36" s="3"/>
-      <c r="H36" s="3" t="s">
-        <v>286</v>
-      </c>
+      <c r="H36" s="3"/>
     </row>
     <row r="37" spans="1:8">
       <c r="A37" s="19" t="s">
@@ -2489,9 +2449,7 @@
       </c>
       <c r="F37" s="3"/>
       <c r="G37" s="3"/>
-      <c r="H37" s="3" t="s">
-        <v>286</v>
-      </c>
+      <c r="H37" s="3"/>
     </row>
     <row r="38" spans="1:8">
       <c r="A38" s="19" t="s">
@@ -2513,9 +2471,7 @@
         <v>10000</v>
       </c>
       <c r="G38" s="3"/>
-      <c r="H38" s="3" t="s">
-        <v>286</v>
-      </c>
+      <c r="H38" s="3"/>
     </row>
     <row r="39" spans="1:8">
       <c r="A39" s="19" t="s">
@@ -2535,9 +2491,7 @@
       </c>
       <c r="F39" s="3"/>
       <c r="G39" s="3"/>
-      <c r="H39" s="3" t="s">
-        <v>287</v>
-      </c>
+      <c r="H39" s="3"/>
     </row>
     <row r="40" spans="1:8">
       <c r="A40" s="19" t="s">
@@ -2559,9 +2513,7 @@
         <v>10000</v>
       </c>
       <c r="G40" s="3"/>
-      <c r="H40" s="3" t="s">
-        <v>286</v>
-      </c>
+      <c r="H40" s="3"/>
     </row>
     <row r="41" spans="1:8">
       <c r="A41" s="19" t="s">
@@ -2581,9 +2533,7 @@
       </c>
       <c r="F41" s="3"/>
       <c r="G41" s="3"/>
-      <c r="H41" s="3" t="s">
-        <v>287</v>
-      </c>
+      <c r="H41" s="3"/>
     </row>
     <row r="42" spans="1:8">
       <c r="A42" s="19" t="s">
@@ -2603,9 +2553,7 @@
       </c>
       <c r="F42" s="3"/>
       <c r="G42" s="3"/>
-      <c r="H42" s="3" t="s">
-        <v>286</v>
-      </c>
+      <c r="H42" s="3"/>
     </row>
     <row r="43" spans="1:8">
       <c r="A43" s="19" t="s">
@@ -2627,9 +2575,7 @@
         <v>30000</v>
       </c>
       <c r="G43" s="3"/>
-      <c r="H43" s="3" t="s">
-        <v>286</v>
-      </c>
+      <c r="H43" s="3"/>
     </row>
     <row r="44" spans="1:8">
       <c r="A44" s="19" t="s">
@@ -2649,9 +2595,7 @@
       </c>
       <c r="F44" s="3"/>
       <c r="G44" s="3"/>
-      <c r="H44" s="3" t="s">
-        <v>286</v>
-      </c>
+      <c r="H44" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2679,7 +2623,6 @@
     <col min="4" max="4" bestFit="true" customWidth="true" width="22.140625" collapsed="true"/>
     <col min="5" max="5" bestFit="true" customWidth="true" width="30.85546875" collapsed="true"/>
     <col min="6" max="6" bestFit="true" customWidth="true" width="26.5703125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="7.86328125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -2762,9 +2705,7 @@
         <v>31</v>
       </c>
       <c r="G5" s="9"/>
-      <c r="H5" s="9" t="s">
-        <v>286</v>
-      </c>
+      <c r="H5" s="9"/>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="3" t="s">
@@ -2786,9 +2727,7 @@
         <v>31</v>
       </c>
       <c r="G6" s="9"/>
-      <c r="H6" s="9" t="s">
-        <v>286</v>
-      </c>
+      <c r="H6" s="9"/>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="3" t="s">
@@ -2810,9 +2749,7 @@
         <v>5000</v>
       </c>
       <c r="G7" s="9"/>
-      <c r="H7" s="9" t="s">
-        <v>286</v>
-      </c>
+      <c r="H7" s="9"/>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="3" t="s">
@@ -2832,9 +2769,7 @@
       </c>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
-      <c r="H8" s="9" t="s">
-        <v>286</v>
-      </c>
+      <c r="H8" s="9"/>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="3" t="s">
@@ -2856,9 +2791,7 @@
         <v>2000</v>
       </c>
       <c r="G9" s="9"/>
-      <c r="H9" s="9" t="s">
-        <v>286</v>
-      </c>
+      <c r="H9" s="9"/>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="3" t="s">
@@ -2878,9 +2811,7 @@
       </c>
       <c r="F10" s="9"/>
       <c r="G10" s="9"/>
-      <c r="H10" s="9" t="s">
-        <v>286</v>
-      </c>
+      <c r="H10" s="9"/>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="3" t="s">
@@ -2902,9 +2833,7 @@
         <v>3000</v>
       </c>
       <c r="G11" s="9"/>
-      <c r="H11" s="9" t="s">
-        <v>286</v>
-      </c>
+      <c r="H11" s="9"/>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="3" t="s">
@@ -2924,9 +2853,7 @@
       </c>
       <c r="F12" s="9"/>
       <c r="G12" s="9"/>
-      <c r="H12" s="9" t="s">
-        <v>286</v>
-      </c>
+      <c r="H12" s="9"/>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="3" t="s">
@@ -2948,9 +2875,7 @@
         <v>3000</v>
       </c>
       <c r="G13" s="9"/>
-      <c r="H13" s="9" t="s">
-        <v>286</v>
-      </c>
+      <c r="H13" s="9"/>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="3" t="s">
@@ -2970,9 +2895,7 @@
       </c>
       <c r="F14" s="9"/>
       <c r="G14" s="9"/>
-      <c r="H14" s="9" t="s">
-        <v>286</v>
-      </c>
+      <c r="H14" s="9"/>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="3" t="s">
@@ -2994,9 +2917,7 @@
         <v>3000</v>
       </c>
       <c r="G15" s="9"/>
-      <c r="H15" s="9" t="s">
-        <v>286</v>
-      </c>
+      <c r="H15" s="9"/>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="3" t="s">
@@ -3018,9 +2939,7 @@
         <v>199</v>
       </c>
       <c r="G16" s="9"/>
-      <c r="H16" s="9" t="s">
-        <v>286</v>
-      </c>
+      <c r="H16" s="9"/>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="3" t="s">
@@ -3042,9 +2961,7 @@
         <v>284</v>
       </c>
       <c r="G17" s="9"/>
-      <c r="H17" s="9" t="s">
-        <v>286</v>
-      </c>
+      <c r="H17" s="9"/>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="3" t="s">
@@ -3064,9 +2981,7 @@
       </c>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
-      <c r="H18" s="9" t="s">
-        <v>286</v>
-      </c>
+      <c r="H18" s="9"/>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="3" t="s">
@@ -3088,9 +3003,7 @@
         <v>133</v>
       </c>
       <c r="G19" s="3"/>
-      <c r="H19" s="9" t="s">
-        <v>287</v>
-      </c>
+      <c r="H19" s="9"/>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="3" t="s">
@@ -3112,9 +3025,7 @@
         <v>65</v>
       </c>
       <c r="G20" s="3"/>
-      <c r="H20" s="9" t="s">
-        <v>287</v>
-      </c>
+      <c r="H20" s="9"/>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="3" t="s">
@@ -3134,9 +3045,7 @@
       </c>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
-      <c r="H21" s="9" t="s">
-        <v>287</v>
-      </c>
+      <c r="H21" s="9"/>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="3" t="s">
@@ -3158,9 +3067,7 @@
         <v>3000</v>
       </c>
       <c r="G22" s="7"/>
-      <c r="H22" s="9" t="s">
-        <v>286</v>
-      </c>
+      <c r="H22" s="9"/>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="3" t="s">
@@ -4911,7 +4818,6 @@
     <col min="5" max="5" customWidth="true" width="33.140625" collapsed="true"/>
     <col min="6" max="6" bestFit="true" customWidth="true" width="21.85546875" collapsed="true"/>
     <col min="7" max="7" customWidth="true" width="21.85546875" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="7.86328125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -4992,9 +4898,7 @@
         <v>31</v>
       </c>
       <c r="G5" s="3"/>
-      <c r="H5" s="3" t="s">
-        <v>286</v>
-      </c>
+      <c r="H5" s="3"/>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="3" t="s">
@@ -5016,9 +4920,7 @@
         <v>31</v>
       </c>
       <c r="G6" s="3"/>
-      <c r="H6" s="3" t="s">
-        <v>286</v>
-      </c>
+      <c r="H6" s="3"/>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="3" t="s">
@@ -5040,9 +4942,7 @@
         <v>56</v>
       </c>
       <c r="G7" s="6"/>
-      <c r="H7" s="3" t="s">
-        <v>286</v>
-      </c>
+      <c r="H7" s="3"/>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="3" t="s">
@@ -5062,9 +4962,7 @@
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
-      <c r="H8" s="3" t="s">
-        <v>286</v>
-      </c>
+      <c r="H8" s="3"/>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="3" t="s">
@@ -5086,9 +4984,7 @@
         <v>57</v>
       </c>
       <c r="G9" s="7"/>
-      <c r="H9" s="3" t="s">
-        <v>286</v>
-      </c>
+      <c r="H9" s="3"/>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="3" t="s">
@@ -5108,9 +5004,7 @@
       </c>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
-      <c r="H10" s="3" t="s">
-        <v>286</v>
-      </c>
+      <c r="H10" s="3"/>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="3" t="s">
@@ -5132,9 +5026,7 @@
         <v>62</v>
       </c>
       <c r="G11" s="7"/>
-      <c r="H11" s="3" t="s">
-        <v>286</v>
-      </c>
+      <c r="H11" s="3"/>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="3" t="s">
@@ -5156,9 +5048,7 @@
         <v>2</v>
       </c>
       <c r="G12" s="3"/>
-      <c r="H12" s="3" t="s">
-        <v>286</v>
-      </c>
+      <c r="H12" s="3"/>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="3" t="s">
@@ -5180,9 +5070,7 @@
         <v>62</v>
       </c>
       <c r="G13" s="7"/>
-      <c r="H13" s="3" t="s">
-        <v>286</v>
-      </c>
+      <c r="H13" s="3"/>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="3" t="s">
@@ -5202,9 +5090,7 @@
       </c>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
-      <c r="H14" s="3" t="s">
-        <v>286</v>
-      </c>
+      <c r="H14" s="3"/>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="3" t="s">
@@ -5226,9 +5112,7 @@
         <v>199</v>
       </c>
       <c r="G15" s="7"/>
-      <c r="H15" s="3" t="s">
-        <v>286</v>
-      </c>
+      <c r="H15" s="3"/>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="3" t="s">
@@ -5248,9 +5132,7 @@
       </c>
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
-      <c r="H16" s="3" t="s">
-        <v>286</v>
-      </c>
+      <c r="H16" s="3"/>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="3" t="s">
@@ -5270,9 +5152,7 @@
       </c>
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
-      <c r="H17" s="3" t="s">
-        <v>286</v>
-      </c>
+      <c r="H17" s="3"/>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="3" t="s">
@@ -5292,9 +5172,7 @@
       </c>
       <c r="F18" s="7"/>
       <c r="G18" s="7"/>
-      <c r="H18" s="3" t="s">
-        <v>286</v>
-      </c>
+      <c r="H18" s="3"/>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="3" t="s">
@@ -5314,9 +5192,7 @@
       </c>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
-      <c r="H19" s="3" t="s">
-        <v>286</v>
-      </c>
+      <c r="H19" s="3"/>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="3" t="s">
@@ -5338,9 +5214,7 @@
         <v>62</v>
       </c>
       <c r="G20" s="7"/>
-      <c r="H20" s="3" t="s">
-        <v>286</v>
-      </c>
+      <c r="H20" s="3"/>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="3" t="s">
@@ -5362,9 +5236,7 @@
         <v>285</v>
       </c>
       <c r="G21" s="7"/>
-      <c r="H21" s="3" t="s">
-        <v>286</v>
-      </c>
+      <c r="H21" s="3"/>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="3" t="s">
@@ -5386,9 +5258,7 @@
         <v>284</v>
       </c>
       <c r="G22" s="7"/>
-      <c r="H22" s="3" t="s">
-        <v>286</v>
-      </c>
+      <c r="H22" s="3"/>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="3" t="s">
@@ -5410,9 +5280,7 @@
         <v>5000</v>
       </c>
       <c r="G23" s="7"/>
-      <c r="H23" s="3" t="s">
-        <v>286</v>
-      </c>
+      <c r="H23" s="3"/>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="3" t="s">
@@ -5432,9 +5300,7 @@
       </c>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
-      <c r="H24" s="3" t="s">
-        <v>286</v>
-      </c>
+      <c r="H24" s="3"/>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="3" t="s">
@@ -5456,9 +5322,7 @@
         <v>161</v>
       </c>
       <c r="G25" s="3"/>
-      <c r="H25" s="3" t="s">
-        <v>286</v>
-      </c>
+      <c r="H25" s="3"/>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="3" t="s">
@@ -5480,9 +5344,7 @@
         <v>161</v>
       </c>
       <c r="G26" s="3"/>
-      <c r="H26" s="3" t="s">
-        <v>286</v>
-      </c>
+      <c r="H26" s="3"/>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="3" t="s">
@@ -5502,9 +5364,7 @@
       </c>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
-      <c r="H27" s="3" t="s">
-        <v>286</v>
-      </c>
+      <c r="H27" s="3"/>
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="3" t="s">
@@ -5526,9 +5386,7 @@
         <v>3000</v>
       </c>
       <c r="G28" s="7"/>
-      <c r="H28" s="3" t="s">
-        <v>286</v>
-      </c>
+      <c r="H28" s="3"/>
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="3" t="s">
@@ -5548,9 +5406,7 @@
       </c>
       <c r="F29" s="7"/>
       <c r="G29" s="7"/>
-      <c r="H29" s="3" t="s">
-        <v>286</v>
-      </c>
+      <c r="H29" s="3"/>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="3" t="s">
@@ -5570,9 +5426,7 @@
       </c>
       <c r="F30" s="7"/>
       <c r="G30" s="7"/>
-      <c r="H30" s="3" t="s">
-        <v>286</v>
-      </c>
+      <c r="H30" s="3"/>
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="3" t="s">
@@ -5592,9 +5446,7 @@
       </c>
       <c r="F31" s="7"/>
       <c r="G31" s="7"/>
-      <c r="H31" s="3" t="s">
-        <v>286</v>
-      </c>
+      <c r="H31" s="3"/>
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="3" t="s">
@@ -5614,9 +5466,7 @@
       </c>
       <c r="F32" s="7"/>
       <c r="G32" s="7"/>
-      <c r="H32" s="3" t="s">
-        <v>286</v>
-      </c>
+      <c r="H32" s="3"/>
     </row>
     <row r="33" spans="1:8">
       <c r="A33" s="3" t="s">
@@ -5638,9 +5488,7 @@
         <v>166</v>
       </c>
       <c r="G33" s="7"/>
-      <c r="H33" s="3" t="s">
-        <v>286</v>
-      </c>
+      <c r="H33" s="3"/>
     </row>
     <row r="34" spans="1:8">
       <c r="A34" s="3" t="s">
@@ -5660,9 +5508,7 @@
       </c>
       <c r="F34" s="7"/>
       <c r="G34" s="7"/>
-      <c r="H34" s="3" t="s">
-        <v>286</v>
-      </c>
+      <c r="H34" s="3"/>
     </row>
     <row r="35" spans="1:8">
       <c r="A35" s="3" t="s">
@@ -5684,9 +5530,7 @@
         <v>166</v>
       </c>
       <c r="G35" s="7"/>
-      <c r="H35" s="3" t="s">
-        <v>286</v>
-      </c>
+      <c r="H35" s="3"/>
     </row>
     <row r="36" spans="1:8">
       <c r="A36" s="3" t="s">
@@ -5706,9 +5550,7 @@
       </c>
       <c r="F36" s="3"/>
       <c r="G36" s="3"/>
-      <c r="H36" s="3" t="s">
-        <v>286</v>
-      </c>
+      <c r="H36" s="3"/>
     </row>
     <row r="37" spans="1:8">
       <c r="A37" s="3" t="s">
@@ -5730,9 +5572,7 @@
         <v>3000</v>
       </c>
       <c r="G37" s="7"/>
-      <c r="H37" s="9" t="s">
-        <v>286</v>
-      </c>
+      <c r="H37" s="9"/>
     </row>
     <row r="38" spans="1:8">
       <c r="A38" s="3" t="s">
@@ -5752,9 +5592,7 @@
       </c>
       <c r="F38" s="9"/>
       <c r="G38" s="9"/>
-      <c r="H38" s="9" t="s">
-        <v>286</v>
-      </c>
+      <c r="H38" s="9"/>
     </row>
     <row r="39" spans="1:8">
       <c r="A39" s="3" t="s">
@@ -5774,9 +5612,7 @@
       </c>
       <c r="F39" s="9"/>
       <c r="G39" s="9"/>
-      <c r="H39" s="9" t="s">
-        <v>286</v>
-      </c>
+      <c r="H39" s="9"/>
     </row>
     <row r="40" spans="1:8">
       <c r="A40" s="3" t="s">
@@ -5798,9 +5634,7 @@
         <v>171</v>
       </c>
       <c r="G40" s="9"/>
-      <c r="H40" s="9" t="s">
-        <v>286</v>
-      </c>
+      <c r="H40" s="9"/>
     </row>
     <row r="41" spans="1:8">
       <c r="A41" s="3" t="s">
@@ -5822,9 +5656,7 @@
         <v>171</v>
       </c>
       <c r="G41" s="9"/>
-      <c r="H41" s="9" t="s">
-        <v>286</v>
-      </c>
+      <c r="H41" s="9"/>
     </row>
     <row r="42" spans="1:8">
       <c r="A42" s="3" t="s">
@@ -5846,9 +5678,7 @@
         <v>43526</v>
       </c>
       <c r="G42" s="12"/>
-      <c r="H42" s="9" t="s">
-        <v>286</v>
-      </c>
+      <c r="H42" s="9"/>
     </row>
     <row r="43" spans="1:8">
       <c r="A43" s="3" t="s">
@@ -5870,9 +5700,7 @@
         <v>45743</v>
       </c>
       <c r="G43" s="12"/>
-      <c r="H43" s="9" t="s">
-        <v>286</v>
-      </c>
+      <c r="H43" s="9"/>
     </row>
     <row r="44" spans="1:8">
       <c r="A44" s="3" t="s">
@@ -5892,9 +5720,7 @@
       </c>
       <c r="F44" s="9"/>
       <c r="G44" s="9"/>
-      <c r="H44" s="9" t="s">
-        <v>286</v>
-      </c>
+      <c r="H44" s="9"/>
     </row>
     <row r="45" spans="1:8">
       <c r="A45" s="3" t="s">
@@ -5914,9 +5740,7 @@
       </c>
       <c r="F45" s="9"/>
       <c r="G45" s="9"/>
-      <c r="H45" s="9" t="s">
-        <v>286</v>
-      </c>
+      <c r="H45" s="9"/>
     </row>
     <row r="46" spans="1:8">
       <c r="A46" s="3" t="s">
@@ -5938,9 +5762,7 @@
         <v>152</v>
       </c>
       <c r="G46" s="3"/>
-      <c r="H46" s="9" t="s">
-        <v>286</v>
-      </c>
+      <c r="H46" s="9"/>
     </row>
     <row r="47" spans="1:8">
       <c r="A47" s="3" t="s">
@@ -5960,9 +5782,7 @@
       </c>
       <c r="F47" s="3"/>
       <c r="G47" s="3"/>
-      <c r="H47" s="9" t="s">
-        <v>286</v>
-      </c>
+      <c r="H47" s="9"/>
     </row>
     <row r="48" spans="1:8">
       <c r="A48" s="3" t="s">
@@ -5984,9 +5804,7 @@
         <v>176</v>
       </c>
       <c r="G48" s="3"/>
-      <c r="H48" s="9" t="s">
-        <v>286</v>
-      </c>
+      <c r="H48" s="9"/>
     </row>
     <row r="49" spans="1:8">
       <c r="A49" s="3" t="s">
@@ -6006,9 +5824,7 @@
       </c>
       <c r="F49" s="9"/>
       <c r="G49" s="9"/>
-      <c r="H49" s="9" t="s">
-        <v>286</v>
-      </c>
+      <c r="H49" s="9"/>
     </row>
     <row r="50" spans="1:8">
       <c r="A50" s="3" t="s">
@@ -6030,9 +5846,7 @@
         <v>5000</v>
       </c>
       <c r="G50" s="9"/>
-      <c r="H50" s="9" t="s">
-        <v>286</v>
-      </c>
+      <c r="H50" s="9"/>
     </row>
     <row r="51" spans="1:8">
       <c r="A51" s="3" t="s">
@@ -6052,9 +5866,7 @@
       </c>
       <c r="F51" s="9"/>
       <c r="G51" s="9"/>
-      <c r="H51" s="9" t="s">
-        <v>286</v>
-      </c>
+      <c r="H51" s="9"/>
     </row>
     <row r="52" spans="1:8">
       <c r="A52" s="3" t="s">
@@ -6078,9 +5890,7 @@
       <c r="G52" s="9" t="s">
         <v>166</v>
       </c>
-      <c r="H52" s="9" t="s">
-        <v>286</v>
-      </c>
+      <c r="H52" s="9"/>
     </row>
     <row r="53" spans="1:8">
       <c r="A53" s="3" t="s">
@@ -6100,9 +5910,7 @@
       </c>
       <c r="F53" s="14"/>
       <c r="G53" s="14"/>
-      <c r="H53" s="9" t="s">
-        <v>286</v>
-      </c>
+      <c r="H53" s="9"/>
     </row>
     <row r="54" spans="1:8">
       <c r="A54" s="3" t="s">
@@ -6122,9 +5930,7 @@
       </c>
       <c r="F54" s="9"/>
       <c r="G54" s="9"/>
-      <c r="H54" s="9" t="s">
-        <v>286</v>
-      </c>
+      <c r="H54" s="9"/>
     </row>
     <row r="55" spans="1:8">
       <c r="A55" s="3" t="s">
@@ -6146,9 +5952,7 @@
         <v>20000</v>
       </c>
       <c r="G55" s="3"/>
-      <c r="H55" s="9" t="s">
-        <v>286</v>
-      </c>
+      <c r="H55" s="9"/>
     </row>
     <row r="56" spans="1:8">
       <c r="A56" s="3" t="s">
@@ -6168,9 +5972,7 @@
       </c>
       <c r="F56" s="3"/>
       <c r="G56" s="3"/>
-      <c r="H56" s="9" t="s">
-        <v>286</v>
-      </c>
+      <c r="H56" s="9"/>
     </row>
     <row r="57" spans="1:8">
       <c r="A57" s="3" t="s">
@@ -6192,9 +5994,7 @@
         <v>60000</v>
       </c>
       <c r="G57" s="3"/>
-      <c r="H57" s="9" t="s">
-        <v>286</v>
-      </c>
+      <c r="H57" s="9"/>
     </row>
     <row r="58" spans="1:8">
       <c r="A58" s="3" t="s">
@@ -6214,9 +6014,7 @@
       </c>
       <c r="F58" s="3"/>
       <c r="G58" s="3"/>
-      <c r="H58" s="9" t="s">
-        <v>286</v>
-      </c>
+      <c r="H58" s="9"/>
     </row>
     <row r="59" spans="1:8">
       <c r="A59" s="3" t="s">
@@ -6238,9 +6036,7 @@
         <v>30000</v>
       </c>
       <c r="G59" s="3"/>
-      <c r="H59" s="9" t="s">
-        <v>286</v>
-      </c>
+      <c r="H59" s="9"/>
     </row>
     <row r="60" spans="1:8">
       <c r="A60" s="3" t="s">
@@ -6262,9 +6058,7 @@
         <v>187</v>
       </c>
       <c r="G60" s="3"/>
-      <c r="H60" s="9" t="s">
-        <v>286</v>
-      </c>
+      <c r="H60" s="9"/>
     </row>
     <row r="61" spans="1:8">
       <c r="A61" s="3" t="s">
@@ -6288,9 +6082,7 @@
       <c r="G61" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="H61" s="9" t="s">
-        <v>287</v>
-      </c>
+      <c r="H61" s="9"/>
     </row>
     <row r="62" spans="1:8">
       <c r="A62" s="3" t="s">
@@ -6310,9 +6102,7 @@
       </c>
       <c r="F62" s="3"/>
       <c r="G62" s="3"/>
-      <c r="H62" s="9" t="s">
-        <v>286</v>
-      </c>
+      <c r="H62" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
only 1 st test to run
</commit_message>
<xml_diff>
--- a/TestDataAndResults/Run1/SophieAutomation.xlsx
+++ b/TestDataAndResults/Run1/SophieAutomation.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1362" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1384" uniqueCount="287">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -895,9 +895,6 @@
   </si>
   <si>
     <t>Pass</t>
-  </si>
-  <si>
-    <t>Fail</t>
   </si>
 </sst>
 </file>
@@ -1824,7 +1821,7 @@
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
       <c r="H8" s="3" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -1870,7 +1867,7 @@
       <c r="F10" s="9"/>
       <c r="G10" s="9"/>
       <c r="H10" s="3" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -1916,7 +1913,7 @@
       <c r="F12" s="9"/>
       <c r="G12" s="9"/>
       <c r="H12" s="3" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -1962,7 +1959,7 @@
       <c r="F14" s="9"/>
       <c r="G14" s="9"/>
       <c r="H14" s="3" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -2010,7 +2007,7 @@
       </c>
       <c r="G16" s="9"/>
       <c r="H16" s="3" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -2033,7 +2030,9 @@
         <v>284</v>
       </c>
       <c r="G17" s="9"/>
-      <c r="H17" s="3"/>
+      <c r="H17" s="3" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="19" t="s">
@@ -2055,7 +2054,9 @@
         <v>5000</v>
       </c>
       <c r="G18" s="7"/>
-      <c r="H18" s="3"/>
+      <c r="H18" s="3" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="19" t="s">
@@ -2075,7 +2076,9 @@
       </c>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
+      <c r="H19" s="3" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="19" t="s">
@@ -2097,7 +2100,9 @@
         <v>131</v>
       </c>
       <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
+      <c r="H20" s="3" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="19" t="s">
@@ -2119,7 +2124,9 @@
         <v>65</v>
       </c>
       <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
+      <c r="H21" s="3" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="19" t="s">
@@ -2139,7 +2146,9 @@
       </c>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
+      <c r="H22" s="3" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="19" t="s">
@@ -2161,7 +2170,9 @@
         <v>3000</v>
       </c>
       <c r="G23" s="7"/>
-      <c r="H23" s="3"/>
+      <c r="H23" s="3" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="19" t="s">
@@ -2181,7 +2192,9 @@
       </c>
       <c r="F24" s="7"/>
       <c r="G24" s="7"/>
-      <c r="H24" s="3"/>
+      <c r="H24" s="3" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="19" t="s">
@@ -2201,7 +2214,9 @@
       </c>
       <c r="F25" s="7"/>
       <c r="G25" s="7"/>
-      <c r="H25" s="3"/>
+      <c r="H25" s="3" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="19" t="s">
@@ -2221,7 +2236,9 @@
       </c>
       <c r="F26" s="7"/>
       <c r="G26" s="7"/>
-      <c r="H26" s="3"/>
+      <c r="H26" s="3" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="19" t="s">
@@ -2241,7 +2258,9 @@
       </c>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
-      <c r="H27" s="3"/>
+      <c r="H27" s="3" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="19" t="s">
@@ -2263,7 +2282,9 @@
         <v>3000</v>
       </c>
       <c r="G28" s="7"/>
-      <c r="H28" s="3"/>
+      <c r="H28" s="3" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="19" t="s">
@@ -2283,7 +2304,9 @@
       </c>
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
-      <c r="H29" s="3"/>
+      <c r="H29" s="3" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="19" t="s">
@@ -2305,7 +2328,9 @@
         <v>3000</v>
       </c>
       <c r="G30" s="7"/>
-      <c r="H30" s="3"/>
+      <c r="H30" s="3" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="19" t="s">
@@ -2325,7 +2350,9 @@
       </c>
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
-      <c r="H31" s="3"/>
+      <c r="H31" s="3" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="19" t="s">
@@ -2347,7 +2374,9 @@
         <v>3000</v>
       </c>
       <c r="G32" s="7"/>
-      <c r="H32" s="3"/>
+      <c r="H32" s="3" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="33" spans="1:8">
       <c r="A33" s="19" t="s">
@@ -2367,7 +2396,9 @@
       </c>
       <c r="F33" s="3"/>
       <c r="G33" s="3"/>
-      <c r="H33" s="3"/>
+      <c r="H33" s="3" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="34" spans="1:8">
       <c r="A34" s="19" t="s">
@@ -2387,7 +2418,9 @@
       </c>
       <c r="F34" s="3"/>
       <c r="G34" s="3"/>
-      <c r="H34" s="3"/>
+      <c r="H34" s="3" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="35" spans="1:8">
       <c r="A35" s="19" t="s">
@@ -2409,7 +2442,9 @@
         <v>20000</v>
       </c>
       <c r="G35" s="7"/>
-      <c r="H35" s="3"/>
+      <c r="H35" s="3" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="36" spans="1:8">
       <c r="A36" s="19" t="s">
@@ -2429,7 +2464,9 @@
       </c>
       <c r="F36" s="3"/>
       <c r="G36" s="3"/>
-      <c r="H36" s="3"/>
+      <c r="H36" s="3" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="37" spans="1:8">
       <c r="A37" s="19" t="s">
@@ -2449,7 +2486,9 @@
       </c>
       <c r="F37" s="3"/>
       <c r="G37" s="3"/>
-      <c r="H37" s="3"/>
+      <c r="H37" s="3" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="38" spans="1:8">
       <c r="A38" s="19" t="s">
@@ -2471,7 +2510,9 @@
         <v>10000</v>
       </c>
       <c r="G38" s="3"/>
-      <c r="H38" s="3"/>
+      <c r="H38" s="3" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="39" spans="1:8">
       <c r="A39" s="19" t="s">

</xml_diff>

<commit_message>
Exception handling added in the driver initialization
</commit_message>
<xml_diff>
--- a/TestDataAndResults/Run1/SophieAutomation.xlsx
+++ b/TestDataAndResults/Run1/SophieAutomation.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr documentId="13_ncr:1_{4AF254F7-357C-499B-A90D-CF8D5F70E2D3}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43"/>
+  <xr:revisionPtr documentId="13_ncr:1_{04C71871-3C07-4582-A741-83D3A270AC71}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43"/>
   <bookViews>
-    <workbookView activeTab="1" firstSheet="1" windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
+    <workbookView activeTab="4" firstSheet="2" windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" r:id="rId1" sheetId="8"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1384" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1390" uniqueCount="288">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -895,6 +895,9 @@
   </si>
   <si>
     <t>Pass</t>
+  </si>
+  <si>
+    <t>Fail</t>
   </si>
 </sst>
 </file>
@@ -1510,8 +1513,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1592,7 +1595,7 @@
         <v>101</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="E6" s="3"/>
     </row>
@@ -1607,7 +1610,7 @@
         <v>184</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="E7" s="3"/>
     </row>
@@ -1654,7 +1657,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32EA4E71-0B53-4881-A15A-C454293CD34C}">
   <dimension ref="A1:I44"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
@@ -2532,7 +2535,9 @@
       </c>
       <c r="F39" s="3"/>
       <c r="G39" s="3"/>
-      <c r="H39" s="3"/>
+      <c r="H39" s="3" t="s">
+        <v>287</v>
+      </c>
     </row>
     <row r="40" spans="1:8">
       <c r="A40" s="19" t="s">
@@ -2554,7 +2559,9 @@
         <v>10000</v>
       </c>
       <c r="G40" s="3"/>
-      <c r="H40" s="3"/>
+      <c r="H40" s="3" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="41" spans="1:8">
       <c r="A41" s="19" t="s">
@@ -2574,7 +2581,9 @@
       </c>
       <c r="F41" s="3"/>
       <c r="G41" s="3"/>
-      <c r="H41" s="3"/>
+      <c r="H41" s="3" t="s">
+        <v>287</v>
+      </c>
     </row>
     <row r="42" spans="1:8">
       <c r="A42" s="19" t="s">
@@ -2594,7 +2603,9 @@
       </c>
       <c r="F42" s="3"/>
       <c r="G42" s="3"/>
-      <c r="H42" s="3"/>
+      <c r="H42" s="3" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="43" spans="1:8">
       <c r="A43" s="19" t="s">
@@ -2616,7 +2627,9 @@
         <v>30000</v>
       </c>
       <c r="G43" s="3"/>
-      <c r="H43" s="3"/>
+      <c r="H43" s="3" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="44" spans="1:8">
       <c r="A44" s="19" t="s">
@@ -2636,7 +2649,9 @@
       </c>
       <c r="F44" s="3"/>
       <c r="G44" s="3"/>
-      <c r="H44" s="3"/>
+      <c r="H44" s="3" t="s">
+        <v>286</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -3810,7 +3825,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D61013C2-7F35-4D0B-B54C-3015EDB52E25}">
   <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="85" zoomScaleNormal="85">
+    <sheetView tabSelected="1" workbookViewId="0" zoomScale="85" zoomScaleNormal="85">
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
@@ -4846,7 +4861,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84C8C304-D672-42E3-8009-BB544F384D0E}">
   <dimension ref="A1:I62"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A55" workbookViewId="0">
       <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added server stand alone
</commit_message>
<xml_diff>
--- a/TestDataAndResults/Run1/SophieAutomation.xlsx
+++ b/TestDataAndResults/Run1/SophieAutomation.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1390" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1353" uniqueCount="288">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -1778,7 +1778,7 @@
       </c>
       <c r="G6" s="9"/>
       <c r="H6" s="3" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -1823,9 +1823,7 @@
       </c>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
-      <c r="H8" s="3" t="s">
-        <v>286</v>
-      </c>
+      <c r="H8" s="3"/>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
@@ -1847,9 +1845,7 @@
         <v>2000</v>
       </c>
       <c r="G9" s="9"/>
-      <c r="H9" s="3" t="s">
-        <v>286</v>
-      </c>
+      <c r="H9" s="3"/>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
@@ -1869,9 +1865,7 @@
       </c>
       <c r="F10" s="9"/>
       <c r="G10" s="9"/>
-      <c r="H10" s="3" t="s">
-        <v>286</v>
-      </c>
+      <c r="H10" s="3"/>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
@@ -1893,9 +1887,7 @@
         <v>3000</v>
       </c>
       <c r="G11" s="9"/>
-      <c r="H11" s="3" t="s">
-        <v>286</v>
-      </c>
+      <c r="H11" s="3"/>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
@@ -1915,9 +1907,7 @@
       </c>
       <c r="F12" s="9"/>
       <c r="G12" s="9"/>
-      <c r="H12" s="3" t="s">
-        <v>286</v>
-      </c>
+      <c r="H12" s="3"/>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
@@ -1939,9 +1929,7 @@
         <v>3000</v>
       </c>
       <c r="G13" s="9"/>
-      <c r="H13" s="3" t="s">
-        <v>286</v>
-      </c>
+      <c r="H13" s="3"/>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" t="s">
@@ -1961,9 +1949,7 @@
       </c>
       <c r="F14" s="9"/>
       <c r="G14" s="9"/>
-      <c r="H14" s="3" t="s">
-        <v>286</v>
-      </c>
+      <c r="H14" s="3"/>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
@@ -1985,9 +1971,7 @@
         <v>3000</v>
       </c>
       <c r="G15" s="9"/>
-      <c r="H15" s="3" t="s">
-        <v>286</v>
-      </c>
+      <c r="H15" s="3"/>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" t="s">
@@ -2009,9 +1993,7 @@
         <v>199</v>
       </c>
       <c r="G16" s="9"/>
-      <c r="H16" s="3" t="s">
-        <v>286</v>
-      </c>
+      <c r="H16" s="3"/>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" t="s">
@@ -2033,9 +2015,7 @@
         <v>284</v>
       </c>
       <c r="G17" s="9"/>
-      <c r="H17" s="3" t="s">
-        <v>286</v>
-      </c>
+      <c r="H17" s="3"/>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="19" t="s">
@@ -2057,9 +2037,7 @@
         <v>5000</v>
       </c>
       <c r="G18" s="7"/>
-      <c r="H18" s="3" t="s">
-        <v>286</v>
-      </c>
+      <c r="H18" s="3"/>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="19" t="s">
@@ -2079,9 +2057,7 @@
       </c>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
-      <c r="H19" s="3" t="s">
-        <v>286</v>
-      </c>
+      <c r="H19" s="3"/>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="19" t="s">
@@ -2103,9 +2079,7 @@
         <v>131</v>
       </c>
       <c r="G20" s="3"/>
-      <c r="H20" s="3" t="s">
-        <v>286</v>
-      </c>
+      <c r="H20" s="3"/>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="19" t="s">
@@ -2127,9 +2101,7 @@
         <v>65</v>
       </c>
       <c r="G21" s="3"/>
-      <c r="H21" s="3" t="s">
-        <v>286</v>
-      </c>
+      <c r="H21" s="3"/>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="19" t="s">
@@ -2149,9 +2121,7 @@
       </c>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
-      <c r="H22" s="3" t="s">
-        <v>286</v>
-      </c>
+      <c r="H22" s="3"/>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="19" t="s">
@@ -2173,9 +2143,7 @@
         <v>3000</v>
       </c>
       <c r="G23" s="7"/>
-      <c r="H23" s="3" t="s">
-        <v>286</v>
-      </c>
+      <c r="H23" s="3"/>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="19" t="s">
@@ -2195,9 +2163,7 @@
       </c>
       <c r="F24" s="7"/>
       <c r="G24" s="7"/>
-      <c r="H24" s="3" t="s">
-        <v>286</v>
-      </c>
+      <c r="H24" s="3"/>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="19" t="s">
@@ -2217,9 +2183,7 @@
       </c>
       <c r="F25" s="7"/>
       <c r="G25" s="7"/>
-      <c r="H25" s="3" t="s">
-        <v>286</v>
-      </c>
+      <c r="H25" s="3"/>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="19" t="s">
@@ -2239,9 +2203,7 @@
       </c>
       <c r="F26" s="7"/>
       <c r="G26" s="7"/>
-      <c r="H26" s="3" t="s">
-        <v>286</v>
-      </c>
+      <c r="H26" s="3"/>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="19" t="s">
@@ -2261,9 +2223,7 @@
       </c>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
-      <c r="H27" s="3" t="s">
-        <v>286</v>
-      </c>
+      <c r="H27" s="3"/>
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="19" t="s">
@@ -2285,9 +2245,7 @@
         <v>3000</v>
       </c>
       <c r="G28" s="7"/>
-      <c r="H28" s="3" t="s">
-        <v>286</v>
-      </c>
+      <c r="H28" s="3"/>
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="19" t="s">
@@ -2307,9 +2265,7 @@
       </c>
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
-      <c r="H29" s="3" t="s">
-        <v>286</v>
-      </c>
+      <c r="H29" s="3"/>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="19" t="s">
@@ -2331,9 +2287,7 @@
         <v>3000</v>
       </c>
       <c r="G30" s="7"/>
-      <c r="H30" s="3" t="s">
-        <v>286</v>
-      </c>
+      <c r="H30" s="3"/>
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="19" t="s">
@@ -2353,9 +2307,7 @@
       </c>
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
-      <c r="H31" s="3" t="s">
-        <v>286</v>
-      </c>
+      <c r="H31" s="3"/>
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="19" t="s">
@@ -2377,9 +2329,7 @@
         <v>3000</v>
       </c>
       <c r="G32" s="7"/>
-      <c r="H32" s="3" t="s">
-        <v>286</v>
-      </c>
+      <c r="H32" s="3"/>
     </row>
     <row r="33" spans="1:8">
       <c r="A33" s="19" t="s">
@@ -2399,9 +2349,7 @@
       </c>
       <c r="F33" s="3"/>
       <c r="G33" s="3"/>
-      <c r="H33" s="3" t="s">
-        <v>286</v>
-      </c>
+      <c r="H33" s="3"/>
     </row>
     <row r="34" spans="1:8">
       <c r="A34" s="19" t="s">
@@ -2421,9 +2369,7 @@
       </c>
       <c r="F34" s="3"/>
       <c r="G34" s="3"/>
-      <c r="H34" s="3" t="s">
-        <v>286</v>
-      </c>
+      <c r="H34" s="3"/>
     </row>
     <row r="35" spans="1:8">
       <c r="A35" s="19" t="s">
@@ -2445,9 +2391,7 @@
         <v>20000</v>
       </c>
       <c r="G35" s="7"/>
-      <c r="H35" s="3" t="s">
-        <v>286</v>
-      </c>
+      <c r="H35" s="3"/>
     </row>
     <row r="36" spans="1:8">
       <c r="A36" s="19" t="s">
@@ -2467,9 +2411,7 @@
       </c>
       <c r="F36" s="3"/>
       <c r="G36" s="3"/>
-      <c r="H36" s="3" t="s">
-        <v>286</v>
-      </c>
+      <c r="H36" s="3"/>
     </row>
     <row r="37" spans="1:8">
       <c r="A37" s="19" t="s">
@@ -2489,9 +2431,7 @@
       </c>
       <c r="F37" s="3"/>
       <c r="G37" s="3"/>
-      <c r="H37" s="3" t="s">
-        <v>286</v>
-      </c>
+      <c r="H37" s="3"/>
     </row>
     <row r="38" spans="1:8">
       <c r="A38" s="19" t="s">
@@ -2513,9 +2453,7 @@
         <v>10000</v>
       </c>
       <c r="G38" s="3"/>
-      <c r="H38" s="3" t="s">
-        <v>286</v>
-      </c>
+      <c r="H38" s="3"/>
     </row>
     <row r="39" spans="1:8">
       <c r="A39" s="19" t="s">
@@ -2535,9 +2473,7 @@
       </c>
       <c r="F39" s="3"/>
       <c r="G39" s="3"/>
-      <c r="H39" s="3" t="s">
-        <v>287</v>
-      </c>
+      <c r="H39" s="3"/>
     </row>
     <row r="40" spans="1:8">
       <c r="A40" s="19" t="s">
@@ -2559,9 +2495,7 @@
         <v>10000</v>
       </c>
       <c r="G40" s="3"/>
-      <c r="H40" s="3" t="s">
-        <v>286</v>
-      </c>
+      <c r="H40" s="3"/>
     </row>
     <row r="41" spans="1:8">
       <c r="A41" s="19" t="s">
@@ -2581,9 +2515,7 @@
       </c>
       <c r="F41" s="3"/>
       <c r="G41" s="3"/>
-      <c r="H41" s="3" t="s">
-        <v>287</v>
-      </c>
+      <c r="H41" s="3"/>
     </row>
     <row r="42" spans="1:8">
       <c r="A42" s="19" t="s">
@@ -2603,9 +2535,7 @@
       </c>
       <c r="F42" s="3"/>
       <c r="G42" s="3"/>
-      <c r="H42" s="3" t="s">
-        <v>286</v>
-      </c>
+      <c r="H42" s="3"/>
     </row>
     <row r="43" spans="1:8">
       <c r="A43" s="19" t="s">
@@ -2627,9 +2557,7 @@
         <v>30000</v>
       </c>
       <c r="G43" s="3"/>
-      <c r="H43" s="3" t="s">
-        <v>286</v>
-      </c>
+      <c r="H43" s="3"/>
     </row>
     <row r="44" spans="1:8">
       <c r="A44" s="19" t="s">
@@ -2649,9 +2577,7 @@
       </c>
       <c r="F44" s="3"/>
       <c r="G44" s="3"/>
-      <c r="H44" s="3" t="s">
-        <v>286</v>
-      </c>
+      <c r="H44" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
changed the permission of the chromedriver and made changes in the Actionclass to add headless
</commit_message>
<xml_diff>
--- a/TestDataAndResults/Run1/SophieAutomation.xlsx
+++ b/TestDataAndResults/Run1/SophieAutomation.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1355" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1363" uniqueCount="288">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -1778,7 +1778,7 @@
       </c>
       <c r="G6" s="9"/>
       <c r="H6" s="3" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -1824,7 +1824,7 @@
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
       <c r="H8" s="3" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -1869,7 +1869,9 @@
       </c>
       <c r="F10" s="9"/>
       <c r="G10" s="9"/>
-      <c r="H10" s="3"/>
+      <c r="H10" s="3" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
@@ -1891,7 +1893,9 @@
         <v>3000</v>
       </c>
       <c r="G11" s="9"/>
-      <c r="H11" s="3"/>
+      <c r="H11" s="3" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
@@ -1911,7 +1915,9 @@
       </c>
       <c r="F12" s="9"/>
       <c r="G12" s="9"/>
-      <c r="H12" s="3"/>
+      <c r="H12" s="3" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
@@ -1933,7 +1939,9 @@
         <v>3000</v>
       </c>
       <c r="G13" s="9"/>
-      <c r="H13" s="3"/>
+      <c r="H13" s="3" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" t="s">
@@ -1953,7 +1961,9 @@
       </c>
       <c r="F14" s="9"/>
       <c r="G14" s="9"/>
-      <c r="H14" s="3"/>
+      <c r="H14" s="3" t="s">
+        <v>287</v>
+      </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
@@ -1975,7 +1985,9 @@
         <v>3000</v>
       </c>
       <c r="G15" s="9"/>
-      <c r="H15" s="3"/>
+      <c r="H15" s="3" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" t="s">
@@ -1997,7 +2009,9 @@
         <v>199</v>
       </c>
       <c r="G16" s="9"/>
-      <c r="H16" s="3"/>
+      <c r="H16" s="3" t="s">
+        <v>287</v>
+      </c>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" t="s">
@@ -2019,7 +2033,9 @@
         <v>284</v>
       </c>
       <c r="G17" s="9"/>
-      <c r="H17" s="3"/>
+      <c r="H17" s="3" t="s">
+        <v>287</v>
+      </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="19" t="s">

</xml_diff>